<commit_message>
Hafta 4 ve notlar
</commit_message>
<xml_diff>
--- a/AdvancedJava/_docs/Notlar.xlsx
+++ b/AdvancedJava/_docs/Notlar.xlsx
@@ -365,7 +365,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +402,18 @@
     <font>
       <sz val="8"/>
       <color indexed="81"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -743,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -829,6 +841,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -838,18 +862,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1352,7 +1376,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y3" sqref="Y3"/>
+      <selection pane="bottomLeft" activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1382,37 +1406,37 @@
       <c r="A1" s="30"/>
       <c r="B1" s="18"/>
       <c r="C1" s="29"/>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="51">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="46">
         <v>2</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="48">
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="45">
         <v>1</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="T1" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="48">
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="45">
         <v>1</v>
       </c>
       <c r="Y1" s="17" t="s">
@@ -1527,13 +1551,15 @@
       <c r="F3" s="7">
         <v>2</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="7">
+        <v>2</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="16">
         <f>SUM(D3:J3)*50/K$1</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L3" s="14"/>
       <c r="M3" s="6"/>
@@ -1559,8 +1585,8 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="44"/>
       <c r="AA3" s="21">
-        <f t="shared" ref="AA3:AA25" si="0">K3*0.2+S3*0.25+X3*0.25+Y3*0.3+Z3*0.15</f>
-        <v>45</v>
+        <f>K3*0.2+S3*0.25+X3*0.25+Y3*0.3+Z3*0.15</f>
+        <v>55</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>37</v>
@@ -1585,13 +1611,15 @@
       <c r="F4" s="7">
         <v>2</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7">
+        <v>2</v>
+      </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="16">
-        <f t="shared" ref="K4:K30" si="1">SUM(D4:J4)*50/K$1</f>
-        <v>150</v>
+        <f>SUM(D4:J4)*50/K$1</f>
+        <v>200</v>
       </c>
       <c r="L4" s="14"/>
       <c r="M4" s="6"/>
@@ -1601,7 +1629,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="16">
-        <f t="shared" ref="S4:S30" si="2">SUM(L4:R4)/S$1</f>
+        <f>SUM(L4:R4)/S$1</f>
         <v>0</v>
       </c>
       <c r="T4" s="14">
@@ -1611,14 +1639,14 @@
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
       <c r="X4" s="16">
-        <f t="shared" ref="X4:X30" si="3">SUM(T4:W4)/X$1</f>
+        <f>SUM(T4:W4)/X$1</f>
         <v>60</v>
       </c>
       <c r="Y4" s="6"/>
       <c r="Z4" s="44"/>
       <c r="AA4" s="21">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>K4*0.2+S4*0.25+X4*0.25+Y4*0.3+Z4*0.15</f>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1640,12 +1668,14 @@
       <c r="F5" s="7">
         <v>2</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(D5:J5)*50/K$1</f>
         <v>150</v>
       </c>
       <c r="L5" s="14"/>
@@ -1656,7 +1686,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="16">
-        <f t="shared" si="2"/>
+        <f>SUM(L5:R5)/S$1</f>
         <v>0</v>
       </c>
       <c r="T5" s="14">
@@ -1666,41 +1696,41 @@
       <c r="V5" s="14"/>
       <c r="W5" s="14"/>
       <c r="X5" s="16">
-        <f t="shared" si="3"/>
+        <f>SUM(T5:W5)/X$1</f>
         <v>60</v>
       </c>
       <c r="Y5" s="6"/>
       <c r="Z5" s="44"/>
       <c r="AA5" s="21">
-        <f t="shared" si="0"/>
+        <f>K5*0.2+S5*0.25+X5*0.25+Y5*0.3+Z5*0.15</f>
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="12">
-        <v>2</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D6" s="12"/>
       <c r="E6" s="7">
         <v>2</v>
       </c>
       <c r="F6" s="7">
         <v>2</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(D6:J6)*50/K$1</f>
         <v>150</v>
       </c>
       <c r="L6" s="14"/>
@@ -1711,49 +1741,51 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T6" s="14"/>
+        <f>SUM(L6:R6)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="14">
+        <v>60</v>
+      </c>
       <c r="U6" s="14"/>
       <c r="V6" s="14"/>
       <c r="W6" s="14"/>
       <c r="X6" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(T6:W6)/X$1</f>
+        <v>60</v>
       </c>
       <c r="Y6" s="6"/>
       <c r="Z6" s="44"/>
       <c r="AA6" s="21">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f>K6*0.2+S6*0.25+X6*0.25+Y6*0.3+Z6*0.15</f>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="12">
-        <v>2</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D7" s="12"/>
       <c r="E7" s="7">
         <v>2</v>
       </c>
       <c r="F7" s="7">
         <v>2</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7">
+        <v>2</v>
+      </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(D7:J7)*50/K$1</f>
         <v>150</v>
       </c>
       <c r="L7" s="14"/>
@@ -1764,44 +1796,52 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T7" s="14"/>
+        <f>SUM(L7:R7)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="14">
+        <v>60</v>
+      </c>
       <c r="U7" s="14"/>
       <c r="V7" s="14"/>
       <c r="W7" s="14"/>
       <c r="X7" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(T7:W7)/X$1</f>
+        <v>60</v>
       </c>
       <c r="Y7" s="6"/>
       <c r="Z7" s="44"/>
       <c r="AA7" s="21">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f>K7*0.2+S7*0.25+X7*0.25+Y7*0.3+Z7*0.15</f>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="7">
         <v>2</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(D8:J8)*50/K$1</f>
+        <v>150</v>
       </c>
       <c r="L8" s="14"/>
       <c r="M8" s="6"/>
@@ -1811,44 +1851,52 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T8" s="14"/>
+        <f>SUM(L8:R8)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="14">
+        <v>60</v>
+      </c>
       <c r="U8" s="14"/>
       <c r="V8" s="14"/>
       <c r="W8" s="14"/>
       <c r="X8" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(T8:W8)/X$1</f>
+        <v>60</v>
       </c>
       <c r="Y8" s="6"/>
       <c r="Z8" s="44"/>
       <c r="AA8" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>K8*0.2+S8*0.25+X8*0.25+Y8*0.3+Z8*0.15</f>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2</v>
+      </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(D9:J9)*50/K$1</f>
+        <v>150</v>
       </c>
       <c r="L9" s="14"/>
       <c r="M9" s="6"/>
@@ -1858,44 +1906,52 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T9" s="14"/>
+        <f>SUM(L9:R9)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="14">
+        <v>60</v>
+      </c>
       <c r="U9" s="14"/>
       <c r="V9" s="14"/>
       <c r="W9" s="14"/>
       <c r="X9" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(T9:W9)/X$1</f>
+        <v>60</v>
       </c>
       <c r="Y9" s="6"/>
       <c r="Z9" s="44"/>
       <c r="AA9" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>K9*0.2+S9*0.25+X9*0.25+Y9*0.3+Z9*0.15</f>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="D10" s="12"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(D10:J10)*50/K$1</f>
+        <v>150</v>
       </c>
       <c r="L10" s="14"/>
       <c r="M10" s="6"/>
@@ -1905,44 +1961,52 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T10" s="14"/>
+        <f>SUM(L10:R10)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="14">
+        <v>60</v>
+      </c>
       <c r="U10" s="14"/>
       <c r="V10" s="14"/>
       <c r="W10" s="14"/>
       <c r="X10" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(T10:W10)/X$1</f>
+        <v>60</v>
       </c>
       <c r="Y10" s="6"/>
       <c r="Z10" s="44"/>
       <c r="AA10" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>K10*0.2+S10*0.25+X10*0.25+Y10*0.3+Z10*0.15</f>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="D11" s="12"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="E11" s="7">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>2</v>
+      </c>
+      <c r="G11" s="7">
+        <v>2</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(D11:J11)*50/K$1</f>
+        <v>150</v>
       </c>
       <c r="L11" s="14"/>
       <c r="M11" s="6"/>
@@ -1952,44 +2016,52 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T11" s="14"/>
+        <f>SUM(L11:R11)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="14">
+        <v>60</v>
+      </c>
       <c r="U11" s="14"/>
       <c r="V11" s="14"/>
       <c r="W11" s="14"/>
       <c r="X11" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(T11:W11)/X$1</f>
+        <v>60</v>
       </c>
       <c r="Y11" s="6"/>
       <c r="Z11" s="44"/>
       <c r="AA11" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>K11*0.2+S11*0.25+X11*0.25+Y11*0.3+Z11*0.1</f>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D12" s="12"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="E12" s="7">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1.7</v>
+      </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(D12:J12)*50/K$1</f>
+        <v>142.5</v>
       </c>
       <c r="L12" s="14"/>
       <c r="M12" s="6"/>
@@ -1999,44 +2071,54 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T12" s="14"/>
+        <f>SUM(L12:R12)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="14">
+        <v>60</v>
+      </c>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
       <c r="W12" s="14"/>
       <c r="X12" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(T12:W12)/X$1</f>
+        <v>60</v>
       </c>
       <c r="Y12" s="6"/>
       <c r="Z12" s="44"/>
       <c r="AA12" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>K12*0.2+S12*0.25+X12*0.25+Y12*0.3+Z12*0.15</f>
+        <v>43.5</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+        <v>55</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7">
+        <v>2</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(D13:J13)*50/K$1</f>
+        <v>200</v>
       </c>
       <c r="L13" s="14"/>
       <c r="M13" s="6"/>
@@ -2046,48 +2128,54 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="14"/>
+        <f>SUM(L13:R13)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="14">
+        <v>0</v>
+      </c>
       <c r="U13" s="14"/>
       <c r="V13" s="14"/>
       <c r="W13" s="14"/>
       <c r="X13" s="16">
-        <f t="shared" si="3"/>
+        <f>SUM(T13:W13)/X$1</f>
         <v>0</v>
       </c>
       <c r="Y13" s="6"/>
       <c r="Z13" s="44"/>
       <c r="AA13" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>K13*0.2+S13*0.25+X13*0.25+Y13*0.3+Z13*0.15</f>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2</v>
+      </c>
       <c r="E14" s="7">
         <v>2</v>
       </c>
       <c r="F14" s="7">
         <v>2</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="7">
+        <v>2</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="16">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f>SUM(D14:J14)*50/K$1</f>
+        <v>200</v>
       </c>
       <c r="L14" s="14"/>
       <c r="M14" s="6"/>
@@ -2097,48 +2185,52 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="16">
-        <f t="shared" si="2"/>
+        <f>SUM(L14:R14)/S$1</f>
         <v>0</v>
       </c>
       <c r="T14" s="14">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="U14" s="14"/>
       <c r="V14" s="14"/>
       <c r="W14" s="14"/>
       <c r="X14" s="16">
-        <f t="shared" si="3"/>
-        <v>60</v>
+        <f>SUM(T14:W14)/X$1</f>
+        <v>0</v>
       </c>
       <c r="Y14" s="6"/>
       <c r="Z14" s="44"/>
       <c r="AA14" s="21">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>K14*0.2+S14*0.25+X14*0.25+Y14*0.3+Z14*0.15</f>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="7">
         <v>2</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="7">
+        <v>2</v>
+      </c>
+      <c r="G15" s="7">
+        <v>2</v>
+      </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="16">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f>SUM(D15:J15)*50/K$1</f>
+        <v>150</v>
       </c>
       <c r="L15" s="14"/>
       <c r="M15" s="6"/>
@@ -2148,33 +2240,35 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T15" s="14"/>
+        <f>SUM(L15:R15)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="14">
+        <v>0</v>
+      </c>
       <c r="U15" s="14"/>
       <c r="V15" s="14"/>
       <c r="W15" s="14"/>
       <c r="X15" s="16">
-        <f t="shared" si="3"/>
+        <f>SUM(T15:W15)/X$1</f>
         <v>0</v>
       </c>
       <c r="Y15" s="6"/>
       <c r="Z15" s="44"/>
       <c r="AA15" s="21">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>K15*0.2+S15*0.25+X15*0.25+Y15*0.3+Z15*0.15</f>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="7">
@@ -2183,13 +2277,15 @@
       <c r="F16" s="7">
         <v>2</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7">
+        <v>2</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="16">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f>SUM(D16:J16)*50/K$1</f>
+        <v>150</v>
       </c>
       <c r="L16" s="14"/>
       <c r="M16" s="6"/>
@@ -2199,49 +2295,49 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="16">
-        <f t="shared" si="2"/>
+        <f>SUM(L16:R16)/S$1</f>
         <v>0</v>
       </c>
       <c r="T16" s="14">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="U16" s="14"/>
       <c r="V16" s="14"/>
       <c r="W16" s="14"/>
       <c r="X16" s="16">
-        <f t="shared" si="3"/>
-        <v>60</v>
+        <f>SUM(T16:W16)/X$1</f>
+        <v>0</v>
       </c>
       <c r="Y16" s="6"/>
       <c r="Z16" s="44"/>
       <c r="AA16" s="21">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>K16*0.2+S16*0.25+X16*0.25+Y16*0.3+Z16*0.15</f>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="7"/>
+      <c r="G17" s="7">
         <v>2</v>
       </c>
-      <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(D17:J17)*50/K$1</f>
         <v>100</v>
       </c>
       <c r="L17" s="14"/>
@@ -2252,619 +2348,587 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="16">
-        <f t="shared" si="2"/>
+        <f>SUM(L17:R17)/S$1</f>
         <v>0</v>
       </c>
       <c r="T17" s="14">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="U17" s="14"/>
       <c r="V17" s="14"/>
       <c r="W17" s="14"/>
       <c r="X17" s="16">
-        <f t="shared" si="3"/>
-        <v>60</v>
+        <f>SUM(T17:W17)/X$1</f>
+        <v>0</v>
       </c>
       <c r="Y17" s="6"/>
       <c r="Z17" s="44"/>
       <c r="AA17" s="21">
-        <f t="shared" si="0"/>
+        <f>K17*0.2+S17*0.25+X17*0.25+Y17*0.3+Z17*0.15</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="57">
+        <f>SUM(D18:J18)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="58"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="59"/>
+      <c r="S18" s="57">
+        <f>SUM(L18:R18)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="58"/>
+      <c r="U18" s="58"/>
+      <c r="V18" s="58"/>
+      <c r="W18" s="58"/>
+      <c r="X18" s="57">
+        <f>SUM(T18:W18)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="59"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61">
+        <f>K18*0.2+S18*0.25+X18*0.25+Y18*0.3+Z18*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57">
+        <f>SUM(D19:J19)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="58"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="57">
+        <f>SUM(L19:R19)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="58"/>
+      <c r="U19" s="58"/>
+      <c r="V19" s="58"/>
+      <c r="W19" s="58"/>
+      <c r="X19" s="57">
+        <f>SUM(T19:W19)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="59"/>
+      <c r="Z19" s="60"/>
+      <c r="AA19" s="61">
+        <f>K19*0.2+S19*0.25+X19*0.25+Y19*0.3+Z19*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="53" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="7">
-        <v>2</v>
-      </c>
-      <c r="F18" s="7">
-        <v>2</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="16">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="L18" s="14"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="44"/>
-      <c r="AA18" s="21">
-        <f t="shared" si="0"/>
+      <c r="C20" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="57">
+        <f>SUM(D20:J20)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="58"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="59"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="59"/>
+      <c r="Q20" s="59"/>
+      <c r="R20" s="59"/>
+      <c r="S20" s="57">
+        <f>SUM(L20:R20)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="58"/>
+      <c r="W20" s="58"/>
+      <c r="X20" s="57">
+        <f>SUM(T20:W20)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="59"/>
+      <c r="Z20" s="60"/>
+      <c r="AA20" s="61">
+        <f>K20*0.2+S20*0.25+X20*0.25+Y20*0.3+Z20*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="57">
+        <f>SUM(D21:J21)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="58"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="59"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="57">
+        <f>SUM(L21:R21)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="57">
+        <f>SUM(T21:W21)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="59"/>
+      <c r="Z21" s="60"/>
+      <c r="AA21" s="61">
+        <f>K21*0.2+S21*0.25+X21*0.25+Y21*0.3+Z21*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57">
+        <f>SUM(D22:J22)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="58"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="57">
+        <f>SUM(L22:R22)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="58"/>
+      <c r="W22" s="58"/>
+      <c r="X22" s="57">
+        <f>SUM(T22:W22)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="59"/>
+      <c r="Z22" s="60"/>
+      <c r="AA22" s="61">
+        <f>K22*0.2+S22*0.25+X22*0.25+Y22*0.3+Z22*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="55"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="57">
+        <f>SUM(D23:J23)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="58"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="59"/>
+      <c r="R23" s="59"/>
+      <c r="S23" s="57">
+        <f>SUM(L23:R23)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="58"/>
+      <c r="U23" s="58"/>
+      <c r="V23" s="58"/>
+      <c r="W23" s="58"/>
+      <c r="X23" s="57">
+        <f>SUM(T23:W23)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="59"/>
+      <c r="Z23" s="60"/>
+      <c r="AA23" s="61">
+        <f>K23*0.2+S23*0.25+X23*0.25+Y23*0.3+Z23*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="B24" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C24" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="44"/>
-      <c r="AA19" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="57">
+        <f>SUM(D24:J24)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="58"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="59"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="57">
+        <f>SUM(L24:R24)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T24" s="58"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="58"/>
+      <c r="W24" s="58"/>
+      <c r="X24" s="57">
+        <f>SUM(T24:W24)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="59"/>
+      <c r="Z24" s="60"/>
+      <c r="AA24" s="61">
+        <f>K24*0.2+S24*0.25+X24*0.25+Y24*0.3+Z24*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B25" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C25" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="44"/>
-      <c r="AA20" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="D25" s="55"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57">
+        <f>SUM(D25:J25)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="58"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="57">
+        <f>SUM(L25:R25)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T25" s="58"/>
+      <c r="U25" s="58"/>
+      <c r="V25" s="58"/>
+      <c r="W25" s="58"/>
+      <c r="X25" s="57">
+        <f>SUM(T25:W25)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="59"/>
+      <c r="Z25" s="60"/>
+      <c r="AA25" s="61">
+        <f>K25*0.2+S25*0.25+X25*0.25+Y25*0.3+Z25*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B26" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C26" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="14"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="44"/>
-      <c r="AA21" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12">
-        <v>2</v>
-      </c>
-      <c r="F22" s="7">
-        <v>2</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="16">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="L22" s="14"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T22" s="14">
-        <v>60</v>
-      </c>
-      <c r="U22" s="14"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="14"/>
-      <c r="X22" s="16">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="44"/>
-      <c r="AA22" s="21">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="7">
-        <v>2</v>
-      </c>
-      <c r="F23" s="7">
-        <v>2</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="16">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="L23" s="14"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
-      <c r="W23" s="14"/>
-      <c r="X23" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="44"/>
-      <c r="AA23" s="21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="7">
-        <v>2</v>
-      </c>
-      <c r="F24" s="7">
-        <v>2</v>
-      </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="16">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="L24" s="14"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T24" s="14">
-        <v>60</v>
-      </c>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="16">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="44"/>
-      <c r="AA24" s="21">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="7">
-        <v>2</v>
-      </c>
-      <c r="F25" s="7">
-        <v>2</v>
-      </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="16">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="L25" s="14"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T25" s="14">
-        <v>60</v>
-      </c>
-      <c r="U25" s="14"/>
-      <c r="V25" s="14"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="16">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="44"/>
-      <c r="AA25" s="21">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="7">
-        <v>2</v>
-      </c>
-      <c r="F26" s="7">
-        <v>2</v>
-      </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="16">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="L26" s="14"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T26" s="14">
-        <v>60</v>
-      </c>
-      <c r="U26" s="14"/>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="16">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="44"/>
-      <c r="AA26" s="21">
-        <f>K26*0.2+S26*0.25+X26*0.25+Y26*0.3+Z26*0.1</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="D26" s="55"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="57">
+        <f>SUM(D26:J26)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="58"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="57">
+        <f>SUM(L26:R26)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
+      <c r="V26" s="58"/>
+      <c r="W26" s="58"/>
+      <c r="X26" s="57">
+        <f>SUM(T26:W26)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="59"/>
+      <c r="Z26" s="60"/>
+      <c r="AA26" s="61">
+        <f>K26*0.2+S26*0.25+X26*0.25+Y26*0.3+Z26*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="14"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="44"/>
-      <c r="AA27" s="21">
+      <c r="D27" s="55"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="57">
+        <f>SUM(D27:J27)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="58"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="57">
+        <f>SUM(L27:R27)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
+      <c r="W27" s="58"/>
+      <c r="X27" s="57">
+        <f>SUM(T27:W27)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="59"/>
+      <c r="Z27" s="60"/>
+      <c r="AA27" s="61">
         <f>K27*0.2+S27*0.25+X27*0.25+Y27*0.3+Z27*0.1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+    <row r="28" spans="1:27" s="62" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="14"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-      <c r="V28" s="14"/>
-      <c r="W28" s="14"/>
-      <c r="X28" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="44"/>
-      <c r="AA28" s="21">
-        <f t="shared" ref="AA28:AA30" si="4">K28*0.2+S28*0.25+X28*0.25+Y28*0.3+Z28*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="D28" s="55"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="57">
+        <f>SUM(D28:J28)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="58"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="59"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="57">
+        <f>SUM(L28:R28)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T28" s="58"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="58"/>
+      <c r="W28" s="58"/>
+      <c r="X28" s="57">
+        <f>SUM(T28:W28)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="59"/>
+      <c r="Z28" s="60"/>
+      <c r="AA28" s="61">
+        <f>K28*0.2+S28*0.25+X28*0.25+Y28*0.3+Z28*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" s="63" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="14"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
-      <c r="V29" s="14"/>
-      <c r="W29" s="14"/>
-      <c r="X29" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="44"/>
-      <c r="AA29" s="21">
-        <f t="shared" si="4"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="57">
+        <f>SUM(D29:J29)*50/K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="58"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="59"/>
+      <c r="R29" s="59"/>
+      <c r="S29" s="57">
+        <f>SUM(L29:R29)/S$1</f>
+        <v>0</v>
+      </c>
+      <c r="T29" s="58"/>
+      <c r="U29" s="58"/>
+      <c r="V29" s="58"/>
+      <c r="W29" s="58"/>
+      <c r="X29" s="57">
+        <f>SUM(T29:W29)/X$1</f>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="59"/>
+      <c r="Z29" s="60"/>
+      <c r="AA29" s="61">
+        <f>K29*0.2+S29*0.25+X29*0.25+Y29*0.3+Z29*0.1</f>
         <v>0</v>
       </c>
     </row>
@@ -2880,7 +2944,7 @@
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="16">
-        <f t="shared" si="1"/>
+        <f>SUM(D30:J30)*50/K$1</f>
         <v>0</v>
       </c>
       <c r="L30" s="14"/>
@@ -2891,7 +2955,7 @@
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
       <c r="S30" s="16">
-        <f t="shared" si="2"/>
+        <f>SUM(L30:R30)/S$1</f>
         <v>0</v>
       </c>
       <c r="T30" s="14"/>
@@ -2899,13 +2963,13 @@
       <c r="V30" s="14"/>
       <c r="W30" s="14"/>
       <c r="X30" s="16">
-        <f t="shared" si="3"/>
+        <f>SUM(T30:W30)/X$1</f>
         <v>0</v>
       </c>
       <c r="Y30" s="6"/>
       <c r="Z30" s="44"/>
       <c r="AA30" s="21">
-        <f t="shared" si="4"/>
+        <f>K30*0.2+S30*0.25+X30*0.25+Y30*0.3+Z30*0.1</f>
         <v>0</v>
       </c>
     </row>
@@ -4106,8 +4170,8 @@
       <c r="X76" s="9"/>
     </row>
   </sheetData>
-  <sortState ref="A3:AB33">
-    <sortCondition descending="1" ref="AA3"/>
+  <sortState ref="A3:AB30">
+    <sortCondition descending="1" ref="AA2"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="D1:J1"/>
@@ -4280,8 +4344,8 @@
   <dimension ref="A1:S81"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:S33"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4309,22 +4373,22 @@
       <c r="B1" s="18"/>
       <c r="C1" s="34"/>
       <c r="D1" s="40"/>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="45" t="s">
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="47"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="51"/>
       <c r="Q1" s="33" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
ileri java hafta 5
</commit_message>
<xml_diff>
--- a/AdvancedJava/_docs/Notlar.xlsx
+++ b/AdvancedJava/_docs/Notlar.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
   <si>
     <t>Adı</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>LAB (%25)</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,6 +437,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -874,11 +883,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="47">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1058,6 +1084,248 @@
         <patternFill>
           <fgColor auto="1"/>
           <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1372,11 +1640,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y76"/>
+  <dimension ref="A1:Z75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1386,23 +1654,26 @@
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.5546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.77734375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="2.77734375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5" style="1" customWidth="1"/>
-    <col min="22" max="22" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7" style="1" customWidth="1"/>
-    <col min="24" max="24" width="5.77734375" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="2.44140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.5546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.77734375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="2.77734375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5" style="1" customWidth="1"/>
+    <col min="23" max="23" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7" style="1" customWidth="1"/>
+    <col min="25" max="25" width="5.77734375" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="18"/>
       <c r="C1" s="29"/>
@@ -1415,38 +1686,39 @@
       <c r="H1" s="60"/>
       <c r="I1" s="60"/>
       <c r="J1" s="60"/>
-      <c r="K1" s="46">
-        <v>2</v>
-      </c>
-      <c r="L1" s="61" t="s">
+      <c r="K1" s="60"/>
+      <c r="L1" s="46">
+        <v>4</v>
+      </c>
+      <c r="M1" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="62"/>
       <c r="N1" s="62"/>
       <c r="O1" s="62"/>
-      <c r="P1" s="45">
+      <c r="P1" s="62"/>
+      <c r="Q1" s="45">
         <v>1</v>
       </c>
-      <c r="Q1" s="61" t="s">
+      <c r="R1" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="62"/>
       <c r="S1" s="62"/>
       <c r="T1" s="62"/>
-      <c r="U1" s="45">
+      <c r="U1" s="62"/>
+      <c r="V1" s="45">
         <v>1</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="W1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="41" t="s">
+      <c r="X1" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>29</v>
       </c>
@@ -1468,7 +1740,7 @@
       <c r="G2" s="27">
         <v>4</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="66">
         <v>5</v>
       </c>
       <c r="I2" s="27">
@@ -1477,50 +1749,53 @@
       <c r="J2" s="27">
         <v>7</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="26">
+      <c r="M2" s="26">
         <v>4</v>
       </c>
-      <c r="M2" s="27">
+      <c r="N2" s="27">
         <v>5</v>
       </c>
-      <c r="N2" s="27">
+      <c r="O2" s="27">
         <v>6</v>
       </c>
-      <c r="O2" s="27">
+      <c r="P2" s="27">
         <v>7</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="Q2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="26">
+      <c r="R2" s="26">
         <v>1</v>
       </c>
-      <c r="R2" s="37">
+      <c r="S2" s="37">
         <v>2</v>
       </c>
-      <c r="S2" s="37">
+      <c r="T2" s="37">
         <v>3</v>
       </c>
-      <c r="T2" s="27">
+      <c r="U2" s="27">
         <v>4</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="V2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="W2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="W2" s="43" t="s">
+      <c r="X2" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="X2" s="19" t="s">
+      <c r="Y2" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>46</v>
       </c>
@@ -1542,44 +1817,49 @@
       <c r="G3" s="7">
         <v>2</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="67">
+        <v>2</v>
+      </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="16">
-        <f t="shared" ref="K3:K30" si="0">SUM(D3:J3)*50/K$1</f>
-        <v>200</v>
-      </c>
-      <c r="L3" s="14">
+      <c r="K3" s="64">
+        <v>0</v>
+      </c>
+      <c r="L3" s="16">
+        <f>SUM(D3:J3)*50/(L$1-K3)</f>
+        <v>125</v>
+      </c>
+      <c r="M3" s="14">
         <v>100</v>
       </c>
-      <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="16">
-        <f>SUM(L3:O3)/P$1</f>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="16">
+        <f>SUM(M3:P3)/Q$1</f>
         <v>100</v>
       </c>
-      <c r="Q3" s="14">
+      <c r="R3" s="14">
         <v>60</v>
       </c>
-      <c r="R3" s="14"/>
       <c r="S3" s="14"/>
       <c r="T3" s="14"/>
-      <c r="U3" s="16">
-        <f t="shared" ref="U3:U30" si="1">SUM(Q3:T3)/U$1</f>
+      <c r="U3" s="14"/>
+      <c r="V3" s="16">
+        <f>SUM(R3:U3)/V$1</f>
         <v>60</v>
       </c>
-      <c r="V3" s="6"/>
-      <c r="W3" s="44"/>
-      <c r="X3" s="21">
-        <f>K3*0.2+P3*0.25+U3*0.25+V3*0.3+W3*0.15</f>
-        <v>80</v>
-      </c>
-      <c r="Y3" s="1" t="s">
+      <c r="W3" s="6"/>
+      <c r="X3" s="44"/>
+      <c r="Y3" s="21">
+        <f>L3*0.2+Q3*0.25+V3*0.25+W3*0.3+X3*0.15</f>
+        <v>65</v>
+      </c>
+      <c r="Z3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>50</v>
       </c>
@@ -1601,52 +1881,57 @@
       <c r="G4" s="7">
         <v>2</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="67">
+        <v>2</v>
+      </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="16">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="L4" s="14">
+      <c r="K4" s="64">
+        <v>0</v>
+      </c>
+      <c r="L4" s="16">
+        <f t="shared" ref="L4:L29" si="0">SUM(D4:J4)*50/(L$1-K4)</f>
+        <v>125</v>
+      </c>
+      <c r="M4" s="14">
         <v>95</v>
       </c>
-      <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
-      <c r="P4" s="16">
-        <f>SUM(L4:O4)/P$1</f>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="16">
+        <f>SUM(M4:P4)/Q$1</f>
         <v>95</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="R4" s="14">
         <v>60</v>
       </c>
-      <c r="R4" s="14"/>
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
-      <c r="U4" s="16">
-        <f t="shared" si="1"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="16">
+        <f>SUM(R4:U4)/V$1</f>
         <v>60</v>
       </c>
-      <c r="V4" s="6"/>
-      <c r="W4" s="44"/>
-      <c r="X4" s="21">
-        <f>K4*0.2+P4*0.25+U4*0.25+V4*0.3+W4*0.15</f>
-        <v>78.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W4" s="6"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="21">
+        <f>L4*0.2+Q4*0.25+V4*0.25+W4*0.3+X4*0.15</f>
+        <v>63.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="D5" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="7">
         <v>2</v>
@@ -1655,43 +1940,48 @@
         <v>2</v>
       </c>
       <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="H5" s="67">
+        <v>2</v>
+      </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="16">
+      <c r="K5" s="64">
+        <v>0</v>
+      </c>
+      <c r="L5" s="16">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L5" s="14">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="M5" s="14">
+        <v>100</v>
+      </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="16">
-        <f>SUM(L5:O5)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="14">
+      <c r="P5" s="6"/>
+      <c r="Q5" s="16">
+        <f>SUM(M5:P5)/Q$1</f>
+        <v>100</v>
+      </c>
+      <c r="R5" s="14">
         <v>60</v>
       </c>
-      <c r="R5" s="14"/>
       <c r="S5" s="14"/>
       <c r="T5" s="14"/>
-      <c r="U5" s="16">
-        <f t="shared" si="1"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="16">
+        <f>SUM(R5:U5)/V$1</f>
         <v>60</v>
       </c>
-      <c r="V5" s="6"/>
-      <c r="W5" s="44"/>
-      <c r="X5" s="21">
-        <f>K5*0.2+P5*0.25+U5*0.25+V5*0.3+W5*0.15</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W5" s="6"/>
+      <c r="X5" s="44"/>
+      <c r="Y5" s="21">
+        <f>L5*0.2+Q5*0.25+V5*0.25+W5*0.3+X5*0.1</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>62</v>
       </c>
@@ -1701,7 +1991,9 @@
       <c r="C6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
       <c r="E6" s="7">
         <v>2</v>
       </c>
@@ -1711,51 +2003,58 @@
       <c r="G6" s="7">
         <v>2</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="67">
+        <v>2</v>
+      </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="16">
+      <c r="K6" s="64">
+        <v>0</v>
+      </c>
+      <c r="L6" s="16">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L6" s="14">
+        <v>100</v>
+      </c>
+      <c r="M6" s="14">
         <v>95</v>
       </c>
-      <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
-      <c r="P6" s="16">
-        <f>SUM(L6:O6)/P$1</f>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="16">
+        <f>SUM(M6:P6)/Q$1</f>
         <v>95</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="R6" s="14">
         <v>60</v>
       </c>
-      <c r="R6" s="14"/>
       <c r="S6" s="14"/>
       <c r="T6" s="14"/>
-      <c r="U6" s="16">
-        <f t="shared" si="1"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="16">
+        <f>SUM(R6:U6)/V$1</f>
         <v>60</v>
       </c>
-      <c r="V6" s="6"/>
-      <c r="W6" s="44"/>
-      <c r="X6" s="21">
-        <f>K6*0.2+P6*0.25+U6*0.25+V6*0.3+W6*0.15</f>
-        <v>68.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W6" s="6"/>
+      <c r="X6" s="44"/>
+      <c r="Y6" s="21">
+        <f>L6*0.2+Q6*0.25+V6*0.25+W6*0.3+X6*0.15</f>
+        <v>58.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
       <c r="E7" s="7">
         <v>2</v>
       </c>
@@ -1765,51 +2064,58 @@
       <c r="G7" s="7">
         <v>2</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="67" t="s">
+        <v>96</v>
+      </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="16">
+      <c r="K7" s="65">
+        <v>1</v>
+      </c>
+      <c r="L7" s="16">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L7" s="14">
-        <v>90</v>
-      </c>
-      <c r="M7" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="M7" s="14">
+        <v>95</v>
+      </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
-      <c r="P7" s="16">
-        <f>SUM(L7:O7)/P$1</f>
-        <v>90</v>
-      </c>
-      <c r="Q7" s="14">
+      <c r="P7" s="6"/>
+      <c r="Q7" s="16">
+        <f>SUM(M7:P7)/Q$1</f>
+        <v>95</v>
+      </c>
+      <c r="R7" s="14">
         <v>60</v>
       </c>
-      <c r="R7" s="14"/>
       <c r="S7" s="14"/>
       <c r="T7" s="14"/>
-      <c r="U7" s="16">
-        <f t="shared" si="1"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="16">
+        <f>SUM(R7:U7)/V$1</f>
         <v>60</v>
       </c>
-      <c r="V7" s="6"/>
-      <c r="W7" s="44"/>
-      <c r="X7" s="21">
-        <f>K7*0.2+P7*0.25+U7*0.25+V7*0.3+W7*0.15</f>
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W7" s="6"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="21">
+        <f>L7*0.2+Q7*0.25+V7*0.25+W7*0.3+X7*0.15</f>
+        <v>58.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="12"/>
+        <v>79</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
       <c r="E8" s="7">
         <v>2</v>
       </c>
@@ -1817,53 +2123,60 @@
         <v>2</v>
       </c>
       <c r="G8" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="H8" s="67">
         <v>2</v>
       </c>
-      <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="16">
+      <c r="K8" s="64">
+        <v>0</v>
+      </c>
+      <c r="L8" s="16">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L8" s="14">
+        <v>97.5</v>
+      </c>
+      <c r="M8" s="14">
         <v>95</v>
       </c>
-      <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="P8" s="16">
-        <f>SUM(L8:O8)/P$1</f>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="16">
+        <f>SUM(M8:P8)/Q$1</f>
         <v>95</v>
       </c>
-      <c r="Q8" s="14">
+      <c r="R8" s="14">
         <v>60</v>
       </c>
-      <c r="R8" s="14"/>
       <c r="S8" s="14"/>
       <c r="T8" s="14"/>
-      <c r="U8" s="16">
-        <f t="shared" si="1"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="16">
+        <f>SUM(R8:U8)/V$1</f>
         <v>60</v>
       </c>
-      <c r="V8" s="6"/>
-      <c r="W8" s="44"/>
-      <c r="X8" s="21">
-        <f>K8*0.2+P8*0.25+U8*0.25+V8*0.3+W8*0.15</f>
-        <v>68.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W8" s="6"/>
+      <c r="X8" s="44"/>
+      <c r="Y8" s="21">
+        <f>L8*0.2+Q8*0.25+V8*0.25+W8*0.3+X8*0.15</f>
+        <v>58.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
       <c r="E9" s="7">
         <v>2</v>
       </c>
@@ -1873,51 +2186,58 @@
       <c r="G9" s="7">
         <v>2</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="67">
+        <v>2</v>
+      </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="16">
+      <c r="K9" s="64">
+        <v>0</v>
+      </c>
+      <c r="L9" s="16">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L9" s="14">
+        <v>100</v>
+      </c>
+      <c r="M9" s="14">
         <v>90</v>
       </c>
-      <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
-      <c r="P9" s="16">
-        <f>SUM(L9:O9)/P$1</f>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="16">
+        <f>SUM(M9:P9)/Q$1</f>
         <v>90</v>
       </c>
-      <c r="Q9" s="14">
+      <c r="R9" s="14">
         <v>60</v>
       </c>
-      <c r="R9" s="14"/>
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
-      <c r="U9" s="16">
-        <f t="shared" si="1"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="16">
+        <f>SUM(R9:U9)/V$1</f>
         <v>60</v>
       </c>
-      <c r="V9" s="6"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="21">
-        <f>K9*0.2+P9*0.25+U9*0.25+V9*0.3+W9*0.15</f>
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W9" s="6"/>
+      <c r="X9" s="44"/>
+      <c r="Y9" s="21">
+        <f>L9*0.2+Q9*0.25+V9*0.25+W9*0.3+X9*0.15</f>
+        <v>57.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="12"/>
+        <v>48</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0</v>
+      </c>
       <c r="E10" s="7">
         <v>2</v>
       </c>
@@ -1927,51 +2247,58 @@
       <c r="G10" s="7">
         <v>2</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="67">
+        <v>1.7</v>
+      </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="16">
+      <c r="K10" s="64">
+        <v>0</v>
+      </c>
+      <c r="L10" s="16">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L10" s="14">
+        <v>96.25</v>
+      </c>
+      <c r="M10" s="14">
         <v>90</v>
       </c>
-      <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
-      <c r="P10" s="16">
-        <f>SUM(L10:O10)/P$1</f>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="16">
+        <f>SUM(M10:P10)/Q$1</f>
         <v>90</v>
       </c>
-      <c r="Q10" s="14">
+      <c r="R10" s="14">
         <v>60</v>
       </c>
-      <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
-      <c r="U10" s="16">
-        <f t="shared" si="1"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="16">
+        <f>SUM(R10:U10)/V$1</f>
         <v>60</v>
       </c>
-      <c r="V10" s="6"/>
-      <c r="W10" s="44"/>
-      <c r="X10" s="21">
-        <f>K10*0.2+P10*0.25+U10*0.25+V10*0.3+W10*0.15</f>
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W10" s="6"/>
+      <c r="X10" s="44"/>
+      <c r="Y10" s="21">
+        <f>L10*0.2+Q10*0.25+V10*0.25+W10*0.3+X10*0.15</f>
+        <v>56.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="12"/>
+        <v>82</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0</v>
+      </c>
       <c r="E11" s="7">
         <v>2</v>
       </c>
@@ -1981,51 +2308,58 @@
       <c r="G11" s="7">
         <v>2</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="67">
+        <v>2</v>
+      </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="16">
+      <c r="K11" s="64">
+        <v>0</v>
+      </c>
+      <c r="L11" s="16">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L11" s="14">
         <v>100</v>
       </c>
-      <c r="M11" s="6"/>
+      <c r="M11" s="14">
+        <v>90</v>
+      </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="16">
-        <f>SUM(L11:O11)/P$1</f>
-        <v>100</v>
-      </c>
-      <c r="Q11" s="14">
+      <c r="P11" s="6"/>
+      <c r="Q11" s="16">
+        <f>SUM(M11:P11)/Q$1</f>
+        <v>90</v>
+      </c>
+      <c r="R11" s="14">
         <v>60</v>
       </c>
-      <c r="R11" s="14"/>
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
-      <c r="U11" s="16">
-        <f t="shared" si="1"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="16">
+        <f>SUM(R11:U11)/V$1</f>
         <v>60</v>
       </c>
-      <c r="V11" s="6"/>
-      <c r="W11" s="44"/>
-      <c r="X11" s="21">
-        <f>K11*0.2+P11*0.25+U11*0.25+V11*0.3+W11*0.1</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W11" s="6"/>
+      <c r="X11" s="44"/>
+      <c r="Y11" s="21">
+        <f>L11*0.2+Q11*0.25+V11*0.25+W11*0.3+X11*0.15</f>
+        <v>57.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="12"/>
+        <v>54</v>
+      </c>
+      <c r="D12" s="12">
+        <v>2</v>
+      </c>
       <c r="E12" s="7">
         <v>2</v>
       </c>
@@ -2033,51 +2367,56 @@
         <v>2</v>
       </c>
       <c r="G12" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="H12" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="H12" s="67">
+        <v>2</v>
+      </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="16">
+      <c r="K12" s="64">
+        <v>0</v>
+      </c>
+      <c r="L12" s="16">
         <f t="shared" si="0"/>
-        <v>145</v>
-      </c>
-      <c r="L12" s="14">
-        <v>95</v>
-      </c>
-      <c r="M12" s="6"/>
+        <v>125</v>
+      </c>
+      <c r="M12" s="14">
+        <v>85</v>
+      </c>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-      <c r="P12" s="16">
-        <f>SUM(L12:O12)/P$1</f>
-        <v>95</v>
-      </c>
-      <c r="Q12" s="14">
-        <v>60</v>
-      </c>
-      <c r="R12" s="14"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="16">
+        <f>SUM(M12:P12)/Q$1</f>
+        <v>85</v>
+      </c>
+      <c r="R12" s="14">
+        <v>0</v>
+      </c>
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
-      <c r="U12" s="16">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="V12" s="6"/>
-      <c r="W12" s="44"/>
-      <c r="X12" s="21">
-        <f>K12*0.2+P12*0.25+U12*0.25+V12*0.3+W12*0.15</f>
-        <v>67.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U12" s="14"/>
+      <c r="V12" s="16">
+        <f>SUM(R12:U12)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W12" s="6"/>
+      <c r="X12" s="44"/>
+      <c r="Y12" s="21">
+        <f>L12*0.2+Q12*0.25+V12*0.25+W12*0.3+X12*0.15</f>
+        <v>46.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D13" s="12">
         <v>2</v>
@@ -2091,52 +2430,57 @@
       <c r="G13" s="7">
         <v>2</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="67">
+        <v>2</v>
+      </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="16">
+      <c r="K13" s="64">
+        <v>0</v>
+      </c>
+      <c r="L13" s="16">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="L13" s="14">
-        <v>85</v>
-      </c>
-      <c r="M13" s="6"/>
+        <v>125</v>
+      </c>
+      <c r="M13" s="14">
+        <v>80</v>
+      </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
-      <c r="P13" s="16">
-        <f>SUM(L13:O13)/P$1</f>
-        <v>85</v>
-      </c>
-      <c r="Q13" s="14">
-        <v>0</v>
-      </c>
-      <c r="R13" s="14"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="16">
+        <f>SUM(M13:P13)/Q$1</f>
+        <v>80</v>
+      </c>
+      <c r="R13" s="14">
+        <v>0</v>
+      </c>
       <c r="S13" s="14"/>
       <c r="T13" s="14"/>
-      <c r="U13" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V13" s="6"/>
-      <c r="W13" s="44"/>
-      <c r="X13" s="21">
-        <f>K13*0.2+P13*0.25+U13*0.25+V13*0.3+W13*0.15</f>
-        <v>61.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U13" s="14"/>
+      <c r="V13" s="16">
+        <f>SUM(R13:U13)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W13" s="6"/>
+      <c r="X13" s="44"/>
+      <c r="Y13" s="21">
+        <f>L13*0.2+Q13*0.25+V13*0.25+W13*0.3+X13*0.15</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="D14" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="7">
         <v>2</v>
@@ -2147,41 +2491,46 @@
       <c r="G14" s="7">
         <v>2</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="67">
+        <v>2</v>
+      </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="16">
+      <c r="K14" s="64">
+        <v>0</v>
+      </c>
+      <c r="L14" s="16">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="L14" s="14">
-        <v>80</v>
-      </c>
-      <c r="M14" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="M14" s="14">
+        <v>90</v>
+      </c>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
-      <c r="P14" s="16">
-        <f>SUM(L14:O14)/P$1</f>
-        <v>80</v>
-      </c>
-      <c r="Q14" s="14">
-        <v>0</v>
-      </c>
-      <c r="R14" s="14"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="16">
+        <f>SUM(M14:P14)/Q$1</f>
+        <v>90</v>
+      </c>
+      <c r="R14" s="14">
+        <v>0</v>
+      </c>
       <c r="S14" s="14"/>
       <c r="T14" s="14"/>
-      <c r="U14" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V14" s="6"/>
-      <c r="W14" s="44"/>
-      <c r="X14" s="21">
-        <f>K14*0.2+P14*0.25+U14*0.25+V14*0.3+W14*0.15</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U14" s="14"/>
+      <c r="V14" s="16">
+        <f>SUM(R14:U14)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="6"/>
+      <c r="X14" s="44"/>
+      <c r="Y14" s="21">
+        <f>L14*0.2+Q14*0.25+V14*0.25+W14*0.3+X14*0.15</f>
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>17</v>
       </c>
@@ -2191,7 +2540,9 @@
       <c r="C15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12">
+        <v>0</v>
+      </c>
       <c r="E15" s="7">
         <v>2</v>
       </c>
@@ -2201,51 +2552,58 @@
       <c r="G15" s="7">
         <v>2</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="67">
+        <v>0</v>
+      </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="16">
+      <c r="K15" s="64">
+        <v>0</v>
+      </c>
+      <c r="L15" s="16">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L15" s="14">
+        <v>75</v>
+      </c>
+      <c r="M15" s="14">
         <v>85</v>
       </c>
-      <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
-      <c r="P15" s="16">
-        <f>SUM(L15:O15)/P$1</f>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="16">
+        <f>SUM(M15:P15)/Q$1</f>
         <v>85</v>
       </c>
-      <c r="Q15" s="14">
-        <v>0</v>
-      </c>
-      <c r="R15" s="14"/>
+      <c r="R15" s="14">
+        <v>0</v>
+      </c>
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
-      <c r="U15" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V15" s="6"/>
-      <c r="W15" s="44"/>
-      <c r="X15" s="21">
-        <f>K15*0.2+P15*0.25+U15*0.25+V15*0.3+W15*0.15</f>
-        <v>51.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="14"/>
+      <c r="V15" s="16">
+        <f>SUM(R15:U15)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W15" s="6"/>
+      <c r="X15" s="44"/>
+      <c r="Y15" s="21">
+        <f>L15*0.2+Q15*0.25+V15*0.25+W15*0.3+X15*0.15</f>
+        <v>36.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="12"/>
+        <v>52</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
       <c r="E16" s="7">
         <v>2</v>
       </c>
@@ -2253,43 +2611,48 @@
         <v>2</v>
       </c>
       <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="67">
         <v>2</v>
       </c>
-      <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="16">
+      <c r="K16" s="64">
+        <v>0</v>
+      </c>
+      <c r="L16" s="16">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L16" s="14">
-        <v>90</v>
-      </c>
-      <c r="M16" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="M16" s="14">
+        <v>0</v>
+      </c>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
-      <c r="P16" s="16">
-        <f>SUM(L16:O16)/P$1</f>
-        <v>90</v>
-      </c>
-      <c r="Q16" s="14">
-        <v>0</v>
-      </c>
-      <c r="R16" s="14"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="16">
+        <f>SUM(M16:P16)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="14">
+        <v>60</v>
+      </c>
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
-      <c r="U16" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V16" s="6"/>
-      <c r="W16" s="44"/>
-      <c r="X16" s="21">
-        <f>K16*0.2+P16*0.25+U16*0.25+V16*0.3+W16*0.15</f>
-        <v>52.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U16" s="14"/>
+      <c r="V16" s="16">
+        <f>SUM(R16:U16)/V$1</f>
+        <v>60</v>
+      </c>
+      <c r="W16" s="6"/>
+      <c r="X16" s="44"/>
+      <c r="Y16" s="21">
+        <f>L16*0.2+Q16*0.25+V16*0.25+W16*0.3+X16*0.15</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>65</v>
       </c>
@@ -2299,181 +2662,243 @@
       <c r="C17" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="12">
+        <v>0</v>
+      </c>
       <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
       <c r="G17" s="7">
         <v>2</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="67">
+        <v>2</v>
+      </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="16">
+      <c r="K17" s="64">
+        <v>0</v>
+      </c>
+      <c r="L17" s="16">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="L17" s="14">
+        <v>75</v>
+      </c>
+      <c r="M17" s="14">
         <v>90</v>
       </c>
-      <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
-      <c r="P17" s="16">
-        <f>SUM(L17:O17)/P$1</f>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="16">
+        <f>SUM(M17:P17)/Q$1</f>
         <v>90</v>
       </c>
-      <c r="Q17" s="14">
-        <v>0</v>
-      </c>
-      <c r="R17" s="14"/>
+      <c r="R17" s="14">
+        <v>0</v>
+      </c>
       <c r="S17" s="14"/>
       <c r="T17" s="14"/>
-      <c r="U17" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V17" s="6"/>
-      <c r="W17" s="44"/>
-      <c r="X17" s="21">
-        <f>K17*0.2+P17*0.25+U17*0.25+V17*0.3+W17*0.15</f>
-        <v>42.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="U17" s="14"/>
+      <c r="V17" s="16">
+        <f>SUM(R17:U17)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W17" s="6"/>
+      <c r="X17" s="44"/>
+      <c r="Y17" s="21">
+        <f>L17*0.2+Q17*0.25+V17*0.25+W17*0.3+X17*0.15</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12">
+        <v>0</v>
+      </c>
+      <c r="H18" s="67">
         <v>2</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="64">
+        <v>0</v>
+      </c>
+      <c r="L18" s="16">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="16">
+        <f>SUM(M18:P18)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="14">
+        <v>0</v>
+      </c>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="16">
+        <f>SUM(R18:U18)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W18" s="6"/>
+      <c r="X18" s="44"/>
+      <c r="Y18" s="21">
+        <f>L18*0.2+Q18*0.25+V18*0.25+W18*0.3+X18*0.15</f>
+        <v>5</v>
+      </c>
+      <c r="Z18" s="1"/>
+    </row>
+    <row r="19" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C19" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="52">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="53"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="52">
-        <f>SUM(L18:O18)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V18" s="54"/>
-      <c r="W18" s="55"/>
-      <c r="X18" s="56">
-        <f>K18*0.2+P18*0.25+U18*0.25+V18*0.3+W18*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
+      <c r="D19" s="50">
+        <v>0</v>
+      </c>
+      <c r="E19" s="50">
+        <v>0</v>
+      </c>
+      <c r="F19" s="50">
+        <v>0</v>
+      </c>
+      <c r="G19" s="50">
+        <v>0</v>
+      </c>
+      <c r="H19" s="68">
+        <v>0</v>
+      </c>
       <c r="I19" s="51"/>
       <c r="J19" s="51"/>
-      <c r="K19" s="52">
+      <c r="K19" s="64">
+        <v>0</v>
+      </c>
+      <c r="L19" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L19" s="53"/>
-      <c r="M19" s="54"/>
+      <c r="M19" s="53">
+        <v>0</v>
+      </c>
       <c r="N19" s="54"/>
       <c r="O19" s="54"/>
-      <c r="P19" s="52">
-        <f>SUM(L19:O19)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="52">
+        <f>SUM(M19:P19)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="53">
+        <v>0</v>
+      </c>
       <c r="S19" s="53"/>
       <c r="T19" s="53"/>
-      <c r="U19" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V19" s="54"/>
-      <c r="W19" s="55"/>
-      <c r="X19" s="56">
-        <f>K19*0.2+P19*0.25+U19*0.25+V19*0.3+W19*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U19" s="53"/>
+      <c r="V19" s="52">
+        <f>SUM(R19:U19)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W19" s="54"/>
+      <c r="X19" s="55"/>
+      <c r="Y19" s="56">
+        <f>L19*0.2+Q19*0.25+V19*0.25+W19*0.3+X19*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
+        <v>6</v>
+      </c>
+      <c r="D20" s="50">
+        <v>0</v>
+      </c>
+      <c r="E20" s="50">
+        <v>0</v>
+      </c>
+      <c r="F20" s="50">
+        <v>0</v>
+      </c>
+      <c r="G20" s="50">
+        <v>0</v>
+      </c>
+      <c r="H20" s="68">
+        <v>0</v>
+      </c>
       <c r="I20" s="51"/>
       <c r="J20" s="51"/>
-      <c r="K20" s="52">
+      <c r="K20" s="64">
+        <v>0</v>
+      </c>
+      <c r="L20" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L20" s="53"/>
-      <c r="M20" s="54"/>
+      <c r="M20" s="53">
+        <v>0</v>
+      </c>
       <c r="N20" s="54"/>
       <c r="O20" s="54"/>
-      <c r="P20" s="52">
-        <f>SUM(L20:O20)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="53"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="52">
+        <f>SUM(M20:P20)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="53">
+        <v>0</v>
+      </c>
       <c r="S20" s="53"/>
       <c r="T20" s="53"/>
-      <c r="U20" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V20" s="54"/>
-      <c r="W20" s="55"/>
-      <c r="X20" s="56">
-        <f>K20*0.2+P20*0.25+U20*0.25+V20*0.3+W20*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U20" s="53"/>
+      <c r="V20" s="52">
+        <f>SUM(R20:U20)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W20" s="54"/>
+      <c r="X20" s="55"/>
+      <c r="Y20" s="56">
+        <f>L20*0.2+Q20*0.25+V20*0.25+W20*0.3+X20*0.15</f>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="57"/>
+    </row>
+    <row r="21" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
         <v>7</v>
       </c>
@@ -2483,41 +2908,58 @@
       <c r="C21" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
+      <c r="D21" s="50">
+        <v>0</v>
+      </c>
+      <c r="E21" s="50">
+        <v>0</v>
+      </c>
+      <c r="F21" s="50">
+        <v>0</v>
+      </c>
+      <c r="G21" s="50">
+        <v>0</v>
+      </c>
+      <c r="H21" s="68">
+        <v>0</v>
+      </c>
       <c r="I21" s="51"/>
       <c r="J21" s="51"/>
-      <c r="K21" s="52">
+      <c r="K21" s="64">
+        <v>0</v>
+      </c>
+      <c r="L21" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L21" s="53"/>
-      <c r="M21" s="54"/>
+      <c r="M21" s="53">
+        <v>0</v>
+      </c>
       <c r="N21" s="54"/>
       <c r="O21" s="54"/>
-      <c r="P21" s="52">
-        <f>SUM(L21:O21)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="53"/>
-      <c r="R21" s="53"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="52">
+        <f>SUM(M21:P21)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="53">
+        <v>0</v>
+      </c>
       <c r="S21" s="53"/>
       <c r="T21" s="53"/>
-      <c r="U21" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V21" s="54"/>
-      <c r="W21" s="55"/>
-      <c r="X21" s="56">
-        <f>K21*0.2+P21*0.25+U21*0.25+V21*0.3+W21*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U21" s="53"/>
+      <c r="V21" s="52">
+        <f>SUM(R21:U21)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W21" s="54"/>
+      <c r="X21" s="55"/>
+      <c r="Y21" s="56">
+        <f>L21*0.2+Q21*0.25+V21*0.25+W21*0.3+X21*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47" t="s">
         <v>11</v>
       </c>
@@ -2527,41 +2969,58 @@
       <c r="C22" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
+      <c r="D22" s="50">
+        <v>0</v>
+      </c>
+      <c r="E22" s="50">
+        <v>0</v>
+      </c>
+      <c r="F22" s="50">
+        <v>0</v>
+      </c>
+      <c r="G22" s="50">
+        <v>0</v>
+      </c>
+      <c r="H22" s="68">
+        <v>0</v>
+      </c>
       <c r="I22" s="51"/>
       <c r="J22" s="51"/>
-      <c r="K22" s="52">
+      <c r="K22" s="64">
+        <v>0</v>
+      </c>
+      <c r="L22" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L22" s="53"/>
-      <c r="M22" s="54"/>
+      <c r="M22" s="53">
+        <v>0</v>
+      </c>
       <c r="N22" s="54"/>
       <c r="O22" s="54"/>
-      <c r="P22" s="52">
-        <f>SUM(L22:O22)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="53"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="52">
+        <f>SUM(M22:P22)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="53">
+        <v>0</v>
+      </c>
       <c r="S22" s="53"/>
       <c r="T22" s="53"/>
-      <c r="U22" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V22" s="54"/>
-      <c r="W22" s="55"/>
-      <c r="X22" s="56">
-        <f>K22*0.2+P22*0.25+U22*0.25+V22*0.3+W22*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U22" s="53"/>
+      <c r="V22" s="52">
+        <f>SUM(R22:U22)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="54"/>
+      <c r="X22" s="55"/>
+      <c r="Y22" s="56">
+        <f>L22*0.2+Q22*0.25+V22*0.25+W22*0.3+X22*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
         <v>14</v>
       </c>
@@ -2571,41 +3030,58 @@
       <c r="C23" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
+      <c r="D23" s="50">
+        <v>0</v>
+      </c>
+      <c r="E23" s="50">
+        <v>0</v>
+      </c>
+      <c r="F23" s="50">
+        <v>0</v>
+      </c>
+      <c r="G23" s="50">
+        <v>0</v>
+      </c>
+      <c r="H23" s="68">
+        <v>0</v>
+      </c>
       <c r="I23" s="51"/>
       <c r="J23" s="51"/>
-      <c r="K23" s="52">
+      <c r="K23" s="64">
+        <v>0</v>
+      </c>
+      <c r="L23" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L23" s="53"/>
-      <c r="M23" s="54"/>
+      <c r="M23" s="53">
+        <v>0</v>
+      </c>
       <c r="N23" s="54"/>
       <c r="O23" s="54"/>
-      <c r="P23" s="52">
-        <f>SUM(L23:O23)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="53"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="52">
+        <f>SUM(M23:P23)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="53">
+        <v>0</v>
+      </c>
       <c r="S23" s="53"/>
       <c r="T23" s="53"/>
-      <c r="U23" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V23" s="54"/>
-      <c r="W23" s="55"/>
-      <c r="X23" s="56">
-        <f>K23*0.2+P23*0.25+U23*0.25+V23*0.3+W23*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U23" s="53"/>
+      <c r="V23" s="52">
+        <f>SUM(R23:U23)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W23" s="54"/>
+      <c r="X23" s="55"/>
+      <c r="Y23" s="56">
+        <f>L23*0.2+Q23*0.25+V23*0.25+W23*0.3+X23*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47" t="s">
         <v>20</v>
       </c>
@@ -2615,41 +3091,58 @@
       <c r="C24" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
+      <c r="D24" s="50">
+        <v>0</v>
+      </c>
+      <c r="E24" s="50">
+        <v>0</v>
+      </c>
+      <c r="F24" s="50">
+        <v>0</v>
+      </c>
+      <c r="G24" s="50">
+        <v>0</v>
+      </c>
+      <c r="H24" s="68">
+        <v>0</v>
+      </c>
       <c r="I24" s="51"/>
       <c r="J24" s="51"/>
-      <c r="K24" s="52">
+      <c r="K24" s="64">
+        <v>0</v>
+      </c>
+      <c r="L24" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L24" s="53"/>
-      <c r="M24" s="54"/>
+      <c r="M24" s="53">
+        <v>0</v>
+      </c>
       <c r="N24" s="54"/>
       <c r="O24" s="54"/>
-      <c r="P24" s="52">
-        <f>SUM(L24:O24)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="53"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="52">
+        <f>SUM(M24:P24)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="53">
+        <v>0</v>
+      </c>
       <c r="S24" s="53"/>
       <c r="T24" s="53"/>
-      <c r="U24" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V24" s="54"/>
-      <c r="W24" s="55"/>
-      <c r="X24" s="56">
-        <f>K24*0.2+P24*0.25+U24*0.25+V24*0.3+W24*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U24" s="53"/>
+      <c r="V24" s="52">
+        <f>SUM(R24:U24)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W24" s="54"/>
+      <c r="X24" s="55"/>
+      <c r="Y24" s="56">
+        <f>L24*0.2+Q24*0.25+V24*0.25+W24*0.3+X24*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
         <v>23</v>
       </c>
@@ -2659,41 +3152,58 @@
       <c r="C25" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
+      <c r="D25" s="50">
+        <v>0</v>
+      </c>
+      <c r="E25" s="50">
+        <v>0</v>
+      </c>
+      <c r="F25" s="50">
+        <v>0</v>
+      </c>
+      <c r="G25" s="50">
+        <v>0</v>
+      </c>
+      <c r="H25" s="68">
+        <v>0</v>
+      </c>
       <c r="I25" s="51"/>
       <c r="J25" s="51"/>
-      <c r="K25" s="52">
+      <c r="K25" s="64">
+        <v>0</v>
+      </c>
+      <c r="L25" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L25" s="53"/>
-      <c r="M25" s="54"/>
+      <c r="M25" s="53">
+        <v>0</v>
+      </c>
       <c r="N25" s="54"/>
       <c r="O25" s="54"/>
-      <c r="P25" s="52">
-        <f>SUM(L25:O25)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="53"/>
-      <c r="R25" s="53"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="52">
+        <f>SUM(M25:P25)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="53">
+        <v>0</v>
+      </c>
       <c r="S25" s="53"/>
       <c r="T25" s="53"/>
-      <c r="U25" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V25" s="54"/>
-      <c r="W25" s="55"/>
-      <c r="X25" s="56">
-        <f>K25*0.2+P25*0.25+U25*0.25+V25*0.3+W25*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U25" s="53"/>
+      <c r="V25" s="52">
+        <f>SUM(R25:U25)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W25" s="54"/>
+      <c r="X25" s="55"/>
+      <c r="Y25" s="56">
+        <f>L25*0.2+Q25*0.25+V25*0.25+W25*0.3+X25*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="47" t="s">
         <v>26</v>
       </c>
@@ -2703,41 +3213,58 @@
       <c r="C26" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
+      <c r="D26" s="50">
+        <v>0</v>
+      </c>
+      <c r="E26" s="50">
+        <v>0</v>
+      </c>
+      <c r="F26" s="50">
+        <v>0</v>
+      </c>
+      <c r="G26" s="50">
+        <v>0</v>
+      </c>
+      <c r="H26" s="68">
+        <v>0</v>
+      </c>
       <c r="I26" s="51"/>
       <c r="J26" s="51"/>
-      <c r="K26" s="52">
+      <c r="K26" s="64">
+        <v>0</v>
+      </c>
+      <c r="L26" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L26" s="53"/>
-      <c r="M26" s="54"/>
+      <c r="M26" s="53">
+        <v>0</v>
+      </c>
       <c r="N26" s="54"/>
       <c r="O26" s="54"/>
-      <c r="P26" s="52">
-        <f>SUM(L26:O26)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="53"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="52">
+        <f>SUM(M26:P26)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="53">
+        <v>0</v>
+      </c>
       <c r="S26" s="53"/>
       <c r="T26" s="53"/>
-      <c r="U26" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V26" s="54"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="56">
-        <f>K26*0.2+P26*0.25+U26*0.25+V26*0.3+W26*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U26" s="53"/>
+      <c r="V26" s="52">
+        <f>SUM(R26:U26)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W26" s="54"/>
+      <c r="X26" s="55"/>
+      <c r="Y26" s="56">
+        <f>L26*0.2+Q26*0.25+V26*0.25+W26*0.3+X26*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47" t="s">
         <v>86</v>
       </c>
@@ -2747,41 +3274,58 @@
       <c r="C27" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
+      <c r="D27" s="50">
+        <v>0</v>
+      </c>
+      <c r="E27" s="50">
+        <v>0</v>
+      </c>
+      <c r="F27" s="50">
+        <v>0</v>
+      </c>
+      <c r="G27" s="50">
+        <v>0</v>
+      </c>
+      <c r="H27" s="68">
+        <v>0</v>
+      </c>
       <c r="I27" s="51"/>
       <c r="J27" s="51"/>
-      <c r="K27" s="52">
+      <c r="K27" s="64">
+        <v>0</v>
+      </c>
+      <c r="L27" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L27" s="53"/>
-      <c r="M27" s="54"/>
+      <c r="M27" s="53">
+        <v>0</v>
+      </c>
       <c r="N27" s="54"/>
       <c r="O27" s="54"/>
-      <c r="P27" s="52">
-        <f>SUM(L27:O27)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="52">
+        <f>SUM(M27:P27)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="53">
+        <v>0</v>
+      </c>
       <c r="S27" s="53"/>
       <c r="T27" s="53"/>
-      <c r="U27" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V27" s="54"/>
-      <c r="W27" s="55"/>
-      <c r="X27" s="56">
-        <f>K27*0.2+P27*0.25+U27*0.25+V27*0.3+W27*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U27" s="53"/>
+      <c r="V27" s="52">
+        <f>SUM(R27:U27)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W27" s="54"/>
+      <c r="X27" s="55"/>
+      <c r="Y27" s="56">
+        <f>L27*0.2+Q27*0.25+V27*0.25+W27*0.3+X27*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47" t="s">
         <v>89</v>
       </c>
@@ -2791,41 +3335,58 @@
       <c r="C28" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="50"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
+      <c r="D28" s="50">
+        <v>0</v>
+      </c>
+      <c r="E28" s="50">
+        <v>0</v>
+      </c>
+      <c r="F28" s="50">
+        <v>0</v>
+      </c>
+      <c r="G28" s="50">
+        <v>0</v>
+      </c>
+      <c r="H28" s="68">
+        <v>0</v>
+      </c>
       <c r="I28" s="51"/>
       <c r="J28" s="51"/>
-      <c r="K28" s="52">
+      <c r="K28" s="64">
+        <v>0</v>
+      </c>
+      <c r="L28" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L28" s="53"/>
-      <c r="M28" s="54"/>
+      <c r="M28" s="53">
+        <v>0</v>
+      </c>
       <c r="N28" s="54"/>
       <c r="O28" s="54"/>
-      <c r="P28" s="52">
-        <f>SUM(L28:O28)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="53"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="52">
+        <f>SUM(M28:P28)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="53">
+        <v>0</v>
+      </c>
       <c r="S28" s="53"/>
       <c r="T28" s="53"/>
-      <c r="U28" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V28" s="54"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="56">
-        <f>K28*0.2+P28*0.25+U28*0.25+V28*0.3+W28*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U28" s="53"/>
+      <c r="V28" s="52">
+        <f>SUM(R28:U28)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W28" s="54"/>
+      <c r="X28" s="55"/>
+      <c r="Y28" s="56">
+        <f>L28*0.2+Q28*0.25+V28*0.25+W28*0.3+X28*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47" t="s">
         <v>92</v>
       </c>
@@ -2835,79 +3396,82 @@
       <c r="C29" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
+      <c r="D29" s="50">
+        <v>0</v>
+      </c>
+      <c r="E29" s="50">
+        <v>0</v>
+      </c>
+      <c r="F29" s="50">
+        <v>0</v>
+      </c>
+      <c r="G29" s="50">
+        <v>0</v>
+      </c>
+      <c r="H29" s="68">
+        <v>0</v>
+      </c>
       <c r="I29" s="51"/>
       <c r="J29" s="51"/>
-      <c r="K29" s="52">
+      <c r="K29" s="64">
+        <v>0</v>
+      </c>
+      <c r="L29" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L29" s="53"/>
-      <c r="M29" s="54"/>
+      <c r="M29" s="53">
+        <v>0</v>
+      </c>
       <c r="N29" s="54"/>
       <c r="O29" s="54"/>
-      <c r="P29" s="52">
-        <f>SUM(L29:O29)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="53"/>
-      <c r="R29" s="53"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="52">
+        <f>SUM(M29:P29)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R29" s="53">
+        <v>0</v>
+      </c>
       <c r="S29" s="53"/>
       <c r="T29" s="53"/>
-      <c r="U29" s="52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V29" s="54"/>
-      <c r="W29" s="55"/>
-      <c r="X29" s="56">
-        <f>K29*0.2+P29*0.25+U29*0.25+V29*0.3+W29*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="14"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="16">
-        <f>SUM(L30:O30)/P$1</f>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V30" s="6"/>
-      <c r="W30" s="44"/>
-      <c r="X30" s="21">
-        <f>K30*0.2+P30*0.25+U30*0.25+V30*0.3+W30*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U29" s="53"/>
+      <c r="V29" s="52">
+        <f>SUM(R29:U29)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W29" s="54"/>
+      <c r="X29" s="55"/>
+      <c r="Y29" s="56">
+        <f>L29*0.2+Q29*0.25+V29*0.25+W29*0.3+X29*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+    </row>
+    <row r="31" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2915,7 +3479,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="9"/>
+      <c r="H31" s="69"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -2929,8 +3493,9 @@
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
       <c r="U31" s="9"/>
-    </row>
-    <row r="32" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V31" s="9"/>
+    </row>
+    <row r="32" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2938,7 +3503,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="9"/>
+      <c r="H32" s="69"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -2952,8 +3517,9 @@
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
       <c r="U32" s="9"/>
-    </row>
-    <row r="33" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V32" s="9"/>
+    </row>
+    <row r="33" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2961,7 +3527,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="9"/>
+      <c r="H33" s="69"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -2975,8 +3541,9 @@
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
       <c r="U33" s="9"/>
-    </row>
-    <row r="34" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V33" s="9"/>
+    </row>
+    <row r="34" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2984,7 +3551,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="9"/>
+      <c r="H34" s="69"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -2998,8 +3565,9 @@
       <c r="S34" s="9"/>
       <c r="T34" s="9"/>
       <c r="U34" s="9"/>
-    </row>
-    <row r="35" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V34" s="9"/>
+    </row>
+    <row r="35" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3007,7 +3575,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="9"/>
+      <c r="H35" s="69"/>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3021,8 +3589,9 @@
       <c r="S35" s="9"/>
       <c r="T35" s="9"/>
       <c r="U35" s="9"/>
-    </row>
-    <row r="36" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V35" s="9"/>
+    </row>
+    <row r="36" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -3030,7 +3599,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="9"/>
+      <c r="H36" s="69"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -3044,8 +3613,9 @@
       <c r="S36" s="9"/>
       <c r="T36" s="9"/>
       <c r="U36" s="9"/>
-    </row>
-    <row r="37" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V36" s="9"/>
+    </row>
+    <row r="37" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3053,7 +3623,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="9"/>
+      <c r="H37" s="69"/>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -3067,8 +3637,9 @@
       <c r="S37" s="9"/>
       <c r="T37" s="9"/>
       <c r="U37" s="9"/>
-    </row>
-    <row r="38" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V37" s="9"/>
+    </row>
+    <row r="38" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3076,7 +3647,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="9"/>
+      <c r="H38" s="69"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -3090,8 +3661,9 @@
       <c r="S38" s="9"/>
       <c r="T38" s="9"/>
       <c r="U38" s="9"/>
-    </row>
-    <row r="39" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V38" s="9"/>
+    </row>
+    <row r="39" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -3099,7 +3671,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="9"/>
+      <c r="H39" s="69"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -3113,8 +3685,9 @@
       <c r="S39" s="9"/>
       <c r="T39" s="9"/>
       <c r="U39" s="9"/>
-    </row>
-    <row r="40" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V39" s="9"/>
+    </row>
+    <row r="40" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -3122,7 +3695,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="9"/>
+      <c r="H40" s="69"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
@@ -3136,8 +3709,9 @@
       <c r="S40" s="9"/>
       <c r="T40" s="9"/>
       <c r="U40" s="9"/>
-    </row>
-    <row r="41" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V40" s="9"/>
+    </row>
+    <row r="41" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -3145,7 +3719,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="9"/>
+      <c r="H41" s="69"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
@@ -3159,8 +3733,9 @@
       <c r="S41" s="9"/>
       <c r="T41" s="9"/>
       <c r="U41" s="9"/>
-    </row>
-    <row r="42" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V41" s="9"/>
+    </row>
+    <row r="42" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -3168,7 +3743,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="9"/>
+      <c r="H42" s="69"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -3182,8 +3757,9 @@
       <c r="S42" s="9"/>
       <c r="T42" s="9"/>
       <c r="U42" s="9"/>
-    </row>
-    <row r="43" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V42" s="9"/>
+    </row>
+    <row r="43" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -3191,7 +3767,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="9"/>
+      <c r="H43" s="69"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
@@ -3205,8 +3781,9 @@
       <c r="S43" s="9"/>
       <c r="T43" s="9"/>
       <c r="U43" s="9"/>
-    </row>
-    <row r="44" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V43" s="9"/>
+    </row>
+    <row r="44" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -3214,7 +3791,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="9"/>
+      <c r="H44" s="69"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -3228,8 +3805,9 @@
       <c r="S44" s="9"/>
       <c r="T44" s="9"/>
       <c r="U44" s="9"/>
-    </row>
-    <row r="45" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V44" s="9"/>
+    </row>
+    <row r="45" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3237,7 +3815,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="9"/>
+      <c r="H45" s="69"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -3251,8 +3829,9 @@
       <c r="S45" s="9"/>
       <c r="T45" s="9"/>
       <c r="U45" s="9"/>
-    </row>
-    <row r="46" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V45" s="9"/>
+    </row>
+    <row r="46" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -3260,7 +3839,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="9"/>
+      <c r="H46" s="69"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -3274,8 +3853,9 @@
       <c r="S46" s="9"/>
       <c r="T46" s="9"/>
       <c r="U46" s="9"/>
-    </row>
-    <row r="47" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V46" s="9"/>
+    </row>
+    <row r="47" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -3283,7 +3863,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="9"/>
+      <c r="H47" s="69"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -3297,8 +3877,9 @@
       <c r="S47" s="9"/>
       <c r="T47" s="9"/>
       <c r="U47" s="9"/>
-    </row>
-    <row r="48" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V47" s="9"/>
+    </row>
+    <row r="48" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -3306,7 +3887,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="9"/>
+      <c r="H48" s="69"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -3320,8 +3901,9 @@
       <c r="S48" s="9"/>
       <c r="T48" s="9"/>
       <c r="U48" s="9"/>
-    </row>
-    <row r="49" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V48" s="9"/>
+    </row>
+    <row r="49" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -3329,7 +3911,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="9"/>
+      <c r="H49" s="69"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -3343,8 +3925,9 @@
       <c r="S49" s="9"/>
       <c r="T49" s="9"/>
       <c r="U49" s="9"/>
-    </row>
-    <row r="50" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V49" s="9"/>
+    </row>
+    <row r="50" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -3352,7 +3935,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="9"/>
+      <c r="H50" s="69"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
@@ -3366,8 +3949,9 @@
       <c r="S50" s="9"/>
       <c r="T50" s="9"/>
       <c r="U50" s="9"/>
-    </row>
-    <row r="51" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V50" s="9"/>
+    </row>
+    <row r="51" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -3375,7 +3959,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="9"/>
+      <c r="H51" s="69"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -3389,8 +3973,9 @@
       <c r="S51" s="9"/>
       <c r="T51" s="9"/>
       <c r="U51" s="9"/>
-    </row>
-    <row r="52" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V51" s="9"/>
+    </row>
+    <row r="52" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -3398,7 +3983,7 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
-      <c r="H52" s="9"/>
+      <c r="H52" s="69"/>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -3412,8 +3997,9 @@
       <c r="S52" s="9"/>
       <c r="T52" s="9"/>
       <c r="U52" s="9"/>
-    </row>
-    <row r="53" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V52" s="9"/>
+    </row>
+    <row r="53" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -3421,7 +4007,7 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="9"/>
+      <c r="H53" s="69"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -3435,8 +4021,9 @@
       <c r="S53" s="9"/>
       <c r="T53" s="9"/>
       <c r="U53" s="9"/>
-    </row>
-    <row r="54" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V53" s="9"/>
+    </row>
+    <row r="54" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -3444,7 +4031,7 @@
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
-      <c r="H54" s="9"/>
+      <c r="H54" s="69"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -3458,8 +4045,9 @@
       <c r="S54" s="9"/>
       <c r="T54" s="9"/>
       <c r="U54" s="9"/>
-    </row>
-    <row r="55" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V54" s="9"/>
+    </row>
+    <row r="55" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -3467,7 +4055,7 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
-      <c r="H55" s="9"/>
+      <c r="H55" s="69"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -3481,8 +4069,9 @@
       <c r="S55" s="9"/>
       <c r="T55" s="9"/>
       <c r="U55" s="9"/>
-    </row>
-    <row r="56" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V55" s="9"/>
+    </row>
+    <row r="56" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -3490,7 +4079,7 @@
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="9"/>
+      <c r="H56" s="69"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -3504,8 +4093,9 @@
       <c r="S56" s="9"/>
       <c r="T56" s="9"/>
       <c r="U56" s="9"/>
-    </row>
-    <row r="57" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V56" s="9"/>
+    </row>
+    <row r="57" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -3513,7 +4103,7 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="9"/>
+      <c r="H57" s="69"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -3527,8 +4117,9 @@
       <c r="S57" s="9"/>
       <c r="T57" s="9"/>
       <c r="U57" s="9"/>
-    </row>
-    <row r="58" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V57" s="9"/>
+    </row>
+    <row r="58" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -3536,7 +4127,7 @@
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
-      <c r="H58" s="9"/>
+      <c r="H58" s="69"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -3550,8 +4141,9 @@
       <c r="S58" s="9"/>
       <c r="T58" s="9"/>
       <c r="U58" s="9"/>
-    </row>
-    <row r="59" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V58" s="9"/>
+    </row>
+    <row r="59" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -3559,7 +4151,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="9"/>
+      <c r="H59" s="69"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -3573,8 +4165,9 @@
       <c r="S59" s="9"/>
       <c r="T59" s="9"/>
       <c r="U59" s="9"/>
-    </row>
-    <row r="60" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V59" s="9"/>
+    </row>
+    <row r="60" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -3582,7 +4175,7 @@
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="9"/>
+      <c r="H60" s="69"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -3596,8 +4189,9 @@
       <c r="S60" s="9"/>
       <c r="T60" s="9"/>
       <c r="U60" s="9"/>
-    </row>
-    <row r="61" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V60" s="9"/>
+    </row>
+    <row r="61" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -3605,7 +4199,7 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
-      <c r="H61" s="9"/>
+      <c r="H61" s="69"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -3619,8 +4213,9 @@
       <c r="S61" s="9"/>
       <c r="T61" s="9"/>
       <c r="U61" s="9"/>
-    </row>
-    <row r="62" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V61" s="9"/>
+    </row>
+    <row r="62" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -3628,7 +4223,7 @@
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
-      <c r="H62" s="9"/>
+      <c r="H62" s="69"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -3642,8 +4237,9 @@
       <c r="S62" s="9"/>
       <c r="T62" s="9"/>
       <c r="U62" s="9"/>
-    </row>
-    <row r="63" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V62" s="9"/>
+    </row>
+    <row r="63" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -3651,7 +4247,7 @@
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
-      <c r="H63" s="9"/>
+      <c r="H63" s="69"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -3665,8 +4261,9 @@
       <c r="S63" s="9"/>
       <c r="T63" s="9"/>
       <c r="U63" s="9"/>
-    </row>
-    <row r="64" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V63" s="9"/>
+    </row>
+    <row r="64" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -3674,7 +4271,7 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
-      <c r="H64" s="9"/>
+      <c r="H64" s="69"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -3688,8 +4285,9 @@
       <c r="S64" s="9"/>
       <c r="T64" s="9"/>
       <c r="U64" s="9"/>
-    </row>
-    <row r="65" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V64" s="9"/>
+    </row>
+    <row r="65" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -3697,7 +4295,7 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="9"/>
+      <c r="H65" s="69"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -3711,8 +4309,9 @@
       <c r="S65" s="9"/>
       <c r="T65" s="9"/>
       <c r="U65" s="9"/>
-    </row>
-    <row r="66" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V65" s="9"/>
+    </row>
+    <row r="66" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -3720,7 +4319,7 @@
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
-      <c r="H66" s="9"/>
+      <c r="H66" s="69"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -3734,8 +4333,9 @@
       <c r="S66" s="9"/>
       <c r="T66" s="9"/>
       <c r="U66" s="9"/>
-    </row>
-    <row r="67" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V66" s="9"/>
+    </row>
+    <row r="67" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -3743,7 +4343,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="9"/>
+      <c r="H67" s="69"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -3757,8 +4357,9 @@
       <c r="S67" s="9"/>
       <c r="T67" s="9"/>
       <c r="U67" s="9"/>
-    </row>
-    <row r="68" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V67" s="9"/>
+    </row>
+    <row r="68" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -3766,7 +4367,7 @@
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
-      <c r="H68" s="9"/>
+      <c r="H68" s="69"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -3780,8 +4381,9 @@
       <c r="S68" s="9"/>
       <c r="T68" s="9"/>
       <c r="U68" s="9"/>
-    </row>
-    <row r="69" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V68" s="9"/>
+    </row>
+    <row r="69" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -3789,7 +4391,7 @@
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
-      <c r="H69" s="9"/>
+      <c r="H69" s="69"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -3803,8 +4405,9 @@
       <c r="S69" s="9"/>
       <c r="T69" s="9"/>
       <c r="U69" s="9"/>
-    </row>
-    <row r="70" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V69" s="9"/>
+    </row>
+    <row r="70" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -3812,7 +4415,7 @@
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
-      <c r="H70" s="9"/>
+      <c r="H70" s="69"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -3826,8 +4429,9 @@
       <c r="S70" s="9"/>
       <c r="T70" s="9"/>
       <c r="U70" s="9"/>
-    </row>
-    <row r="71" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V70" s="9"/>
+    </row>
+    <row r="71" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -3835,7 +4439,7 @@
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
-      <c r="H71" s="9"/>
+      <c r="H71" s="69"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -3849,8 +4453,9 @@
       <c r="S71" s="9"/>
       <c r="T71" s="9"/>
       <c r="U71" s="9"/>
-    </row>
-    <row r="72" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V71" s="9"/>
+    </row>
+    <row r="72" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -3858,7 +4463,7 @@
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
-      <c r="H72" s="9"/>
+      <c r="H72" s="69"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -3872,8 +4477,9 @@
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
       <c r="U72" s="9"/>
-    </row>
-    <row r="73" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V72" s="9"/>
+    </row>
+    <row r="73" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -3881,7 +4487,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
-      <c r="H73" s="9"/>
+      <c r="H73" s="69"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -3895,8 +4501,9 @@
       <c r="S73" s="9"/>
       <c r="T73" s="9"/>
       <c r="U73" s="9"/>
-    </row>
-    <row r="74" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V73" s="9"/>
+    </row>
+    <row r="74" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -3904,7 +4511,7 @@
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
-      <c r="H74" s="9"/>
+      <c r="H74" s="69"/>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -3918,8 +4525,9 @@
       <c r="S74" s="9"/>
       <c r="T74" s="9"/>
       <c r="U74" s="9"/>
-    </row>
-    <row r="75" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V74" s="9"/>
+    </row>
+    <row r="75" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -3927,7 +4535,7 @@
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
-      <c r="H75" s="9"/>
+      <c r="H75" s="69"/>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -3941,87 +4549,65 @@
       <c r="S75" s="9"/>
       <c r="T75" s="9"/>
       <c r="U75" s="9"/>
-    </row>
-    <row r="76" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="8"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
-      <c r="L76" s="9"/>
-      <c r="M76" s="9"/>
-      <c r="N76" s="9"/>
-      <c r="O76" s="9"/>
-      <c r="P76" s="9"/>
-      <c r="Q76" s="9"/>
-      <c r="R76" s="9"/>
-      <c r="S76" s="9"/>
-      <c r="T76" s="9"/>
-      <c r="U76" s="9"/>
+      <c r="V75" s="9"/>
     </row>
   </sheetData>
-  <sortState ref="A3:AB30">
-    <sortCondition descending="1" ref="X2"/>
+  <sortState ref="A3:Z30">
+    <sortCondition descending="1" ref="Y3"/>
   </sortState>
   <mergeCells count="3">
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:J30">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="between">
+  <conditionalFormatting sqref="D3:J29">
+    <cfRule type="cellIs" dxfId="32" priority="19" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:W30 L3:O30">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
+  <conditionalFormatting sqref="W3:X29 M3:P29">
+    <cfRule type="cellIs" dxfId="29" priority="10" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:T30">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
+  <conditionalFormatting sqref="R3:U29">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="between">
       <formula>80</formula>
       <formula>200</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K30">
-    <cfRule type="dataBar" priority="182">
+  <conditionalFormatting sqref="L3:L29">
+    <cfRule type="dataBar" priority="189">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4034,8 +4620,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P30">
-    <cfRule type="dataBar" priority="184">
+  <conditionalFormatting sqref="Q3:Q29">
+    <cfRule type="dataBar" priority="190">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4048,8 +4634,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U30">
-    <cfRule type="dataBar" priority="186">
+  <conditionalFormatting sqref="V3:V29">
+    <cfRule type="dataBar" priority="191">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4062,8 +4648,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3:X30">
-    <cfRule type="dataBar" priority="188">
+  <conditionalFormatting sqref="Y3:Y29">
+    <cfRule type="dataBar" priority="192">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4091,7 +4677,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K3:K30</xm:sqref>
+          <xm:sqref>L3:L29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C1E54EB9-FD52-4CFD-8B29-7F3B7B6681D5}">
@@ -4102,7 +4688,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>P3:P30</xm:sqref>
+          <xm:sqref>Q3:Q29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{03C5F189-3F43-4B84-A0F5-49F108E9F2B6}">
@@ -4113,7 +4699,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U3:U30</xm:sqref>
+          <xm:sqref>V3:V29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{43DC70F4-8291-4430-AFF0-577FC5E79CD9}">
@@ -4124,7 +4710,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>X3:X30</xm:sqref>
+          <xm:sqref>Y3:Y29</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5770,14 +6356,14 @@
     <mergeCell ref="K1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:I33">
-    <cfRule type="cellIs" dxfId="10" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5824,18 +6410,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:O33">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
@@ -5883,18 +6469,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q33">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThanOrEqual">
       <formula>80</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ileri java hafta 6
</commit_message>
<xml_diff>
--- a/AdvancedJava/_docs/Notlar.xlsx
+++ b/AdvancedJava/_docs/Notlar.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t>Adı</t>
   </si>
@@ -359,6 +359,15 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>FUAT</t>
+  </si>
+  <si>
+    <t>SEKİZKARDEŞ</t>
+  </si>
+  <si>
+    <t>H5150063</t>
   </si>
 </sst>
 </file>
@@ -764,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -867,22 +876,6 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -900,11 +893,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="22">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1084,248 +1092,6 @@
         <patternFill>
           <fgColor auto="1"/>
           <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1640,11 +1406,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z75"/>
+  <dimension ref="A1:Z76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1654,7 +1420,7 @@
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.44140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.44140625" style="64" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.44140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -1677,36 +1443,36 @@
       <c r="A1" s="30"/>
       <c r="B1" s="18"/>
       <c r="C1" s="29"/>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="46">
-        <v>4</v>
-      </c>
-      <c r="M1" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
       <c r="Q1" s="45">
-        <v>1</v>
-      </c>
-      <c r="R1" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
       <c r="V1" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W1" s="17" t="s">
         <v>34</v>
@@ -1740,7 +1506,7 @@
       <c r="G2" s="27">
         <v>4</v>
       </c>
-      <c r="H2" s="66">
+      <c r="H2" s="60">
         <v>5</v>
       </c>
       <c r="I2" s="27">
@@ -1817,22 +1583,26 @@
       <c r="G3" s="7">
         <v>2</v>
       </c>
-      <c r="H3" s="67">
-        <v>2</v>
-      </c>
-      <c r="I3" s="7"/>
+      <c r="H3" s="61">
+        <v>2</v>
+      </c>
+      <c r="I3" s="7">
+        <v>2</v>
+      </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="64">
+      <c r="K3" s="58">
         <v>0</v>
       </c>
       <c r="L3" s="16">
         <f>SUM(D3:J3)*50/(L$1-K3)</f>
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="M3" s="14">
         <v>100</v>
       </c>
-      <c r="N3" s="6"/>
+      <c r="N3" s="6">
+        <v>100</v>
+      </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="16">
@@ -1842,7 +1612,9 @@
       <c r="R3" s="14">
         <v>60</v>
       </c>
-      <c r="S3" s="14"/>
+      <c r="S3" s="14">
+        <v>60</v>
+      </c>
       <c r="T3" s="14"/>
       <c r="U3" s="14"/>
       <c r="V3" s="16">
@@ -1853,7 +1625,7 @@
       <c r="X3" s="44"/>
       <c r="Y3" s="21">
         <f>L3*0.2+Q3*0.25+V3*0.25+W3*0.3+X3*0.15</f>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>37</v>
@@ -1881,32 +1653,38 @@
       <c r="G4" s="7">
         <v>2</v>
       </c>
-      <c r="H4" s="67">
-        <v>2</v>
-      </c>
-      <c r="I4" s="7"/>
+      <c r="H4" s="61">
+        <v>2</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2</v>
+      </c>
       <c r="J4" s="7"/>
-      <c r="K4" s="64">
+      <c r="K4" s="58">
         <v>0</v>
       </c>
       <c r="L4" s="16">
-        <f t="shared" ref="L4:L29" si="0">SUM(D4:J4)*50/(L$1-K4)</f>
-        <v>125</v>
+        <f>SUM(D4:J4)*50/(L$1-K4)</f>
+        <v>120</v>
       </c>
       <c r="M4" s="14">
         <v>95</v>
       </c>
-      <c r="N4" s="6"/>
+      <c r="N4" s="6">
+        <v>100</v>
+      </c>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="16">
         <f>SUM(M4:P4)/Q$1</f>
-        <v>95</v>
+        <v>97.5</v>
       </c>
       <c r="R4" s="14">
         <v>60</v>
       </c>
-      <c r="S4" s="14"/>
+      <c r="S4" s="14">
+        <v>60</v>
+      </c>
       <c r="T4" s="14"/>
       <c r="U4" s="14"/>
       <c r="V4" s="16">
@@ -1917,18 +1695,18 @@
       <c r="X4" s="44"/>
       <c r="Y4" s="21">
         <f>L4*0.2+Q4*0.25+V4*0.25+W4*0.3+X4*0.15</f>
-        <v>63.75</v>
+        <v>63.375</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D5" s="12">
         <v>0</v>
@@ -1942,32 +1720,38 @@
       <c r="G5" s="7">
         <v>2</v>
       </c>
-      <c r="H5" s="67">
-        <v>2</v>
-      </c>
-      <c r="I5" s="7"/>
+      <c r="H5" s="61">
+        <v>2</v>
+      </c>
+      <c r="I5" s="7">
+        <v>2</v>
+      </c>
       <c r="J5" s="7"/>
-      <c r="K5" s="64">
+      <c r="K5" s="58">
         <v>0</v>
       </c>
       <c r="L5" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D5:J5)*50/(L$1-K5)</f>
         <v>100</v>
       </c>
       <c r="M5" s="14">
+        <v>95</v>
+      </c>
+      <c r="N5" s="6">
         <v>100</v>
       </c>
-      <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="16">
         <f>SUM(M5:P5)/Q$1</f>
-        <v>100</v>
+        <v>97.5</v>
       </c>
       <c r="R5" s="14">
         <v>60</v>
       </c>
-      <c r="S5" s="14"/>
+      <c r="S5" s="14">
+        <v>60</v>
+      </c>
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
       <c r="V5" s="16">
@@ -1977,19 +1761,19 @@
       <c r="W5" s="6"/>
       <c r="X5" s="44"/>
       <c r="Y5" s="21">
-        <f>L5*0.2+Q5*0.25+V5*0.25+W5*0.3+X5*0.1</f>
-        <v>60</v>
+        <f>L5*0.2+Q5*0.25+V5*0.25+W5*0.3+X5*0.15</f>
+        <v>59.375</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D6" s="12">
         <v>0</v>
@@ -2003,32 +1787,38 @@
       <c r="G6" s="7">
         <v>2</v>
       </c>
-      <c r="H6" s="67">
-        <v>2</v>
-      </c>
-      <c r="I6" s="7"/>
+      <c r="H6" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1.8</v>
+      </c>
       <c r="J6" s="7"/>
-      <c r="K6" s="64">
-        <v>0</v>
+      <c r="K6" s="59">
+        <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>SUM(D6:J6)*50/(L$1-K6)</f>
+        <v>97.5</v>
       </c>
       <c r="M6" s="14">
         <v>95</v>
       </c>
-      <c r="N6" s="6"/>
+      <c r="N6" s="6">
+        <v>100</v>
+      </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="16">
         <f>SUM(M6:P6)/Q$1</f>
-        <v>95</v>
+        <v>97.5</v>
       </c>
       <c r="R6" s="14">
         <v>60</v>
       </c>
-      <c r="S6" s="14"/>
+      <c r="S6" s="14">
+        <v>60</v>
+      </c>
       <c r="T6" s="14"/>
       <c r="U6" s="14"/>
       <c r="V6" s="16">
@@ -2039,18 +1829,18 @@
       <c r="X6" s="44"/>
       <c r="Y6" s="21">
         <f>L6*0.2+Q6*0.25+V6*0.25+W6*0.3+X6*0.15</f>
-        <v>58.75</v>
+        <v>58.875</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D7" s="12">
         <v>0</v>
@@ -2064,22 +1854,26 @@
       <c r="G7" s="7">
         <v>2</v>
       </c>
-      <c r="H7" s="67" t="s">
-        <v>96</v>
-      </c>
-      <c r="I7" s="7"/>
+      <c r="H7" s="61">
+        <v>2</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2</v>
+      </c>
       <c r="J7" s="7"/>
-      <c r="K7" s="65">
-        <v>1</v>
+      <c r="K7" s="58">
+        <v>0</v>
       </c>
       <c r="L7" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D7:J7)*50/(L$1-K7)</f>
         <v>100</v>
       </c>
       <c r="M7" s="14">
-        <v>95</v>
-      </c>
-      <c r="N7" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="N7" s="6">
+        <v>90</v>
+      </c>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="16">
@@ -2089,7 +1883,9 @@
       <c r="R7" s="14">
         <v>60</v>
       </c>
-      <c r="S7" s="14"/>
+      <c r="S7" s="14">
+        <v>60</v>
+      </c>
       <c r="T7" s="14"/>
       <c r="U7" s="14"/>
       <c r="V7" s="16">
@@ -2099,19 +1895,19 @@
       <c r="W7" s="6"/>
       <c r="X7" s="44"/>
       <c r="Y7" s="21">
-        <f>L7*0.2+Q7*0.25+V7*0.25+W7*0.3+X7*0.15</f>
+        <f>L7*0.2+Q7*0.25+V7*0.25+W7*0.3+X7*0.1</f>
         <v>58.75</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D8" s="12">
         <v>0</v>
@@ -2123,24 +1919,28 @@
         <v>2</v>
       </c>
       <c r="G8" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="H8" s="67">
-        <v>2</v>
-      </c>
-      <c r="I8" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="H8" s="61">
+        <v>2</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2</v>
+      </c>
       <c r="J8" s="7"/>
-      <c r="K8" s="64">
+      <c r="K8" s="58">
         <v>0</v>
       </c>
       <c r="L8" s="16">
-        <f t="shared" si="0"/>
-        <v>97.5</v>
+        <f>SUM(D8:J8)*50/(L$1-K8)</f>
+        <v>100</v>
       </c>
       <c r="M8" s="14">
-        <v>95</v>
-      </c>
-      <c r="N8" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="N8" s="6">
+        <v>100</v>
+      </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="16">
@@ -2150,7 +1950,9 @@
       <c r="R8" s="14">
         <v>60</v>
       </c>
-      <c r="S8" s="14"/>
+      <c r="S8" s="14">
+        <v>60</v>
+      </c>
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
       <c r="V8" s="16">
@@ -2161,21 +1963,21 @@
       <c r="X8" s="44"/>
       <c r="Y8" s="21">
         <f>L8*0.2+Q8*0.25+V8*0.25+W8*0.3+X8*0.15</f>
-        <v>58.25</v>
+        <v>58.75</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D9" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="7">
         <v>2</v>
@@ -2186,54 +1988,60 @@
       <c r="G9" s="7">
         <v>2</v>
       </c>
-      <c r="H9" s="67">
-        <v>2</v>
-      </c>
-      <c r="I9" s="7"/>
+      <c r="H9" s="61">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2</v>
+      </c>
       <c r="J9" s="7"/>
-      <c r="K9" s="64">
+      <c r="K9" s="58">
         <v>0</v>
       </c>
       <c r="L9" s="16">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>SUM(D9:J9)*50/(L$1-K9)</f>
+        <v>120</v>
       </c>
       <c r="M9" s="14">
+        <v>85</v>
+      </c>
+      <c r="N9" s="6">
         <v>90</v>
       </c>
-      <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="16">
         <f>SUM(M9:P9)/Q$1</f>
-        <v>90</v>
+        <v>87.5</v>
       </c>
       <c r="R9" s="14">
+        <v>40</v>
+      </c>
+      <c r="S9" s="14">
         <v>60</v>
       </c>
-      <c r="S9" s="14"/>
       <c r="T9" s="14"/>
       <c r="U9" s="14"/>
       <c r="V9" s="16">
         <f>SUM(R9:U9)/V$1</f>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="W9" s="6"/>
       <c r="X9" s="44"/>
       <c r="Y9" s="21">
         <f>L9*0.2+Q9*0.25+V9*0.25+W9*0.3+X9*0.15</f>
-        <v>57.5</v>
+        <v>58.375</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="D10" s="12">
         <v>0</v>
@@ -2245,34 +2053,40 @@
         <v>2</v>
       </c>
       <c r="G10" s="7">
-        <v>2</v>
-      </c>
-      <c r="H10" s="67">
-        <v>1.7</v>
-      </c>
-      <c r="I10" s="7"/>
+        <v>1.8</v>
+      </c>
+      <c r="H10" s="61">
+        <v>2</v>
+      </c>
+      <c r="I10" s="7">
+        <v>2</v>
+      </c>
       <c r="J10" s="7"/>
-      <c r="K10" s="64">
+      <c r="K10" s="58">
         <v>0</v>
       </c>
       <c r="L10" s="16">
-        <f t="shared" si="0"/>
-        <v>96.25</v>
+        <f>SUM(D10:J10)*50/(L$1-K10)</f>
+        <v>98.000000000000014</v>
       </c>
       <c r="M10" s="14">
-        <v>90</v>
-      </c>
-      <c r="N10" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="N10" s="6">
+        <v>95</v>
+      </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="16">
         <f>SUM(M10:P10)/Q$1</f>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="R10" s="14">
         <v>60</v>
       </c>
-      <c r="S10" s="14"/>
+      <c r="S10" s="14">
+        <v>60</v>
+      </c>
       <c r="T10" s="14"/>
       <c r="U10" s="14"/>
       <c r="V10" s="16">
@@ -2283,18 +2097,18 @@
       <c r="X10" s="44"/>
       <c r="Y10" s="21">
         <f>L10*0.2+Q10*0.25+V10*0.25+W10*0.3+X10*0.15</f>
-        <v>56.75</v>
+        <v>58.350000000000009</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="D11" s="12">
         <v>0</v>
@@ -2308,32 +2122,38 @@
       <c r="G11" s="7">
         <v>2</v>
       </c>
-      <c r="H11" s="67">
-        <v>2</v>
-      </c>
-      <c r="I11" s="7"/>
+      <c r="H11" s="61">
+        <v>1.7</v>
+      </c>
+      <c r="I11" s="7">
+        <v>2</v>
+      </c>
       <c r="J11" s="7"/>
-      <c r="K11" s="64">
+      <c r="K11" s="58">
         <v>0</v>
       </c>
       <c r="L11" s="16">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>SUM(D11:J11)*50/(L$1-K11)</f>
+        <v>96.999999999999986</v>
       </c>
       <c r="M11" s="14">
         <v>90</v>
       </c>
-      <c r="N11" s="6"/>
+      <c r="N11" s="6">
+        <v>85</v>
+      </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="16">
         <f>SUM(M11:P11)/Q$1</f>
-        <v>90</v>
+        <v>87.5</v>
       </c>
       <c r="R11" s="14">
         <v>60</v>
       </c>
-      <c r="S11" s="14"/>
+      <c r="S11" s="14">
+        <v>60</v>
+      </c>
       <c r="T11" s="14"/>
       <c r="U11" s="14"/>
       <c r="V11" s="16">
@@ -2344,21 +2164,21 @@
       <c r="X11" s="44"/>
       <c r="Y11" s="21">
         <f>L11*0.2+Q11*0.25+V11*0.25+W11*0.3+X11*0.15</f>
-        <v>57.5</v>
+        <v>56.274999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="D12" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E12" s="7">
         <v>2</v>
@@ -2369,22 +2189,26 @@
       <c r="G12" s="7">
         <v>2</v>
       </c>
-      <c r="H12" s="67">
-        <v>2</v>
-      </c>
-      <c r="I12" s="7"/>
+      <c r="H12" s="61">
+        <v>2</v>
+      </c>
+      <c r="I12" s="7">
+        <v>2</v>
+      </c>
       <c r="J12" s="7"/>
-      <c r="K12" s="64">
+      <c r="K12" s="58">
         <v>0</v>
       </c>
       <c r="L12" s="16">
-        <f t="shared" si="0"/>
-        <v>125</v>
+        <f>SUM(D12:J12)*50/(L$1-K12)</f>
+        <v>100</v>
       </c>
       <c r="M12" s="14">
-        <v>85</v>
-      </c>
-      <c r="N12" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="N12" s="6">
+        <v>80</v>
+      </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="16">
@@ -2392,34 +2216,36 @@
         <v>85</v>
       </c>
       <c r="R12" s="14">
-        <v>0</v>
-      </c>
-      <c r="S12" s="14"/>
+        <v>60</v>
+      </c>
+      <c r="S12" s="14">
+        <v>60</v>
+      </c>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
       <c r="V12" s="16">
         <f>SUM(R12:U12)/V$1</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="W12" s="6"/>
       <c r="X12" s="44"/>
       <c r="Y12" s="21">
         <f>L12*0.2+Q12*0.25+V12*0.25+W12*0.3+X12*0.15</f>
-        <v>46.25</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="D13" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
@@ -2430,57 +2256,63 @@
       <c r="G13" s="7">
         <v>2</v>
       </c>
-      <c r="H13" s="67">
-        <v>2</v>
-      </c>
-      <c r="I13" s="7"/>
+      <c r="H13" s="61">
+        <v>2</v>
+      </c>
+      <c r="I13" s="7">
+        <v>2</v>
+      </c>
       <c r="J13" s="7"/>
-      <c r="K13" s="64">
+      <c r="K13" s="58">
         <v>0</v>
       </c>
       <c r="L13" s="16">
-        <f t="shared" si="0"/>
-        <v>125</v>
+        <f>SUM(D13:J13)*50/(L$1-K13)</f>
+        <v>100</v>
       </c>
       <c r="M13" s="14">
-        <v>80</v>
-      </c>
-      <c r="N13" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="N13" s="6">
+        <v>90</v>
+      </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="16">
         <f>SUM(M13:P13)/Q$1</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="R13" s="14">
-        <v>0</v>
-      </c>
-      <c r="S13" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="S13" s="14">
+        <v>60</v>
+      </c>
       <c r="T13" s="14"/>
       <c r="U13" s="14"/>
       <c r="V13" s="16">
         <f>SUM(R13:U13)/V$1</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="W13" s="6"/>
       <c r="X13" s="44"/>
       <c r="Y13" s="21">
         <f>L13*0.2+Q13*0.25+V13*0.25+W13*0.3+X13*0.15</f>
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="D14" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14" s="7">
         <v>2</v>
@@ -2491,54 +2323,60 @@
       <c r="G14" s="7">
         <v>2</v>
       </c>
-      <c r="H14" s="67">
-        <v>2</v>
-      </c>
-      <c r="I14" s="7"/>
+      <c r="H14" s="61">
+        <v>2</v>
+      </c>
+      <c r="I14" s="7">
+        <v>2</v>
+      </c>
       <c r="J14" s="7"/>
-      <c r="K14" s="64">
+      <c r="K14" s="58">
         <v>0</v>
       </c>
       <c r="L14" s="16">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>SUM(D14:J14)*50/(L$1-K14)</f>
+        <v>120</v>
       </c>
       <c r="M14" s="14">
+        <v>80</v>
+      </c>
+      <c r="N14" s="6">
         <v>90</v>
       </c>
-      <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="16">
         <f>SUM(M14:P14)/Q$1</f>
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R14" s="14">
         <v>0</v>
       </c>
-      <c r="S14" s="14"/>
+      <c r="S14" s="14">
+        <v>60</v>
+      </c>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
       <c r="V14" s="16">
         <f>SUM(R14:U14)/V$1</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="W14" s="6"/>
       <c r="X14" s="44"/>
       <c r="Y14" s="21">
         <f>L14*0.2+Q14*0.25+V14*0.25+W14*0.3+X14*0.15</f>
-        <v>42.5</v>
+        <v>52.75</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
@@ -2547,48 +2385,54 @@
         <v>2</v>
       </c>
       <c r="F15" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="7">
         <v>2</v>
       </c>
-      <c r="H15" s="67">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7"/>
+      <c r="H15" s="61">
+        <v>2</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1.8</v>
+      </c>
       <c r="J15" s="7"/>
-      <c r="K15" s="64">
+      <c r="K15" s="58">
         <v>0</v>
       </c>
       <c r="L15" s="16">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f>SUM(D15:J15)*50/(L$1-K15)</f>
+        <v>78</v>
       </c>
       <c r="M15" s="14">
-        <v>85</v>
-      </c>
-      <c r="N15" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="N15" s="6">
+        <v>100</v>
+      </c>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="16">
         <f>SUM(M15:P15)/Q$1</f>
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="R15" s="14">
-        <v>0</v>
-      </c>
-      <c r="S15" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="S15" s="14">
+        <v>60</v>
+      </c>
       <c r="T15" s="14"/>
       <c r="U15" s="14"/>
       <c r="V15" s="16">
         <f>SUM(R15:U15)/V$1</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="W15" s="6"/>
       <c r="X15" s="44"/>
       <c r="Y15" s="21">
         <f>L15*0.2+Q15*0.25+V15*0.25+W15*0.3+X15*0.15</f>
-        <v>36.25</v>
+        <v>51.85</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2613,32 +2457,38 @@
       <c r="G16" s="7">
         <v>0</v>
       </c>
-      <c r="H16" s="67">
-        <v>2</v>
-      </c>
-      <c r="I16" s="7"/>
+      <c r="H16" s="61">
+        <v>2</v>
+      </c>
+      <c r="I16" s="7">
+        <v>2</v>
+      </c>
       <c r="J16" s="7"/>
-      <c r="K16" s="64">
+      <c r="K16" s="58">
         <v>0</v>
       </c>
       <c r="L16" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D16:J16)*50/(L$1-K16)</f>
         <v>100</v>
       </c>
       <c r="M16" s="14">
         <v>0</v>
       </c>
-      <c r="N16" s="6"/>
+      <c r="N16" s="6">
+        <v>100</v>
+      </c>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="16">
         <f>SUM(M16:P16)/Q$1</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="R16" s="14">
         <v>60</v>
       </c>
-      <c r="S16" s="14"/>
+      <c r="S16" s="14">
+        <v>60</v>
+      </c>
       <c r="T16" s="14"/>
       <c r="U16" s="14"/>
       <c r="V16" s="16">
@@ -2649,18 +2499,18 @@
       <c r="X16" s="44"/>
       <c r="Y16" s="21">
         <f>L16*0.2+Q16*0.25+V16*0.25+W16*0.3+X16*0.15</f>
-        <v>35</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="D17" s="12">
         <v>0</v>
@@ -2669,27 +2519,31 @@
         <v>2</v>
       </c>
       <c r="F17" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="7">
         <v>2</v>
       </c>
-      <c r="H17" s="67">
-        <v>2</v>
-      </c>
-      <c r="I17" s="7"/>
+      <c r="H17" s="61">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
+        <v>2</v>
+      </c>
       <c r="J17" s="7"/>
-      <c r="K17" s="64">
+      <c r="K17" s="58">
         <v>0</v>
       </c>
       <c r="L17" s="16">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f>SUM(D17:J17)*50/(L$1-K17)</f>
+        <v>80</v>
       </c>
       <c r="M17" s="14">
-        <v>90</v>
-      </c>
-      <c r="N17" s="6"/>
+        <v>85</v>
+      </c>
+      <c r="N17" s="6">
+        <v>95</v>
+      </c>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="16">
@@ -2697,20 +2551,22 @@
         <v>90</v>
       </c>
       <c r="R17" s="14">
-        <v>0</v>
-      </c>
-      <c r="S17" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="S17" s="14">
+        <v>0</v>
+      </c>
       <c r="T17" s="14"/>
       <c r="U17" s="14"/>
       <c r="V17" s="16">
         <f>SUM(R17:U17)/V$1</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W17" s="6"/>
       <c r="X17" s="44"/>
       <c r="Y17" s="21">
         <f>L17*0.2+Q17*0.25+V17*0.25+W17*0.3+X17*0.15</f>
-        <v>37.5</v>
+        <v>43.5</v>
       </c>
     </row>
     <row r="18" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2735,22 +2591,26 @@
       <c r="G18" s="12">
         <v>0</v>
       </c>
-      <c r="H18" s="67">
-        <v>2</v>
-      </c>
-      <c r="I18" s="7"/>
+      <c r="H18" s="61">
+        <v>2</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0</v>
+      </c>
       <c r="J18" s="7"/>
-      <c r="K18" s="64">
+      <c r="K18" s="58">
         <v>0</v>
       </c>
       <c r="L18" s="16">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>SUM(D18:J18)*50/(L$1-K18)</f>
+        <v>20</v>
       </c>
       <c r="M18" s="14">
         <v>0</v>
       </c>
-      <c r="N18" s="6"/>
+      <c r="N18" s="6">
+        <v>0</v>
+      </c>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="16">
@@ -2758,216 +2618,235 @@
         <v>0</v>
       </c>
       <c r="R18" s="14">
-        <v>0</v>
-      </c>
-      <c r="S18" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="S18" s="14">
+        <v>60</v>
+      </c>
       <c r="T18" s="14"/>
       <c r="U18" s="14"/>
       <c r="V18" s="16">
         <f>SUM(R18:U18)/V$1</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="W18" s="6"/>
       <c r="X18" s="44"/>
       <c r="Y18" s="21">
         <f>L18*0.2+Q18*0.25+V18*0.25+W18*0.3+X18*0.15</f>
-        <v>5</v>
+        <v>16.5</v>
       </c>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="50">
-        <v>0</v>
-      </c>
-      <c r="E19" s="50">
-        <v>0</v>
-      </c>
-      <c r="F19" s="50">
-        <v>0</v>
-      </c>
-      <c r="G19" s="50">
-        <v>0</v>
-      </c>
-      <c r="H19" s="68">
-        <v>0</v>
-      </c>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="64">
-        <v>0</v>
-      </c>
+    <row r="19" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0</v>
+      </c>
+      <c r="E19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12">
+        <v>0</v>
+      </c>
+      <c r="H19" s="61">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7">
+        <v>2</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="58"/>
       <c r="L19" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="53">
-        <v>0</v>
-      </c>
-      <c r="N19" s="54"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="54"/>
-      <c r="Q19" s="52">
+        <f>SUM(D19:J19)*50/(L$1-K19)</f>
+        <v>20</v>
+      </c>
+      <c r="M19" s="14">
+        <v>0</v>
+      </c>
+      <c r="N19" s="6">
+        <v>75</v>
+      </c>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="16">
         <f>SUM(M19:P19)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R19" s="53">
-        <v>0</v>
-      </c>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="52">
+        <v>37.5</v>
+      </c>
+      <c r="R19" s="14">
+        <v>0</v>
+      </c>
+      <c r="S19" s="14">
+        <v>0</v>
+      </c>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="16">
         <f>SUM(R19:U19)/V$1</f>
         <v>0</v>
       </c>
-      <c r="W19" s="54"/>
-      <c r="X19" s="55"/>
-      <c r="Y19" s="56">
-        <f>L19*0.2+Q19*0.25+V19*0.25+W19*0.3+X19*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="50">
-        <v>0</v>
-      </c>
-      <c r="E20" s="50">
-        <v>0</v>
-      </c>
-      <c r="F20" s="50">
-        <v>0</v>
-      </c>
-      <c r="G20" s="50">
-        <v>0</v>
-      </c>
-      <c r="H20" s="68">
-        <v>0</v>
-      </c>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="64">
+      <c r="W19" s="6"/>
+      <c r="X19" s="44"/>
+      <c r="Y19" s="21">
+        <f>L19*0.2+Q19*0.25+V19*0.25+W19*0.3+X19*0.1</f>
+        <v>13.375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0</v>
+      </c>
+      <c r="H20" s="61">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="58">
         <v>0</v>
       </c>
       <c r="L20" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="53">
-        <v>0</v>
-      </c>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
-      <c r="P20" s="54"/>
-      <c r="Q20" s="52">
+        <f>SUM(D20:J20)*50/(L$1-K20)</f>
+        <v>16</v>
+      </c>
+      <c r="M20" s="14">
+        <v>0</v>
+      </c>
+      <c r="N20" s="6">
+        <v>40</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="16">
         <f>SUM(M20:P20)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R20" s="53">
-        <v>0</v>
-      </c>
-      <c r="S20" s="53"/>
-      <c r="T20" s="53"/>
-      <c r="U20" s="53"/>
-      <c r="V20" s="52">
+        <v>20</v>
+      </c>
+      <c r="R20" s="14">
+        <v>0</v>
+      </c>
+      <c r="S20" s="14">
+        <v>0</v>
+      </c>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="16">
         <f>SUM(R20:U20)/V$1</f>
         <v>0</v>
       </c>
-      <c r="W20" s="54"/>
-      <c r="X20" s="55"/>
-      <c r="Y20" s="56">
-        <f>L20*0.2+Q20*0.25+V20*0.25+W20*0.3+X20*0.15</f>
-        <v>0</v>
-      </c>
-      <c r="Z20" s="57"/>
-    </row>
-    <row r="21" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="48" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="49" t="s">
+      <c r="W20" s="6"/>
+      <c r="X20" s="44"/>
+      <c r="Y20" s="21">
+        <f>L20*0.2+Q20*0.25+V20*0.25+W20*0.3+X20*0.1</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="Z20" s="1"/>
+    </row>
+    <row r="21" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="12">
+        <v>0</v>
+      </c>
+      <c r="E21" s="12">
+        <v>0</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0</v>
+      </c>
+      <c r="G21" s="12">
+        <v>0</v>
+      </c>
+      <c r="H21" s="61">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" s="58">
+        <v>0</v>
+      </c>
+      <c r="L21" s="16">
+        <f>SUM(D21:J21)*50/(L$1-K21)</f>
         <v>9</v>
       </c>
-      <c r="D21" s="50">
-        <v>0</v>
-      </c>
-      <c r="E21" s="50">
-        <v>0</v>
-      </c>
-      <c r="F21" s="50">
-        <v>0</v>
-      </c>
-      <c r="G21" s="50">
-        <v>0</v>
-      </c>
-      <c r="H21" s="68">
-        <v>0</v>
-      </c>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="64">
-        <v>0</v>
-      </c>
-      <c r="L21" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="53">
-        <v>0</v>
-      </c>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="52">
+      <c r="M21" s="14">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6">
+        <v>40</v>
+      </c>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="16">
         <f>SUM(M21:P21)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R21" s="53">
-        <v>0</v>
-      </c>
-      <c r="S21" s="53"/>
-      <c r="T21" s="53"/>
-      <c r="U21" s="53"/>
-      <c r="V21" s="52">
+        <v>20</v>
+      </c>
+      <c r="R21" s="14">
+        <v>0</v>
+      </c>
+      <c r="S21" s="14">
+        <v>0</v>
+      </c>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="16">
         <f>SUM(R21:U21)/V$1</f>
         <v>0</v>
       </c>
-      <c r="W21" s="54"/>
-      <c r="X21" s="55"/>
-      <c r="Y21" s="56">
-        <f>L21*0.2+Q21*0.25+V21*0.25+W21*0.3+X21*0.15</f>
-        <v>0</v>
-      </c>
+      <c r="W21" s="6"/>
+      <c r="X21" s="44"/>
+      <c r="Y21" s="21">
+        <f>L21*0.2+Q21*0.25+V21*0.25+W21*0.3+X21*0.1</f>
+        <v>6.8</v>
+      </c>
+      <c r="Z21" s="9"/>
     </row>
     <row r="22" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B22" s="48" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D22" s="50">
         <v>0</v>
@@ -2981,22 +2860,26 @@
       <c r="G22" s="50">
         <v>0</v>
       </c>
-      <c r="H22" s="68">
-        <v>0</v>
-      </c>
-      <c r="I22" s="51"/>
+      <c r="H22" s="62">
+        <v>0</v>
+      </c>
+      <c r="I22" s="51">
+        <v>0</v>
+      </c>
       <c r="J22" s="51"/>
-      <c r="K22" s="64">
+      <c r="K22" s="58">
         <v>0</v>
       </c>
       <c r="L22" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D22:J22)*50/(L$1-K22)</f>
         <v>0</v>
       </c>
       <c r="M22" s="53">
         <v>0</v>
       </c>
-      <c r="N22" s="54"/>
+      <c r="N22" s="54">
+        <v>0</v>
+      </c>
       <c r="O22" s="54"/>
       <c r="P22" s="54"/>
       <c r="Q22" s="52">
@@ -3006,7 +2889,9 @@
       <c r="R22" s="53">
         <v>0</v>
       </c>
-      <c r="S22" s="53"/>
+      <c r="S22" s="53">
+        <v>0</v>
+      </c>
       <c r="T22" s="53"/>
       <c r="U22" s="53"/>
       <c r="V22" s="52">
@@ -3022,13 +2907,13 @@
     </row>
     <row r="23" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D23" s="50">
         <v>0</v>
@@ -3042,22 +2927,26 @@
       <c r="G23" s="50">
         <v>0</v>
       </c>
-      <c r="H23" s="68">
-        <v>0</v>
-      </c>
-      <c r="I23" s="51"/>
+      <c r="H23" s="62">
+        <v>0</v>
+      </c>
+      <c r="I23" s="51">
+        <v>0</v>
+      </c>
       <c r="J23" s="51"/>
-      <c r="K23" s="64">
+      <c r="K23" s="58">
         <v>0</v>
       </c>
       <c r="L23" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D23:J23)*50/(L$1-K23)</f>
         <v>0</v>
       </c>
       <c r="M23" s="53">
         <v>0</v>
       </c>
-      <c r="N23" s="54"/>
+      <c r="N23" s="54">
+        <v>0</v>
+      </c>
       <c r="O23" s="54"/>
       <c r="P23" s="54"/>
       <c r="Q23" s="52">
@@ -3067,7 +2956,9 @@
       <c r="R23" s="53">
         <v>0</v>
       </c>
-      <c r="S23" s="53"/>
+      <c r="S23" s="53">
+        <v>0</v>
+      </c>
       <c r="T23" s="53"/>
       <c r="U23" s="53"/>
       <c r="V23" s="52">
@@ -3083,13 +2974,13 @@
     </row>
     <row r="24" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D24" s="50">
         <v>0</v>
@@ -3103,22 +2994,26 @@
       <c r="G24" s="50">
         <v>0</v>
       </c>
-      <c r="H24" s="68">
-        <v>0</v>
-      </c>
-      <c r="I24" s="51"/>
+      <c r="H24" s="62">
+        <v>0</v>
+      </c>
+      <c r="I24" s="51">
+        <v>0</v>
+      </c>
       <c r="J24" s="51"/>
-      <c r="K24" s="64">
+      <c r="K24" s="58">
         <v>0</v>
       </c>
       <c r="L24" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D24:J24)*50/(L$1-K24)</f>
         <v>0</v>
       </c>
       <c r="M24" s="53">
         <v>0</v>
       </c>
-      <c r="N24" s="54"/>
+      <c r="N24" s="54">
+        <v>0</v>
+      </c>
       <c r="O24" s="54"/>
       <c r="P24" s="54"/>
       <c r="Q24" s="52">
@@ -3128,7 +3023,9 @@
       <c r="R24" s="53">
         <v>0</v>
       </c>
-      <c r="S24" s="53"/>
+      <c r="S24" s="53">
+        <v>0</v>
+      </c>
       <c r="T24" s="53"/>
       <c r="U24" s="53"/>
       <c r="V24" s="52">
@@ -3144,13 +3041,13 @@
     </row>
     <row r="25" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B25" s="48" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D25" s="50">
         <v>0</v>
@@ -3164,22 +3061,26 @@
       <c r="G25" s="50">
         <v>0</v>
       </c>
-      <c r="H25" s="68">
-        <v>0</v>
-      </c>
-      <c r="I25" s="51"/>
+      <c r="H25" s="62">
+        <v>0</v>
+      </c>
+      <c r="I25" s="51">
+        <v>0</v>
+      </c>
       <c r="J25" s="51"/>
-      <c r="K25" s="64">
+      <c r="K25" s="58">
         <v>0</v>
       </c>
       <c r="L25" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D25:J25)*50/(L$1-K25)</f>
         <v>0</v>
       </c>
       <c r="M25" s="53">
         <v>0</v>
       </c>
-      <c r="N25" s="54"/>
+      <c r="N25" s="54">
+        <v>0</v>
+      </c>
       <c r="O25" s="54"/>
       <c r="P25" s="54"/>
       <c r="Q25" s="52">
@@ -3189,7 +3090,9 @@
       <c r="R25" s="53">
         <v>0</v>
       </c>
-      <c r="S25" s="53"/>
+      <c r="S25" s="53">
+        <v>0</v>
+      </c>
       <c r="T25" s="53"/>
       <c r="U25" s="53"/>
       <c r="V25" s="52">
@@ -3205,13 +3108,13 @@
     </row>
     <row r="26" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="47" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B26" s="48" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D26" s="50">
         <v>0</v>
@@ -3225,22 +3128,26 @@
       <c r="G26" s="50">
         <v>0</v>
       </c>
-      <c r="H26" s="68">
-        <v>0</v>
-      </c>
-      <c r="I26" s="51"/>
+      <c r="H26" s="62">
+        <v>0</v>
+      </c>
+      <c r="I26" s="51">
+        <v>0</v>
+      </c>
       <c r="J26" s="51"/>
-      <c r="K26" s="64">
+      <c r="K26" s="58">
         <v>0</v>
       </c>
       <c r="L26" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D26:J26)*50/(L$1-K26)</f>
         <v>0</v>
       </c>
       <c r="M26" s="53">
         <v>0</v>
       </c>
-      <c r="N26" s="54"/>
+      <c r="N26" s="54">
+        <v>0</v>
+      </c>
       <c r="O26" s="54"/>
       <c r="P26" s="54"/>
       <c r="Q26" s="52">
@@ -3250,7 +3157,9 @@
       <c r="R26" s="53">
         <v>0</v>
       </c>
-      <c r="S26" s="53"/>
+      <c r="S26" s="53">
+        <v>0</v>
+      </c>
       <c r="T26" s="53"/>
       <c r="U26" s="53"/>
       <c r="V26" s="52">
@@ -3264,15 +3173,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B27" s="48" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="D27" s="50">
         <v>0</v>
@@ -3286,22 +3195,26 @@
       <c r="G27" s="50">
         <v>0</v>
       </c>
-      <c r="H27" s="68">
-        <v>0</v>
-      </c>
-      <c r="I27" s="51"/>
+      <c r="H27" s="62">
+        <v>0</v>
+      </c>
+      <c r="I27" s="51">
+        <v>0</v>
+      </c>
       <c r="J27" s="51"/>
-      <c r="K27" s="64">
+      <c r="K27" s="58">
         <v>0</v>
       </c>
       <c r="L27" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D27:J27)*50/(L$1-K27)</f>
         <v>0</v>
       </c>
       <c r="M27" s="53">
         <v>0</v>
       </c>
-      <c r="N27" s="54"/>
+      <c r="N27" s="54">
+        <v>0</v>
+      </c>
       <c r="O27" s="54"/>
       <c r="P27" s="54"/>
       <c r="Q27" s="52">
@@ -3311,7 +3224,9 @@
       <c r="R27" s="53">
         <v>0</v>
       </c>
-      <c r="S27" s="53"/>
+      <c r="S27" s="53">
+        <v>0</v>
+      </c>
       <c r="T27" s="53"/>
       <c r="U27" s="53"/>
       <c r="V27" s="52">
@@ -3321,19 +3236,20 @@
       <c r="W27" s="54"/>
       <c r="X27" s="55"/>
       <c r="Y27" s="56">
-        <f>L27*0.2+Q27*0.25+V27*0.25+W27*0.3+X27*0.1</f>
-        <v>0</v>
-      </c>
+        <f>L27*0.2+Q27*0.25+V27*0.25+W27*0.3+X27*0.15</f>
+        <v>0</v>
+      </c>
+      <c r="Z27" s="57"/>
     </row>
     <row r="28" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="B28" s="48" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="D28" s="50">
         <v>0</v>
@@ -3347,22 +3263,26 @@
       <c r="G28" s="50">
         <v>0</v>
       </c>
-      <c r="H28" s="68">
-        <v>0</v>
-      </c>
-      <c r="I28" s="51"/>
+      <c r="H28" s="62">
+        <v>0</v>
+      </c>
+      <c r="I28" s="51">
+        <v>0</v>
+      </c>
       <c r="J28" s="51"/>
-      <c r="K28" s="64">
+      <c r="K28" s="58">
         <v>0</v>
       </c>
       <c r="L28" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D28:J28)*50/(L$1-K28)</f>
         <v>0</v>
       </c>
       <c r="M28" s="53">
         <v>0</v>
       </c>
-      <c r="N28" s="54"/>
+      <c r="N28" s="54">
+        <v>0</v>
+      </c>
       <c r="O28" s="54"/>
       <c r="P28" s="54"/>
       <c r="Q28" s="52">
@@ -3372,7 +3292,9 @@
       <c r="R28" s="53">
         <v>0</v>
       </c>
-      <c r="S28" s="53"/>
+      <c r="S28" s="53">
+        <v>0</v>
+      </c>
       <c r="T28" s="53"/>
       <c r="U28" s="53"/>
       <c r="V28" s="52">
@@ -3382,19 +3304,19 @@
       <c r="W28" s="54"/>
       <c r="X28" s="55"/>
       <c r="Y28" s="56">
-        <f>L28*0.2+Q28*0.25+V28*0.25+W28*0.3+X28*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" s="58" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f>L28*0.2+Q28*0.25+V28*0.25+W28*0.3+X28*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="B29" s="48" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="D29" s="50">
         <v>0</v>
@@ -3408,22 +3330,26 @@
       <c r="G29" s="50">
         <v>0</v>
       </c>
-      <c r="H29" s="68">
-        <v>0</v>
-      </c>
-      <c r="I29" s="51"/>
+      <c r="H29" s="62">
+        <v>0</v>
+      </c>
+      <c r="I29" s="51">
+        <v>0</v>
+      </c>
       <c r="J29" s="51"/>
-      <c r="K29" s="64">
+      <c r="K29" s="58">
         <v>0</v>
       </c>
       <c r="L29" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(D29:J29)*50/(L$1-K29)</f>
         <v>0</v>
       </c>
       <c r="M29" s="53">
         <v>0</v>
       </c>
-      <c r="N29" s="54"/>
+      <c r="N29" s="54">
+        <v>0</v>
+      </c>
       <c r="O29" s="54"/>
       <c r="P29" s="54"/>
       <c r="Q29" s="52">
@@ -3433,7 +3359,9 @@
       <c r="R29" s="53">
         <v>0</v>
       </c>
-      <c r="S29" s="53"/>
+      <c r="S29" s="53">
+        <v>0</v>
+      </c>
       <c r="T29" s="53"/>
       <c r="U29" s="53"/>
       <c r="V29" s="52">
@@ -3443,33 +3371,77 @@
       <c r="W29" s="54"/>
       <c r="X29" s="55"/>
       <c r="Y29" s="56">
-        <f>L29*0.2+Q29*0.25+V29*0.25+W29*0.3+X29*0.1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
+        <f>L29*0.2+Q29*0.25+V29*0.25+W29*0.3+X29*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="50">
+        <v>0</v>
+      </c>
+      <c r="E30" s="50">
+        <v>0</v>
+      </c>
+      <c r="F30" s="50">
+        <v>0</v>
+      </c>
+      <c r="G30" s="50">
+        <v>0</v>
+      </c>
+      <c r="H30" s="62">
+        <v>0</v>
+      </c>
+      <c r="I30" s="51">
+        <v>0</v>
+      </c>
+      <c r="J30" s="51"/>
+      <c r="K30" s="58">
+        <v>0</v>
+      </c>
+      <c r="L30" s="16">
+        <f>SUM(D30:J30)*50/(L$1-K30)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="53">
+        <v>0</v>
+      </c>
+      <c r="N30" s="54">
+        <v>0</v>
+      </c>
+      <c r="O30" s="54"/>
+      <c r="P30" s="54"/>
+      <c r="Q30" s="52">
+        <f>SUM(M30:P30)/Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="53">
+        <v>0</v>
+      </c>
+      <c r="S30" s="53">
+        <v>0</v>
+      </c>
+      <c r="T30" s="53"/>
+      <c r="U30" s="53"/>
+      <c r="V30" s="52">
+        <f>SUM(R30:U30)/V$1</f>
+        <v>0</v>
+      </c>
+      <c r="W30" s="54"/>
+      <c r="X30" s="55"/>
+      <c r="Y30" s="56">
+        <f>L30*0.2+Q30*0.25+V30*0.25+W30*0.3+X30*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="57"/>
     </row>
     <row r="31" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
@@ -3479,7 +3451,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="69"/>
+      <c r="H31" s="63"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3503,7 +3475,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="69"/>
+      <c r="H32" s="63"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3527,7 +3499,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="69"/>
+      <c r="H33" s="63"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3551,7 +3523,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="69"/>
+      <c r="H34" s="63"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3575,7 +3547,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="69"/>
+      <c r="H35" s="63"/>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3599,7 +3571,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="69"/>
+      <c r="H36" s="63"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -3623,7 +3595,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="69"/>
+      <c r="H37" s="63"/>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -3647,7 +3619,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="69"/>
+      <c r="H38" s="63"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -3671,7 +3643,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="69"/>
+      <c r="H39" s="63"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -3695,7 +3667,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="69"/>
+      <c r="H40" s="63"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
@@ -3719,7 +3691,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="69"/>
+      <c r="H41" s="63"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
@@ -3743,7 +3715,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="69"/>
+      <c r="H42" s="63"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -3767,7 +3739,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="69"/>
+      <c r="H43" s="63"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
@@ -3791,7 +3763,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="69"/>
+      <c r="H44" s="63"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -3815,7 +3787,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="69"/>
+      <c r="H45" s="63"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -3839,7 +3811,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="69"/>
+      <c r="H46" s="63"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -3863,7 +3835,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="69"/>
+      <c r="H47" s="63"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -3887,7 +3859,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="69"/>
+      <c r="H48" s="63"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -3911,7 +3883,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="69"/>
+      <c r="H49" s="63"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -3935,7 +3907,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="69"/>
+      <c r="H50" s="63"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
@@ -3959,7 +3931,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="69"/>
+      <c r="H51" s="63"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -3983,7 +3955,7 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
-      <c r="H52" s="69"/>
+      <c r="H52" s="63"/>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -4007,7 +3979,7 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="69"/>
+      <c r="H53" s="63"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -4031,7 +4003,7 @@
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
-      <c r="H54" s="69"/>
+      <c r="H54" s="63"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -4055,7 +4027,7 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
-      <c r="H55" s="69"/>
+      <c r="H55" s="63"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -4079,7 +4051,7 @@
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="69"/>
+      <c r="H56" s="63"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -4103,7 +4075,7 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="69"/>
+      <c r="H57" s="63"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -4127,7 +4099,7 @@
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
-      <c r="H58" s="69"/>
+      <c r="H58" s="63"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -4151,7 +4123,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="69"/>
+      <c r="H59" s="63"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -4175,7 +4147,7 @@
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="69"/>
+      <c r="H60" s="63"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -4199,7 +4171,7 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
-      <c r="H61" s="69"/>
+      <c r="H61" s="63"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -4223,7 +4195,7 @@
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
-      <c r="H62" s="69"/>
+      <c r="H62" s="63"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -4247,7 +4219,7 @@
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
-      <c r="H63" s="69"/>
+      <c r="H63" s="63"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -4271,7 +4243,7 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
-      <c r="H64" s="69"/>
+      <c r="H64" s="63"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -4295,7 +4267,7 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="69"/>
+      <c r="H65" s="63"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -4319,7 +4291,7 @@
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
-      <c r="H66" s="69"/>
+      <c r="H66" s="63"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -4343,7 +4315,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="69"/>
+      <c r="H67" s="63"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -4367,7 +4339,7 @@
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
-      <c r="H68" s="69"/>
+      <c r="H68" s="63"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -4391,7 +4363,7 @@
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
-      <c r="H69" s="69"/>
+      <c r="H69" s="63"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -4415,7 +4387,7 @@
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
-      <c r="H70" s="69"/>
+      <c r="H70" s="63"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -4439,7 +4411,7 @@
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
-      <c r="H71" s="69"/>
+      <c r="H71" s="63"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -4463,7 +4435,7 @@
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
-      <c r="H72" s="69"/>
+      <c r="H72" s="63"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -4487,7 +4459,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
-      <c r="H73" s="69"/>
+      <c r="H73" s="63"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -4511,7 +4483,7 @@
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
-      <c r="H74" s="69"/>
+      <c r="H74" s="63"/>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -4535,7 +4507,7 @@
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
-      <c r="H75" s="69"/>
+      <c r="H75" s="63"/>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -4551,6 +4523,30 @@
       <c r="U75" s="9"/>
       <c r="V75" s="9"/>
     </row>
+    <row r="76" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="63"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
+      <c r="O76" s="9"/>
+      <c r="P76" s="9"/>
+      <c r="Q76" s="9"/>
+      <c r="R76" s="9"/>
+      <c r="S76" s="9"/>
+      <c r="T76" s="9"/>
+      <c r="U76" s="9"/>
+      <c r="V76" s="9"/>
+    </row>
   </sheetData>
   <sortState ref="A3:Z30">
     <sortCondition descending="1" ref="Y3"/>
@@ -4560,53 +4556,53 @@
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="R1:U1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:J29">
-    <cfRule type="cellIs" dxfId="32" priority="19" operator="between">
+  <conditionalFormatting sqref="D3:J30">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W3:X29 M3:P29">
-    <cfRule type="cellIs" dxfId="29" priority="10" operator="between">
+  <conditionalFormatting sqref="W3:X30 M3:P30">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:U29">
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="between">
+  <conditionalFormatting sqref="R3:U30">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="between">
       <formula>80</formula>
       <formula>200</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L29">
+  <conditionalFormatting sqref="L3:L30">
     <cfRule type="dataBar" priority="189">
       <dataBar>
         <cfvo type="min"/>
@@ -4620,7 +4616,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q29">
+  <conditionalFormatting sqref="Q3:Q30">
     <cfRule type="dataBar" priority="190">
       <dataBar>
         <cfvo type="min"/>
@@ -4634,7 +4630,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V29">
+  <conditionalFormatting sqref="V3:V30">
     <cfRule type="dataBar" priority="191">
       <dataBar>
         <cfvo type="min"/>
@@ -4648,7 +4644,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y29">
+  <conditionalFormatting sqref="Y3:Y30">
     <cfRule type="dataBar" priority="192">
       <dataBar>
         <cfvo type="min"/>
@@ -4677,7 +4673,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L3:L29</xm:sqref>
+          <xm:sqref>L3:L30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C1E54EB9-FD52-4CFD-8B29-7F3B7B6681D5}">
@@ -4688,7 +4684,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Q3:Q29</xm:sqref>
+          <xm:sqref>Q3:Q30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{03C5F189-3F43-4B84-A0F5-49F108E9F2B6}">
@@ -4699,7 +4695,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V3:V29</xm:sqref>
+          <xm:sqref>V3:V30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{43DC70F4-8291-4430-AFF0-577FC5E79CD9}">
@@ -4710,7 +4706,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Y3:Y29</xm:sqref>
+          <xm:sqref>Y3:Y30</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4755,22 +4751,22 @@
       <c r="B1" s="18"/>
       <c r="C1" s="34"/>
       <c r="D1" s="40"/>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="61" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="63"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="69"/>
       <c r="Q1" s="33" t="s">
         <v>45</v>
       </c>
@@ -6356,14 +6352,14 @@
     <mergeCell ref="K1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:I33">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="25" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6410,18 +6406,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:O33">
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="18" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="19" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
@@ -6469,18 +6465,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q33">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
       <formula>80</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ileri java hafta 7
</commit_message>
<xml_diff>
--- a/AdvancedJava/_docs/Notlar.xlsx
+++ b/AdvancedJava/_docs/Notlar.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="100">
   <si>
     <t>Adı</t>
   </si>
@@ -187,9 +187,6 @@
     <t>DEVAM DURUMU (%20)</t>
   </si>
   <si>
-    <t>ÖDEVLER (%25)</t>
-  </si>
-  <si>
     <t>FİNAL</t>
   </si>
   <si>
@@ -368,6 +365,9 @@
   </si>
   <si>
     <t>H5150063</t>
+  </si>
+  <si>
+    <t>ÖDEV (%25)</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,14 +418,20 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color theme="2" tint="-0.249977111117893"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -773,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -865,17 +871,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -884,15 +880,34 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1406,11 +1421,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z76"/>
+  <dimension ref="A1:X76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC14" sqref="AC14"/>
+      <selection pane="bottomLeft" activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1420,7 +1435,7 @@
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.44140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.44140625" style="53" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.44140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -1430,61 +1445,58 @@
     <col min="16" max="16" width="2.5546875" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.77734375" style="1" customWidth="1"/>
     <col min="18" max="18" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="2.77734375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5" style="1" customWidth="1"/>
-    <col min="23" max="23" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7" style="1" customWidth="1"/>
-    <col min="25" max="25" width="5.77734375" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.88671875" style="1"/>
+    <col min="19" max="19" width="2.77734375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7" style="1" customWidth="1"/>
+    <col min="23" max="23" width="5.77734375" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="18"/>
       <c r="C1" s="29"/>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
       <c r="L1" s="46">
-        <v>5</v>
-      </c>
-      <c r="M1" s="67" t="s">
-        <v>95</v>
-      </c>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
+        <v>6</v>
+      </c>
+      <c r="M1" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
       <c r="Q1" s="45">
-        <v>2</v>
-      </c>
-      <c r="R1" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="45">
-        <v>2</v>
-      </c>
-      <c r="W1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="S1" s="73"/>
+      <c r="T1" s="45">
+        <v>2</v>
+      </c>
+      <c r="U1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y1" s="19" t="s">
+      <c r="V1" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>29</v>
       </c>
@@ -1506,7 +1518,7 @@
       <c r="G2" s="27">
         <v>4</v>
       </c>
-      <c r="H2" s="60">
+      <c r="H2" s="50">
         <v>5</v>
       </c>
       <c r="I2" s="27">
@@ -1516,7 +1528,7 @@
         <v>7</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L2" s="28" t="s">
         <v>30</v>
@@ -1528,10 +1540,10 @@
         <v>5</v>
       </c>
       <c r="O2" s="27">
-        <v>6</v>
-      </c>
-      <c r="P2" s="27">
         <v>7</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="Q2" s="28" t="s">
         <v>30</v>
@@ -1542,35 +1554,29 @@
       <c r="S2" s="37">
         <v>2</v>
       </c>
-      <c r="T2" s="37">
-        <v>3</v>
-      </c>
-      <c r="U2" s="27">
-        <v>4</v>
-      </c>
-      <c r="V2" s="28" t="s">
+      <c r="T2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="26" t="s">
+      <c r="U2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y2" s="19" t="s">
+      <c r="V2" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>48</v>
-      </c>
       <c r="D3" s="12">
         <v>2</v>
       </c>
@@ -1583,19 +1589,21 @@
       <c r="G3" s="7">
         <v>2</v>
       </c>
-      <c r="H3" s="61">
+      <c r="H3" s="51">
         <v>2</v>
       </c>
       <c r="I3" s="7">
         <v>2</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="58">
+      <c r="J3" s="7">
+        <v>2</v>
+      </c>
+      <c r="K3" s="48">
         <v>0</v>
       </c>
       <c r="L3" s="16">
         <f>SUM(D3:J3)*50/(L$1-K3)</f>
-        <v>120</v>
+        <v>116.66666666666667</v>
       </c>
       <c r="M3" s="14">
         <v>100</v>
@@ -1603,10 +1611,14 @@
       <c r="N3" s="6">
         <v>100</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="O3" s="6">
+        <v>100</v>
+      </c>
+      <c r="P3" s="48">
+        <v>0</v>
+      </c>
       <c r="Q3" s="16">
-        <f>SUM(M3:P3)/Q$1</f>
+        <f>SUM(M3:O3)/(Q$1-P3)</f>
         <v>100</v>
       </c>
       <c r="R3" s="14">
@@ -1615,28 +1627,26 @@
       <c r="S3" s="14">
         <v>60</v>
       </c>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="16">
-        <f>SUM(R3:U3)/V$1</f>
+      <c r="T3" s="16">
+        <f>SUM(R3:S3)/T$1</f>
         <v>60</v>
       </c>
-      <c r="W3" s="6"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="21">
-        <f>L3*0.2+Q3*0.25+V3*0.25+W3*0.3+X3*0.15</f>
-        <v>64</v>
-      </c>
-      <c r="Z3" s="1" t="s">
+      <c r="U3" s="6"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="21">
+        <f>L3*0.2+Q3*0.25+T3*0.25+U3*0.3+V3*0.15</f>
+        <v>63.333333333333336</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>6</v>
@@ -1653,19 +1663,21 @@
       <c r="G4" s="7">
         <v>2</v>
       </c>
-      <c r="H4" s="61">
+      <c r="H4" s="51">
         <v>2</v>
       </c>
       <c r="I4" s="7">
         <v>2</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="58">
+      <c r="J4" s="7">
+        <v>2</v>
+      </c>
+      <c r="K4" s="48">
         <v>0</v>
       </c>
       <c r="L4" s="16">
         <f>SUM(D4:J4)*50/(L$1-K4)</f>
-        <v>120</v>
+        <v>116.66666666666667</v>
       </c>
       <c r="M4" s="14">
         <v>95</v>
@@ -1673,11 +1685,15 @@
       <c r="N4" s="6">
         <v>100</v>
       </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
+      <c r="O4" s="6">
+        <v>90</v>
+      </c>
+      <c r="P4" s="48">
+        <v>0</v>
+      </c>
       <c r="Q4" s="16">
-        <f>SUM(M4:P4)/Q$1</f>
-        <v>97.5</v>
+        <f>SUM(M4:O4)/(Q$1-P4)</f>
+        <v>95</v>
       </c>
       <c r="R4" s="14">
         <v>60</v>
@@ -1685,31 +1701,29 @@
       <c r="S4" s="14">
         <v>60</v>
       </c>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="16">
-        <f>SUM(R4:U4)/V$1</f>
+      <c r="T4" s="16">
+        <f>SUM(R4:S4)/T$1</f>
         <v>60</v>
       </c>
-      <c r="W4" s="6"/>
-      <c r="X4" s="44"/>
-      <c r="Y4" s="21">
-        <f>L4*0.2+Q4*0.25+V4*0.25+W4*0.3+X4*0.15</f>
-        <v>63.375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U4" s="6"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="21">
+        <f>L4*0.2+Q4*0.25+T4*0.25+U4*0.3+V4*0.15</f>
+        <v>62.083333333333336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D5" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="7">
         <v>2</v>
@@ -1720,31 +1734,37 @@
       <c r="G5" s="7">
         <v>2</v>
       </c>
-      <c r="H5" s="61">
+      <c r="H5" s="51">
         <v>2</v>
       </c>
       <c r="I5" s="7">
         <v>2</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="58">
+      <c r="J5" s="7">
+        <v>2</v>
+      </c>
+      <c r="K5" s="48">
         <v>0</v>
       </c>
       <c r="L5" s="16">
         <f>SUM(D5:J5)*50/(L$1-K5)</f>
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="M5" s="14">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="N5" s="6">
+        <v>100</v>
+      </c>
+      <c r="O5" s="6">
         <v>90</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="P5" s="48">
+        <v>0</v>
+      </c>
       <c r="Q5" s="16">
-        <f>SUM(M5:P5)/Q$1</f>
-        <v>85</v>
+        <f>SUM(M5:O5)/(Q$1-P5)</f>
+        <v>95</v>
       </c>
       <c r="R5" s="14">
         <v>60</v>
@@ -1752,28 +1772,26 @@
       <c r="S5" s="14">
         <v>60</v>
       </c>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="16">
-        <f>SUM(R5:U5)/V$1</f>
+      <c r="T5" s="16">
+        <f>SUM(R5:S5)/T$1</f>
         <v>60</v>
       </c>
-      <c r="W5" s="6"/>
-      <c r="X5" s="44"/>
-      <c r="Y5" s="21">
-        <f>L5*0.2+Q5*0.25+V5*0.25+W5*0.3+X5*0.15</f>
-        <v>60.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="6"/>
+      <c r="V5" s="44"/>
+      <c r="W5" s="21">
+        <f>L5*0.2+Q5*0.25+T5*0.25+U5*0.3+V5*0.15</f>
+        <v>58.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="D6" s="12">
         <v>0</v>
@@ -1787,14 +1805,16 @@
       <c r="G6" s="7">
         <v>2</v>
       </c>
-      <c r="H6" s="61">
+      <c r="H6" s="51">
         <v>2</v>
       </c>
       <c r="I6" s="7">
         <v>2</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="58">
+      <c r="J6" s="7">
+        <v>2</v>
+      </c>
+      <c r="K6" s="48">
         <v>0</v>
       </c>
       <c r="L6" s="16">
@@ -1802,16 +1822,20 @@
         <v>100</v>
       </c>
       <c r="M6" s="14">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="N6" s="6">
-        <v>100</v>
-      </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="O6" s="6">
+        <v>90</v>
+      </c>
+      <c r="P6" s="48">
+        <v>0</v>
+      </c>
       <c r="Q6" s="16">
-        <f>SUM(M6:P6)/Q$1</f>
-        <v>97.5</v>
+        <f>SUM(M6:O6)/(Q$1-P6)</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="R6" s="14">
         <v>60</v>
@@ -1819,28 +1843,26 @@
       <c r="S6" s="14">
         <v>60</v>
       </c>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="16">
-        <f>SUM(R6:U6)/V$1</f>
+      <c r="T6" s="16">
+        <f>SUM(R6:S6)/T$1</f>
         <v>60</v>
       </c>
-      <c r="W6" s="6"/>
-      <c r="X6" s="44"/>
-      <c r="Y6" s="21">
-        <f>L6*0.2+Q6*0.25+V6*0.25+W6*0.3+X6*0.15</f>
-        <v>59.375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U6" s="6"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="21">
+        <f>L6*0.2+Q6*0.25+T6*0.25+U6*0.3+V6*0.1</f>
+        <v>58.333333333333329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D7" s="12">
         <v>0</v>
@@ -1854,31 +1876,37 @@
       <c r="G7" s="7">
         <v>2</v>
       </c>
-      <c r="H7" s="61" t="s">
-        <v>96</v>
+      <c r="H7" s="51">
+        <v>2</v>
       </c>
       <c r="I7" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="59">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J7" s="7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="48">
+        <v>0</v>
       </c>
       <c r="L7" s="16">
         <f>SUM(D7:J7)*50/(L$1-K7)</f>
-        <v>97.5</v>
+        <v>100</v>
       </c>
       <c r="M7" s="14">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N7" s="6">
         <v>100</v>
       </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
+      <c r="O7" s="6">
+        <v>90</v>
+      </c>
+      <c r="P7" s="48">
+        <v>0</v>
+      </c>
       <c r="Q7" s="16">
-        <f>SUM(M7:P7)/Q$1</f>
-        <v>97.5</v>
+        <f>SUM(M7:O7)/(Q$1-P7)</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="R7" s="14">
         <v>60</v>
@@ -1886,28 +1914,26 @@
       <c r="S7" s="14">
         <v>60</v>
       </c>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="16">
-        <f>SUM(R7:U7)/V$1</f>
+      <c r="T7" s="16">
+        <f>SUM(R7:S7)/T$1</f>
         <v>60</v>
       </c>
-      <c r="W7" s="6"/>
-      <c r="X7" s="44"/>
-      <c r="Y7" s="21">
-        <f>L7*0.2+Q7*0.25+V7*0.25+W7*0.3+X7*0.15</f>
-        <v>58.875</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U7" s="6"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="21">
+        <f>L7*0.2+Q7*0.25+T7*0.25+U7*0.3+V7*0.15</f>
+        <v>58.333333333333329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D8" s="12">
         <v>0</v>
@@ -1921,31 +1947,37 @@
       <c r="G8" s="7">
         <v>2</v>
       </c>
-      <c r="H8" s="61">
-        <v>2</v>
+      <c r="H8" s="51" t="s">
+        <v>95</v>
       </c>
       <c r="I8" s="7">
-        <v>2</v>
-      </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="58">
-        <v>0</v>
+        <v>1.8</v>
+      </c>
+      <c r="J8" s="7">
+        <v>2</v>
+      </c>
+      <c r="K8" s="49">
+        <v>1</v>
       </c>
       <c r="L8" s="16">
         <f>SUM(D8:J8)*50/(L$1-K8)</f>
+        <v>98.000000000000014</v>
+      </c>
+      <c r="M8" s="14">
+        <v>95</v>
+      </c>
+      <c r="N8" s="6">
         <v>100</v>
       </c>
-      <c r="M8" s="14">
-        <v>100</v>
-      </c>
-      <c r="N8" s="6">
-        <v>90</v>
-      </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
+      <c r="O8" s="6">
+        <v>80</v>
+      </c>
+      <c r="P8" s="48">
+        <v>0</v>
+      </c>
       <c r="Q8" s="16">
-        <f>SUM(M8:P8)/Q$1</f>
-        <v>95</v>
+        <f>SUM(M8:O8)/(Q$1-P8)</f>
+        <v>91.666666666666671</v>
       </c>
       <c r="R8" s="14">
         <v>60</v>
@@ -1953,31 +1985,29 @@
       <c r="S8" s="14">
         <v>60</v>
       </c>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="16">
-        <f>SUM(R8:U8)/V$1</f>
+      <c r="T8" s="16">
+        <f>SUM(R8:S8)/T$1</f>
         <v>60</v>
       </c>
-      <c r="W8" s="6"/>
-      <c r="X8" s="44"/>
-      <c r="Y8" s="21">
-        <f>L8*0.2+Q8*0.25+V8*0.25+W8*0.3+X8*0.1</f>
-        <v>58.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="6"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="21">
+        <f>L8*0.2+Q8*0.25+T8*0.25+U8*0.3+V8*0.15</f>
+        <v>57.516666666666673</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D9" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="7">
         <v>2</v>
@@ -1988,31 +2018,37 @@
       <c r="G9" s="7">
         <v>2</v>
       </c>
-      <c r="H9" s="61">
+      <c r="H9" s="51">
         <v>2</v>
       </c>
       <c r="I9" s="7">
         <v>2</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="58">
+      <c r="J9" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="K9" s="48">
         <v>0</v>
       </c>
       <c r="L9" s="16">
         <f>SUM(D9:J9)*50/(L$1-K9)</f>
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="M9" s="14">
+        <v>80</v>
+      </c>
+      <c r="N9" s="6">
         <v>90</v>
       </c>
-      <c r="N9" s="6">
-        <v>100</v>
-      </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="O9" s="6">
+        <v>60</v>
+      </c>
+      <c r="P9" s="48">
+        <v>0</v>
+      </c>
       <c r="Q9" s="16">
-        <f>SUM(M9:P9)/Q$1</f>
-        <v>95</v>
+        <f>SUM(M9:O9)/(Q$1-P9)</f>
+        <v>76.666666666666671</v>
       </c>
       <c r="R9" s="14">
         <v>60</v>
@@ -2020,31 +2056,29 @@
       <c r="S9" s="14">
         <v>60</v>
       </c>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="16">
-        <f>SUM(R9:U9)/V$1</f>
+      <c r="T9" s="16">
+        <f>SUM(R9:S9)/T$1</f>
         <v>60</v>
       </c>
-      <c r="W9" s="6"/>
-      <c r="X9" s="44"/>
-      <c r="Y9" s="21">
-        <f>L9*0.2+Q9*0.25+V9*0.25+W9*0.3+X9*0.15</f>
-        <v>58.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U9" s="6"/>
+      <c r="V9" s="44"/>
+      <c r="W9" s="21">
+        <f>L9*0.2+Q9*0.25+T9*0.25+U9*0.3+V9*0.15</f>
+        <v>57.166666666666671</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="D10" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="7">
         <v>2</v>
@@ -2053,62 +2087,66 @@
         <v>2</v>
       </c>
       <c r="G10" s="7">
-        <v>2</v>
-      </c>
-      <c r="H10" s="61">
+        <v>1.8</v>
+      </c>
+      <c r="H10" s="51">
         <v>2</v>
       </c>
       <c r="I10" s="7">
         <v>2</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="58">
+      <c r="J10" s="7">
+        <v>2</v>
+      </c>
+      <c r="K10" s="48">
         <v>0</v>
       </c>
       <c r="L10" s="16">
         <f>SUM(D10:J10)*50/(L$1-K10)</f>
-        <v>120</v>
+        <v>98.333333333333329</v>
       </c>
       <c r="M10" s="14">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="N10" s="6">
-        <v>90</v>
-      </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="O10" s="6">
+        <v>70</v>
+      </c>
+      <c r="P10" s="48">
+        <v>0</v>
+      </c>
       <c r="Q10" s="16">
-        <f>SUM(M10:P10)/Q$1</f>
-        <v>87.5</v>
+        <f>SUM(M10:O10)/(Q$1-P10)</f>
+        <v>86.666666666666671</v>
       </c>
       <c r="R10" s="14">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="S10" s="14">
         <v>60</v>
       </c>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="16">
-        <f>SUM(R10:U10)/V$1</f>
-        <v>50</v>
-      </c>
-      <c r="W10" s="6"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="21">
-        <f>L10*0.2+Q10*0.25+V10*0.25+W10*0.3+X10*0.15</f>
-        <v>58.375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T10" s="16">
+        <f>SUM(R10:S10)/T$1</f>
+        <v>60</v>
+      </c>
+      <c r="U10" s="6"/>
+      <c r="V10" s="44"/>
+      <c r="W10" s="21">
+        <f>L10*0.2+Q10*0.25+T10*0.25+U10*0.3+V10*0.15</f>
+        <v>56.333333333333336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D11" s="12">
         <v>0</v>
@@ -2120,33 +2158,39 @@
         <v>2</v>
       </c>
       <c r="G11" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="H11" s="61">
+        <v>2</v>
+      </c>
+      <c r="H11" s="51">
         <v>2</v>
       </c>
       <c r="I11" s="7">
         <v>2</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="58">
+      <c r="J11" s="7">
+        <v>2</v>
+      </c>
+      <c r="K11" s="48">
         <v>0</v>
       </c>
       <c r="L11" s="16">
         <f>SUM(D11:J11)*50/(L$1-K11)</f>
-        <v>98.000000000000014</v>
+        <v>100</v>
       </c>
       <c r="M11" s="14">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N11" s="6">
-        <v>95</v>
-      </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="O11" s="6">
+        <v>80</v>
+      </c>
+      <c r="P11" s="48">
+        <v>0</v>
+      </c>
       <c r="Q11" s="16">
-        <f>SUM(M11:P11)/Q$1</f>
-        <v>95</v>
+        <f>SUM(M11:O11)/(Q$1-P11)</f>
+        <v>83.333333333333329</v>
       </c>
       <c r="R11" s="14">
         <v>60</v>
@@ -2154,28 +2198,26 @@
       <c r="S11" s="14">
         <v>60</v>
       </c>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="16">
-        <f>SUM(R11:U11)/V$1</f>
+      <c r="T11" s="16">
+        <f>SUM(R11:S11)/T$1</f>
         <v>60</v>
       </c>
-      <c r="W11" s="6"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="21">
-        <f>L11*0.2+Q11*0.25+V11*0.25+W11*0.3+X11*0.15</f>
-        <v>58.350000000000009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="6"/>
+      <c r="V11" s="44"/>
+      <c r="W11" s="21">
+        <f>L11*0.2+Q11*0.25+T11*0.25+U11*0.3+V11*0.15</f>
+        <v>55.833333333333329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="D12" s="12">
         <v>0</v>
@@ -2189,63 +2231,67 @@
       <c r="G12" s="7">
         <v>2</v>
       </c>
-      <c r="H12" s="61">
-        <v>1.7</v>
+      <c r="H12" s="51">
+        <v>2</v>
       </c>
       <c r="I12" s="7">
         <v>2</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="58">
+      <c r="J12" s="7">
+        <v>2</v>
+      </c>
+      <c r="K12" s="48">
         <v>0</v>
       </c>
       <c r="L12" s="16">
         <f>SUM(D12:J12)*50/(L$1-K12)</f>
-        <v>96.999999999999986</v>
+        <v>100</v>
       </c>
       <c r="M12" s="14">
         <v>90</v>
       </c>
       <c r="N12" s="6">
-        <v>85</v>
-      </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="O12" s="6">
+        <v>80</v>
+      </c>
+      <c r="P12" s="48">
+        <v>0</v>
+      </c>
       <c r="Q12" s="16">
-        <f>SUM(M12:P12)/Q$1</f>
-        <v>87.5</v>
+        <f>SUM(M12:O12)/(Q$1-P12)</f>
+        <v>90</v>
       </c>
       <c r="R12" s="14">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="S12" s="14">
         <v>60</v>
       </c>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="16">
-        <f>SUM(R12:U12)/V$1</f>
-        <v>60</v>
-      </c>
-      <c r="W12" s="6"/>
-      <c r="X12" s="44"/>
-      <c r="Y12" s="21">
-        <f>L12*0.2+Q12*0.25+V12*0.25+W12*0.3+X12*0.15</f>
-        <v>56.274999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T12" s="16">
+        <f>SUM(R12:S12)/T$1</f>
+        <v>50</v>
+      </c>
+      <c r="U12" s="6"/>
+      <c r="V12" s="44"/>
+      <c r="W12" s="21">
+        <f>L12*0.2+Q12*0.25+T12*0.25+U12*0.3+V12*0.15</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D13" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
@@ -2256,60 +2302,64 @@
       <c r="G13" s="7">
         <v>2</v>
       </c>
-      <c r="H13" s="61">
+      <c r="H13" s="51">
         <v>2</v>
       </c>
       <c r="I13" s="7">
         <v>2</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="58">
+      <c r="J13" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="K13" s="48">
         <v>0</v>
       </c>
       <c r="L13" s="16">
         <f>SUM(D13:J13)*50/(L$1-K13)</f>
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="M13" s="14">
+        <v>85</v>
+      </c>
+      <c r="N13" s="6">
         <v>90</v>
       </c>
-      <c r="N13" s="6">
-        <v>80</v>
-      </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="O13" s="6">
+        <v>50</v>
+      </c>
+      <c r="P13" s="48">
+        <v>0</v>
+      </c>
       <c r="Q13" s="16">
-        <f>SUM(M13:P13)/Q$1</f>
-        <v>85</v>
+        <f>SUM(M13:O13)/(Q$1-P13)</f>
+        <v>75</v>
       </c>
       <c r="R13" s="14">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="S13" s="14">
         <v>60</v>
       </c>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="16">
-        <f>SUM(R13:U13)/V$1</f>
-        <v>60</v>
-      </c>
-      <c r="W13" s="6"/>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="21">
-        <f>L13*0.2+Q13*0.25+V13*0.25+W13*0.3+X13*0.15</f>
-        <v>56.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T13" s="16">
+        <f>SUM(R13:S13)/T$1</f>
+        <v>50</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="21">
+        <f>L13*0.2+Q13*0.25+T13*0.25+U13*0.3+V13*0.15</f>
+        <v>54.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="D14" s="12">
         <v>0</v>
@@ -2323,61 +2373,65 @@
       <c r="G14" s="7">
         <v>2</v>
       </c>
-      <c r="H14" s="61">
-        <v>2</v>
+      <c r="H14" s="51">
+        <v>1.7</v>
       </c>
       <c r="I14" s="7">
         <v>2</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="58">
+      <c r="J14" s="7">
+        <v>2</v>
+      </c>
+      <c r="K14" s="48">
         <v>0</v>
       </c>
       <c r="L14" s="16">
         <f>SUM(D14:J14)*50/(L$1-K14)</f>
-        <v>100</v>
+        <v>97.5</v>
       </c>
       <c r="M14" s="14">
         <v>90</v>
       </c>
       <c r="N14" s="6">
-        <v>100</v>
-      </c>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
+        <v>85</v>
+      </c>
+      <c r="O14" s="6">
+        <v>50</v>
+      </c>
+      <c r="P14" s="48">
+        <v>0</v>
+      </c>
       <c r="Q14" s="16">
-        <f>SUM(M14:P14)/Q$1</f>
-        <v>95</v>
+        <f>SUM(M14:O14)/(Q$1-P14)</f>
+        <v>75</v>
       </c>
       <c r="R14" s="14">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="S14" s="14">
         <v>60</v>
       </c>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="16">
-        <f>SUM(R14:U14)/V$1</f>
-        <v>50</v>
-      </c>
-      <c r="W14" s="6"/>
-      <c r="X14" s="44"/>
-      <c r="Y14" s="21">
-        <f>L14*0.2+Q14*0.25+V14*0.25+W14*0.3+X14*0.15</f>
-        <v>56.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T14" s="16">
+        <f>SUM(R14:S14)/T$1</f>
+        <v>60</v>
+      </c>
+      <c r="U14" s="6"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="21">
+        <f>L14*0.2+Q14*0.25+T14*0.25+U14*0.3+V14*0.15</f>
+        <v>53.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>67</v>
-      </c>
       <c r="D15" s="12">
         <v>0</v>
       </c>
@@ -2390,19 +2444,21 @@
       <c r="G15" s="7">
         <v>2</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="51">
         <v>2</v>
       </c>
       <c r="I15" s="7">
         <v>1.8</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="58">
+      <c r="J15" s="7">
+        <v>2</v>
+      </c>
+      <c r="K15" s="48">
         <v>0</v>
       </c>
       <c r="L15" s="16">
         <f>SUM(D15:J15)*50/(L$1-K15)</f>
-        <v>78</v>
+        <v>81.666666666666671</v>
       </c>
       <c r="M15" s="14">
         <v>90</v>
@@ -2410,11 +2466,15 @@
       <c r="N15" s="6">
         <v>100</v>
       </c>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
+      <c r="O15" s="6">
+        <v>90</v>
+      </c>
+      <c r="P15" s="48">
+        <v>0</v>
+      </c>
       <c r="Q15" s="16">
-        <f>SUM(M15:P15)/Q$1</f>
-        <v>95</v>
+        <f>SUM(M15:O15)/(Q$1-P15)</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="R15" s="14">
         <v>40</v>
@@ -2422,29 +2482,27 @@
       <c r="S15" s="14">
         <v>60</v>
       </c>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="16">
-        <f>SUM(R15:U15)/V$1</f>
+      <c r="T15" s="16">
+        <f>SUM(R15:S15)/T$1</f>
         <v>50</v>
       </c>
-      <c r="W15" s="6"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="21">
-        <f>L15*0.2+Q15*0.25+V15*0.25+W15*0.3+X15*0.15</f>
-        <v>51.85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="6"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="21">
+        <f>L15*0.2+Q15*0.25+T15*0.25+U15*0.3+V15*0.15</f>
+        <v>52.166666666666671</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="D16" s="12">
         <v>2</v>
       </c>
@@ -2457,19 +2515,21 @@
       <c r="G16" s="7">
         <v>0</v>
       </c>
-      <c r="H16" s="61">
+      <c r="H16" s="51">
         <v>2</v>
       </c>
       <c r="I16" s="7">
         <v>2</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="58">
+      <c r="J16" s="7">
+        <v>0</v>
+      </c>
+      <c r="K16" s="48">
         <v>0</v>
       </c>
       <c r="L16" s="16">
         <f>SUM(D16:J16)*50/(L$1-K16)</f>
-        <v>100</v>
+        <v>83.333333333333329</v>
       </c>
       <c r="M16" s="14">
         <v>0</v>
@@ -2477,11 +2537,15 @@
       <c r="N16" s="6">
         <v>100</v>
       </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="48">
+        <v>0</v>
+      </c>
       <c r="Q16" s="16">
-        <f>SUM(M16:P16)/Q$1</f>
-        <v>50</v>
+        <f>SUM(M16:O16)/(Q$1-P16)</f>
+        <v>33.333333333333336</v>
       </c>
       <c r="R16" s="14">
         <v>60</v>
@@ -2489,20 +2553,18 @@
       <c r="S16" s="14">
         <v>60</v>
       </c>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="16">
-        <f>SUM(R16:U16)/V$1</f>
+      <c r="T16" s="16">
+        <f>SUM(R16:S16)/T$1</f>
         <v>60</v>
       </c>
-      <c r="W16" s="6"/>
-      <c r="X16" s="44"/>
-      <c r="Y16" s="21">
-        <f>L16*0.2+Q16*0.25+V16*0.25+W16*0.3+X16*0.15</f>
-        <v>47.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U16" s="6"/>
+      <c r="V16" s="44"/>
+      <c r="W16" s="21">
+        <f>L16*0.2+Q16*0.25+T16*0.25+U16*0.3+V16*0.15</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>17</v>
       </c>
@@ -2524,19 +2586,21 @@
       <c r="G17" s="7">
         <v>2</v>
       </c>
-      <c r="H17" s="61">
+      <c r="H17" s="51">
         <v>0</v>
       </c>
       <c r="I17" s="7">
         <v>2</v>
       </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="58">
+      <c r="J17" s="7">
+        <v>0</v>
+      </c>
+      <c r="K17" s="48">
         <v>0</v>
       </c>
       <c r="L17" s="16">
         <f>SUM(D17:J17)*50/(L$1-K17)</f>
-        <v>80</v>
+        <v>66.666666666666671</v>
       </c>
       <c r="M17" s="14">
         <v>85</v>
@@ -2544,11 +2608,15 @@
       <c r="N17" s="6">
         <v>95</v>
       </c>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="O17" s="6">
+        <v>0</v>
+      </c>
+      <c r="P17" s="48">
+        <v>0</v>
+      </c>
       <c r="Q17" s="16">
-        <f>SUM(M17:P17)/Q$1</f>
-        <v>90</v>
+        <f>SUM(M17:O17)/(Q$1-P17)</f>
+        <v>60</v>
       </c>
       <c r="R17" s="14">
         <v>40</v>
@@ -2556,96 +2624,98 @@
       <c r="S17" s="14">
         <v>0</v>
       </c>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="16">
-        <f>SUM(R17:U17)/V$1</f>
+      <c r="T17" s="16">
+        <f>SUM(R17:S17)/T$1</f>
         <v>20</v>
       </c>
-      <c r="W17" s="6"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="21">
-        <f>L17*0.2+Q17*0.25+V17*0.25+W17*0.3+X17*0.15</f>
-        <v>43.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="6"/>
+      <c r="V17" s="44"/>
+      <c r="W17" s="21">
+        <f>L17*0.2+Q17*0.25+T17*0.25+U17*0.3+V17*0.15</f>
+        <v>33.333333333333336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" s="47" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="D18" s="12">
         <v>0</v>
       </c>
-      <c r="E18" s="12">
-        <v>0</v>
-      </c>
-      <c r="F18" s="12">
-        <v>0</v>
-      </c>
-      <c r="G18" s="12">
-        <v>0</v>
-      </c>
-      <c r="H18" s="61">
-        <v>2</v>
+      <c r="E18" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="51">
+        <v>0</v>
       </c>
       <c r="I18" s="7">
-        <v>0</v>
-      </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="58">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J18" s="7">
+        <v>2</v>
+      </c>
+      <c r="K18" s="48">
+        <v>3</v>
       </c>
       <c r="L18" s="16">
         <f>SUM(D18:J18)*50/(L$1-K18)</f>
-        <v>20</v>
-      </c>
-      <c r="M18" s="14">
-        <v>0</v>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="M18" s="55" t="s">
+        <v>95</v>
       </c>
       <c r="N18" s="6">
-        <v>0</v>
-      </c>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="O18" s="6">
+        <v>50</v>
+      </c>
+      <c r="P18" s="48">
+        <v>1</v>
+      </c>
       <c r="Q18" s="16">
-        <f>SUM(M18:P18)/Q$1</f>
-        <v>0</v>
+        <f>SUM(M18:O18)/(Q$1-P18)</f>
+        <v>62.5</v>
       </c>
       <c r="R18" s="14">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="S18" s="14">
+        <v>0</v>
+      </c>
+      <c r="T18" s="16">
+        <f>SUM(R18:S18)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="6"/>
+      <c r="V18" s="44"/>
+      <c r="W18" s="21">
+        <f>L18*0.2+Q18*0.25+T18*0.25+U18*0.3+V18*0.1</f>
+        <v>28.958333333333336</v>
+      </c>
+      <c r="X18" s="1"/>
+    </row>
+    <row r="19" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="16">
-        <f>SUM(R18:U18)/V$1</f>
-        <v>50</v>
-      </c>
-      <c r="W18" s="6"/>
-      <c r="X18" s="44"/>
-      <c r="Y18" s="21">
-        <f>L18*0.2+Q18*0.25+V18*0.25+W18*0.3+X18*0.15</f>
-        <v>16.5</v>
-      </c>
-      <c r="Z18" s="1"/>
-    </row>
-    <row r="19" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>99</v>
-      </c>
       <c r="B19" s="3" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="D19" s="12">
         <v>0</v>
@@ -2659,64 +2729,70 @@
       <c r="G19" s="12">
         <v>0</v>
       </c>
-      <c r="H19" s="61">
-        <v>0</v>
+      <c r="H19" s="51">
+        <v>2</v>
       </c>
       <c r="I19" s="7">
-        <v>2</v>
-      </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="58"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0</v>
+      </c>
+      <c r="K19" s="48">
+        <v>0</v>
+      </c>
       <c r="L19" s="16">
         <f>SUM(D19:J19)*50/(L$1-K19)</f>
-        <v>20</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="M19" s="14">
         <v>0</v>
       </c>
       <c r="N19" s="6">
-        <v>75</v>
-      </c>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="6">
+        <v>0</v>
+      </c>
+      <c r="P19" s="48">
+        <v>0</v>
+      </c>
       <c r="Q19" s="16">
-        <f>SUM(M19:P19)/Q$1</f>
-        <v>37.5</v>
+        <f>SUM(M19:O19)/(Q$1-P19)</f>
+        <v>0</v>
       </c>
       <c r="R19" s="14">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="S19" s="14">
-        <v>0</v>
-      </c>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="16">
-        <f>SUM(R19:U19)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W19" s="6"/>
-      <c r="X19" s="44"/>
-      <c r="Y19" s="21">
-        <f>L19*0.2+Q19*0.25+V19*0.25+W19*0.3+X19*0.1</f>
-        <v>13.375</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="T19" s="16">
+        <f>SUM(R19:S19)/T$1</f>
+        <v>50</v>
+      </c>
+      <c r="U19" s="6"/>
+      <c r="V19" s="44"/>
+      <c r="W19" s="21">
+        <f>L19*0.2+Q19*0.25+T19*0.25+U19*0.3+V19*0.15</f>
+        <v>15.833333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" s="47" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>88</v>
-      </c>
       <c r="D20" s="12">
         <v>0</v>
       </c>
-      <c r="E20" s="12">
-        <v>0</v>
+      <c r="E20" s="54" t="s">
+        <v>95</v>
       </c>
       <c r="F20" s="12">
         <v>0</v>
@@ -2724,19 +2800,21 @@
       <c r="G20" s="12">
         <v>0</v>
       </c>
-      <c r="H20" s="61">
+      <c r="H20" s="51">
         <v>0</v>
       </c>
       <c r="I20" s="7">
         <v>1.6</v>
       </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="58">
-        <v>0</v>
+      <c r="J20" s="7">
+        <v>2</v>
+      </c>
+      <c r="K20" s="48">
+        <v>1</v>
       </c>
       <c r="L20" s="16">
         <f>SUM(D20:J20)*50/(L$1-K20)</f>
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="M20" s="14">
         <v>0</v>
@@ -2744,10 +2822,14 @@
       <c r="N20" s="6">
         <v>40</v>
       </c>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="O20" s="6">
+        <v>20</v>
+      </c>
+      <c r="P20" s="48">
+        <v>0</v>
+      </c>
       <c r="Q20" s="16">
-        <f>SUM(M20:P20)/Q$1</f>
+        <f>SUM(M20:O20)/(Q$1-P20)</f>
         <v>20</v>
       </c>
       <c r="R20" s="14">
@@ -2756,30 +2838,28 @@
       <c r="S20" s="14">
         <v>0</v>
       </c>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="16">
-        <f>SUM(R20:U20)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W20" s="6"/>
-      <c r="X20" s="44"/>
-      <c r="Y20" s="21">
-        <f>L20*0.2+Q20*0.25+V20*0.25+W20*0.3+X20*0.1</f>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="Z20" s="1"/>
-    </row>
-    <row r="21" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T20" s="16">
+        <f>SUM(R20:S20)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U20" s="6"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="21">
+        <f>L20*0.2+Q20*0.25+T20*0.25+U20*0.3+V20*0.1</f>
+        <v>12.2</v>
+      </c>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>94</v>
-      </c>
       <c r="D21" s="12">
         <v>0</v>
       </c>
@@ -2792,19 +2872,21 @@
       <c r="G21" s="12">
         <v>0</v>
       </c>
-      <c r="H21" s="61">
+      <c r="H21" s="51">
         <v>0</v>
       </c>
       <c r="I21" s="7">
         <v>0.9</v>
       </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="58">
+      <c r="J21" s="7">
+        <v>0</v>
+      </c>
+      <c r="K21" s="48">
         <v>0</v>
       </c>
       <c r="L21" s="16">
         <f>SUM(D21:J21)*50/(L$1-K21)</f>
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="M21" s="14">
         <v>0</v>
@@ -2812,638 +2894,675 @@
       <c r="N21" s="6">
         <v>40</v>
       </c>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
+      <c r="O21" s="6">
+        <v>80</v>
+      </c>
+      <c r="P21" s="48">
+        <v>0</v>
+      </c>
       <c r="Q21" s="16">
-        <f>SUM(M21:P21)/Q$1</f>
+        <f>SUM(M21:O21)/(Q$1-P21)</f>
+        <v>40</v>
+      </c>
+      <c r="R21" s="14">
+        <v>0</v>
+      </c>
+      <c r="S21" s="14">
+        <v>0</v>
+      </c>
+      <c r="T21" s="16">
+        <f>SUM(R21:S21)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U21" s="6"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="21">
+        <f>L21*0.2+Q21*0.25+T21*0.25+U21*0.3+V21*0.1</f>
+        <v>11.5</v>
+      </c>
+      <c r="X21" s="9"/>
+    </row>
+    <row r="22" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="59">
+        <v>0</v>
+      </c>
+      <c r="E22" s="59">
+        <v>0</v>
+      </c>
+      <c r="F22" s="59">
+        <v>0</v>
+      </c>
+      <c r="G22" s="59">
+        <v>0</v>
+      </c>
+      <c r="H22" s="60">
+        <v>0</v>
+      </c>
+      <c r="I22" s="61">
+        <v>0</v>
+      </c>
+      <c r="J22" s="61">
+        <v>0</v>
+      </c>
+      <c r="K22" s="62">
+        <v>0</v>
+      </c>
+      <c r="L22" s="63">
+        <f>SUM(D22:J22)*50/(L$1-K22)</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="64">
+        <v>0</v>
+      </c>
+      <c r="N22" s="65">
+        <v>0</v>
+      </c>
+      <c r="O22" s="65">
+        <v>0</v>
+      </c>
+      <c r="P22" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="63">
+        <f>SUM(M22:O22)/(Q$1-P22)</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="64">
+        <v>0</v>
+      </c>
+      <c r="S22" s="64">
+        <v>0</v>
+      </c>
+      <c r="T22" s="63">
+        <f>SUM(R22:S22)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="65"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="67">
+        <f>L22*0.2+Q22*0.25+T22*0.25+U22*0.3+V22*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="59">
+        <v>0</v>
+      </c>
+      <c r="E23" s="59">
+        <v>0</v>
+      </c>
+      <c r="F23" s="59">
+        <v>0</v>
+      </c>
+      <c r="G23" s="59">
+        <v>0</v>
+      </c>
+      <c r="H23" s="60">
+        <v>0</v>
+      </c>
+      <c r="I23" s="61">
+        <v>0</v>
+      </c>
+      <c r="J23" s="61">
+        <v>0</v>
+      </c>
+      <c r="K23" s="62">
+        <v>0</v>
+      </c>
+      <c r="L23" s="63">
+        <f>SUM(D23:J23)*50/(L$1-K23)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="64">
+        <v>0</v>
+      </c>
+      <c r="N23" s="65">
+        <v>0</v>
+      </c>
+      <c r="O23" s="65">
+        <v>0</v>
+      </c>
+      <c r="P23" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="63">
+        <f>SUM(M23:O23)/(Q$1-P23)</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="64">
+        <v>0</v>
+      </c>
+      <c r="S23" s="64">
+        <v>0</v>
+      </c>
+      <c r="T23" s="63">
+        <f>SUM(R23:S23)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U23" s="65"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="67">
+        <f>L23*0.2+Q23*0.25+T23*0.25+U23*0.3+V23*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="59">
+        <v>0</v>
+      </c>
+      <c r="E24" s="59">
+        <v>0</v>
+      </c>
+      <c r="F24" s="59">
+        <v>0</v>
+      </c>
+      <c r="G24" s="59">
+        <v>0</v>
+      </c>
+      <c r="H24" s="60">
+        <v>0</v>
+      </c>
+      <c r="I24" s="61">
+        <v>0</v>
+      </c>
+      <c r="J24" s="61">
+        <v>0</v>
+      </c>
+      <c r="K24" s="62">
+        <v>0</v>
+      </c>
+      <c r="L24" s="63">
+        <f>SUM(D24:J24)*50/(L$1-K24)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="64">
+        <v>0</v>
+      </c>
+      <c r="N24" s="65">
+        <v>0</v>
+      </c>
+      <c r="O24" s="65">
+        <v>0</v>
+      </c>
+      <c r="P24" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="63">
+        <f>SUM(M24:O24)/(Q$1-P24)</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="64">
+        <v>0</v>
+      </c>
+      <c r="S24" s="64">
+        <v>0</v>
+      </c>
+      <c r="T24" s="63">
+        <f>SUM(R24:S24)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U24" s="65"/>
+      <c r="V24" s="66"/>
+      <c r="W24" s="67">
+        <f>L24*0.2+Q24*0.25+T24*0.25+U24*0.3+V24*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="59">
+        <v>0</v>
+      </c>
+      <c r="E25" s="59">
+        <v>0</v>
+      </c>
+      <c r="F25" s="59">
+        <v>0</v>
+      </c>
+      <c r="G25" s="59">
+        <v>0</v>
+      </c>
+      <c r="H25" s="60">
+        <v>0</v>
+      </c>
+      <c r="I25" s="61">
+        <v>0</v>
+      </c>
+      <c r="J25" s="61">
+        <v>0</v>
+      </c>
+      <c r="K25" s="62">
+        <v>0</v>
+      </c>
+      <c r="L25" s="63">
+        <f>SUM(D25:J25)*50/(L$1-K25)</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="64">
+        <v>0</v>
+      </c>
+      <c r="N25" s="65">
+        <v>0</v>
+      </c>
+      <c r="O25" s="65">
+        <v>0</v>
+      </c>
+      <c r="P25" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="63">
+        <f>SUM(M25:O25)/(Q$1-P25)</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="64">
+        <v>0</v>
+      </c>
+      <c r="S25" s="64">
+        <v>0</v>
+      </c>
+      <c r="T25" s="63">
+        <f>SUM(R25:S25)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U25" s="65"/>
+      <c r="V25" s="66"/>
+      <c r="W25" s="67">
+        <f>L25*0.2+Q25*0.25+T25*0.25+U25*0.3+V25*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="59">
+        <v>0</v>
+      </c>
+      <c r="E26" s="59">
+        <v>0</v>
+      </c>
+      <c r="F26" s="59">
+        <v>0</v>
+      </c>
+      <c r="G26" s="59">
+        <v>0</v>
+      </c>
+      <c r="H26" s="60">
+        <v>0</v>
+      </c>
+      <c r="I26" s="61">
+        <v>0</v>
+      </c>
+      <c r="J26" s="61">
+        <v>0</v>
+      </c>
+      <c r="K26" s="62">
+        <v>0</v>
+      </c>
+      <c r="L26" s="63">
+        <f>SUM(D26:J26)*50/(L$1-K26)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="64">
+        <v>0</v>
+      </c>
+      <c r="N26" s="65">
+        <v>0</v>
+      </c>
+      <c r="O26" s="65">
+        <v>0</v>
+      </c>
+      <c r="P26" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="63">
+        <f>SUM(M26:O26)/(Q$1-P26)</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="64">
+        <v>0</v>
+      </c>
+      <c r="S26" s="64">
+        <v>0</v>
+      </c>
+      <c r="T26" s="63">
+        <f>SUM(R26:S26)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U26" s="65"/>
+      <c r="V26" s="66"/>
+      <c r="W26" s="67">
+        <f>L26*0.2+Q26*0.25+T26*0.25+U26*0.3+V26*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="R21" s="14">
-        <v>0</v>
-      </c>
-      <c r="S21" s="14">
-        <v>0</v>
-      </c>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="16">
-        <f>SUM(R21:U21)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W21" s="6"/>
-      <c r="X21" s="44"/>
-      <c r="Y21" s="21">
-        <f>L21*0.2+Q21*0.25+V21*0.25+W21*0.3+X21*0.1</f>
-        <v>6.8</v>
-      </c>
-      <c r="Z21" s="9"/>
-    </row>
-    <row r="22" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="50">
-        <v>0</v>
-      </c>
-      <c r="E22" s="50">
-        <v>0</v>
-      </c>
-      <c r="F22" s="50">
-        <v>0</v>
-      </c>
-      <c r="G22" s="50">
-        <v>0</v>
-      </c>
-      <c r="H22" s="62">
-        <v>0</v>
-      </c>
-      <c r="I22" s="51">
-        <v>0</v>
-      </c>
-      <c r="J22" s="51"/>
-      <c r="K22" s="58">
-        <v>0</v>
-      </c>
-      <c r="L22" s="16">
-        <f>SUM(D22:J22)*50/(L$1-K22)</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="53">
-        <v>0</v>
-      </c>
-      <c r="N22" s="54">
-        <v>0</v>
-      </c>
-      <c r="O22" s="54"/>
-      <c r="P22" s="54"/>
-      <c r="Q22" s="52">
-        <f>SUM(M22:P22)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R22" s="53">
-        <v>0</v>
-      </c>
-      <c r="S22" s="53">
-        <v>0</v>
-      </c>
-      <c r="T22" s="53"/>
-      <c r="U22" s="53"/>
-      <c r="V22" s="52">
-        <f>SUM(R22:U22)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W22" s="54"/>
-      <c r="X22" s="55"/>
-      <c r="Y22" s="56">
-        <f>L22*0.2+Q22*0.25+V22*0.25+W22*0.3+X22*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="50">
-        <v>0</v>
-      </c>
-      <c r="E23" s="50">
-        <v>0</v>
-      </c>
-      <c r="F23" s="50">
-        <v>0</v>
-      </c>
-      <c r="G23" s="50">
-        <v>0</v>
-      </c>
-      <c r="H23" s="62">
-        <v>0</v>
-      </c>
-      <c r="I23" s="51">
-        <v>0</v>
-      </c>
-      <c r="J23" s="51"/>
-      <c r="K23" s="58">
-        <v>0</v>
-      </c>
-      <c r="L23" s="16">
-        <f>SUM(D23:J23)*50/(L$1-K23)</f>
-        <v>0</v>
-      </c>
-      <c r="M23" s="53">
-        <v>0</v>
-      </c>
-      <c r="N23" s="54">
-        <v>0</v>
-      </c>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="52">
-        <f>SUM(M23:P23)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R23" s="53">
-        <v>0</v>
-      </c>
-      <c r="S23" s="53">
-        <v>0</v>
-      </c>
-      <c r="T23" s="53"/>
-      <c r="U23" s="53"/>
-      <c r="V23" s="52">
-        <f>SUM(R23:U23)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W23" s="54"/>
-      <c r="X23" s="55"/>
-      <c r="Y23" s="56">
-        <f>L23*0.2+Q23*0.25+V23*0.25+W23*0.3+X23*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="50">
-        <v>0</v>
-      </c>
-      <c r="E24" s="50">
-        <v>0</v>
-      </c>
-      <c r="F24" s="50">
-        <v>0</v>
-      </c>
-      <c r="G24" s="50">
-        <v>0</v>
-      </c>
-      <c r="H24" s="62">
-        <v>0</v>
-      </c>
-      <c r="I24" s="51">
-        <v>0</v>
-      </c>
-      <c r="J24" s="51"/>
-      <c r="K24" s="58">
-        <v>0</v>
-      </c>
-      <c r="L24" s="16">
-        <f>SUM(D24:J24)*50/(L$1-K24)</f>
-        <v>0</v>
-      </c>
-      <c r="M24" s="53">
-        <v>0</v>
-      </c>
-      <c r="N24" s="54">
-        <v>0</v>
-      </c>
-      <c r="O24" s="54"/>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="52">
-        <f>SUM(M24:P24)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R24" s="53">
-        <v>0</v>
-      </c>
-      <c r="S24" s="53">
-        <v>0</v>
-      </c>
-      <c r="T24" s="53"/>
-      <c r="U24" s="53"/>
-      <c r="V24" s="52">
-        <f>SUM(R24:U24)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W24" s="54"/>
-      <c r="X24" s="55"/>
-      <c r="Y24" s="56">
-        <f>L24*0.2+Q24*0.25+V24*0.25+W24*0.3+X24*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="50">
-        <v>0</v>
-      </c>
-      <c r="E25" s="50">
-        <v>0</v>
-      </c>
-      <c r="F25" s="50">
-        <v>0</v>
-      </c>
-      <c r="G25" s="50">
-        <v>0</v>
-      </c>
-      <c r="H25" s="62">
-        <v>0</v>
-      </c>
-      <c r="I25" s="51">
-        <v>0</v>
-      </c>
-      <c r="J25" s="51"/>
-      <c r="K25" s="58">
-        <v>0</v>
-      </c>
-      <c r="L25" s="16">
-        <f>SUM(D25:J25)*50/(L$1-K25)</f>
-        <v>0</v>
-      </c>
-      <c r="M25" s="53">
-        <v>0</v>
-      </c>
-      <c r="N25" s="54">
-        <v>0</v>
-      </c>
-      <c r="O25" s="54"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="52">
-        <f>SUM(M25:P25)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R25" s="53">
-        <v>0</v>
-      </c>
-      <c r="S25" s="53">
-        <v>0</v>
-      </c>
-      <c r="T25" s="53"/>
-      <c r="U25" s="53"/>
-      <c r="V25" s="52">
-        <f>SUM(R25:U25)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W25" s="54"/>
-      <c r="X25" s="55"/>
-      <c r="Y25" s="56">
-        <f>L25*0.2+Q25*0.25+V25*0.25+W25*0.3+X25*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="50">
-        <v>0</v>
-      </c>
-      <c r="E26" s="50">
-        <v>0</v>
-      </c>
-      <c r="F26" s="50">
-        <v>0</v>
-      </c>
-      <c r="G26" s="50">
-        <v>0</v>
-      </c>
-      <c r="H26" s="62">
-        <v>0</v>
-      </c>
-      <c r="I26" s="51">
-        <v>0</v>
-      </c>
-      <c r="J26" s="51"/>
-      <c r="K26" s="58">
-        <v>0</v>
-      </c>
-      <c r="L26" s="16">
-        <f>SUM(D26:J26)*50/(L$1-K26)</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="53">
-        <v>0</v>
-      </c>
-      <c r="N26" s="54">
-        <v>0</v>
-      </c>
-      <c r="O26" s="54"/>
-      <c r="P26" s="54"/>
-      <c r="Q26" s="52">
-        <f>SUM(M26:P26)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R26" s="53">
-        <v>0</v>
-      </c>
-      <c r="S26" s="53">
-        <v>0</v>
-      </c>
-      <c r="T26" s="53"/>
-      <c r="U26" s="53"/>
-      <c r="V26" s="52">
-        <f>SUM(R26:U26)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W26" s="54"/>
-      <c r="X26" s="55"/>
-      <c r="Y26" s="56">
-        <f>L26*0.2+Q26*0.25+V26*0.25+W26*0.3+X26*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="50">
-        <v>0</v>
-      </c>
-      <c r="E27" s="50">
-        <v>0</v>
-      </c>
-      <c r="F27" s="50">
-        <v>0</v>
-      </c>
-      <c r="G27" s="50">
-        <v>0</v>
-      </c>
-      <c r="H27" s="62">
-        <v>0</v>
-      </c>
-      <c r="I27" s="51">
-        <v>0</v>
-      </c>
-      <c r="J27" s="51"/>
-      <c r="K27" s="58">
-        <v>0</v>
-      </c>
-      <c r="L27" s="16">
+      <c r="D27" s="59">
+        <v>0</v>
+      </c>
+      <c r="E27" s="59">
+        <v>0</v>
+      </c>
+      <c r="F27" s="59">
+        <v>0</v>
+      </c>
+      <c r="G27" s="59">
+        <v>0</v>
+      </c>
+      <c r="H27" s="60">
+        <v>0</v>
+      </c>
+      <c r="I27" s="61">
+        <v>0</v>
+      </c>
+      <c r="J27" s="61">
+        <v>0</v>
+      </c>
+      <c r="K27" s="62">
+        <v>0</v>
+      </c>
+      <c r="L27" s="63">
         <f>SUM(D27:J27)*50/(L$1-K27)</f>
         <v>0</v>
       </c>
-      <c r="M27" s="53">
-        <v>0</v>
-      </c>
-      <c r="N27" s="54">
-        <v>0</v>
-      </c>
-      <c r="O27" s="54"/>
-      <c r="P27" s="54"/>
-      <c r="Q27" s="52">
-        <f>SUM(M27:P27)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R27" s="53">
-        <v>0</v>
-      </c>
-      <c r="S27" s="53">
-        <v>0</v>
-      </c>
-      <c r="T27" s="53"/>
-      <c r="U27" s="53"/>
-      <c r="V27" s="52">
-        <f>SUM(R27:U27)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W27" s="54"/>
-      <c r="X27" s="55"/>
-      <c r="Y27" s="56">
-        <f>L27*0.2+Q27*0.25+V27*0.25+W27*0.3+X27*0.15</f>
-        <v>0</v>
-      </c>
-      <c r="Z27" s="57"/>
-    </row>
-    <row r="28" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47" t="s">
+      <c r="M27" s="64">
+        <v>0</v>
+      </c>
+      <c r="N27" s="65">
+        <v>0</v>
+      </c>
+      <c r="O27" s="65">
+        <v>0</v>
+      </c>
+      <c r="P27" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="63">
+        <f>SUM(M27:O27)/(Q$1-P27)</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="64">
+        <v>0</v>
+      </c>
+      <c r="S27" s="64">
+        <v>0</v>
+      </c>
+      <c r="T27" s="63">
+        <f>SUM(R27:S27)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U27" s="65"/>
+      <c r="V27" s="66"/>
+      <c r="W27" s="67">
+        <f>L27*0.2+Q27*0.25+T27*0.25+U27*0.3+V27*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="50">
-        <v>0</v>
-      </c>
-      <c r="E28" s="50">
-        <v>0</v>
-      </c>
-      <c r="F28" s="50">
-        <v>0</v>
-      </c>
-      <c r="G28" s="50">
-        <v>0</v>
-      </c>
-      <c r="H28" s="62">
-        <v>0</v>
-      </c>
-      <c r="I28" s="51">
-        <v>0</v>
-      </c>
-      <c r="J28" s="51"/>
-      <c r="K28" s="58">
-        <v>0</v>
-      </c>
-      <c r="L28" s="16">
+      <c r="D28" s="59">
+        <v>0</v>
+      </c>
+      <c r="E28" s="59">
+        <v>0</v>
+      </c>
+      <c r="F28" s="59">
+        <v>0</v>
+      </c>
+      <c r="G28" s="59">
+        <v>0</v>
+      </c>
+      <c r="H28" s="60">
+        <v>0</v>
+      </c>
+      <c r="I28" s="61">
+        <v>0</v>
+      </c>
+      <c r="J28" s="61">
+        <v>0</v>
+      </c>
+      <c r="K28" s="62">
+        <v>0</v>
+      </c>
+      <c r="L28" s="63">
         <f>SUM(D28:J28)*50/(L$1-K28)</f>
         <v>0</v>
       </c>
-      <c r="M28" s="53">
-        <v>0</v>
-      </c>
-      <c r="N28" s="54">
-        <v>0</v>
-      </c>
-      <c r="O28" s="54"/>
-      <c r="P28" s="54"/>
-      <c r="Q28" s="52">
-        <f>SUM(M28:P28)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R28" s="53">
-        <v>0</v>
-      </c>
-      <c r="S28" s="53">
-        <v>0</v>
-      </c>
-      <c r="T28" s="53"/>
-      <c r="U28" s="53"/>
-      <c r="V28" s="52">
-        <f>SUM(R28:U28)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W28" s="54"/>
-      <c r="X28" s="55"/>
-      <c r="Y28" s="56">
-        <f>L28*0.2+Q28*0.25+V28*0.25+W28*0.3+X28*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" s="57" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47" t="s">
+      <c r="M28" s="64">
+        <v>0</v>
+      </c>
+      <c r="N28" s="65">
+        <v>0</v>
+      </c>
+      <c r="O28" s="65">
+        <v>0</v>
+      </c>
+      <c r="P28" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="63">
+        <f>SUM(M28:O28)/(Q$1-P28)</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="64">
+        <v>0</v>
+      </c>
+      <c r="S28" s="64">
+        <v>0</v>
+      </c>
+      <c r="T28" s="63">
+        <f>SUM(R28:S28)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U28" s="65"/>
+      <c r="V28" s="66"/>
+      <c r="W28" s="67">
+        <f>L28*0.2+Q28*0.25+T28*0.25+U28*0.3+V28*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="50">
-        <v>0</v>
-      </c>
-      <c r="E29" s="50">
-        <v>0</v>
-      </c>
-      <c r="F29" s="50">
-        <v>0</v>
-      </c>
-      <c r="G29" s="50">
-        <v>0</v>
-      </c>
-      <c r="H29" s="62">
-        <v>0</v>
-      </c>
-      <c r="I29" s="51">
-        <v>0</v>
-      </c>
-      <c r="J29" s="51"/>
-      <c r="K29" s="58">
-        <v>0</v>
-      </c>
-      <c r="L29" s="16">
+      <c r="D29" s="59">
+        <v>0</v>
+      </c>
+      <c r="E29" s="59">
+        <v>0</v>
+      </c>
+      <c r="F29" s="59">
+        <v>0</v>
+      </c>
+      <c r="G29" s="59">
+        <v>0</v>
+      </c>
+      <c r="H29" s="60">
+        <v>0</v>
+      </c>
+      <c r="I29" s="61">
+        <v>0</v>
+      </c>
+      <c r="J29" s="61">
+        <v>0</v>
+      </c>
+      <c r="K29" s="62">
+        <v>0</v>
+      </c>
+      <c r="L29" s="63">
         <f>SUM(D29:J29)*50/(L$1-K29)</f>
         <v>0</v>
       </c>
-      <c r="M29" s="53">
-        <v>0</v>
-      </c>
-      <c r="N29" s="54">
-        <v>0</v>
-      </c>
-      <c r="O29" s="54"/>
-      <c r="P29" s="54"/>
-      <c r="Q29" s="52">
-        <f>SUM(M29:P29)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R29" s="53">
-        <v>0</v>
-      </c>
-      <c r="S29" s="53">
-        <v>0</v>
-      </c>
-      <c r="T29" s="53"/>
-      <c r="U29" s="53"/>
-      <c r="V29" s="52">
-        <f>SUM(R29:U29)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W29" s="54"/>
-      <c r="X29" s="55"/>
-      <c r="Y29" s="56">
-        <f>L29*0.2+Q29*0.25+V29*0.25+W29*0.3+X29*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47" t="s">
+      <c r="M29" s="64">
+        <v>0</v>
+      </c>
+      <c r="N29" s="65">
+        <v>0</v>
+      </c>
+      <c r="O29" s="65">
+        <v>0</v>
+      </c>
+      <c r="P29" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="63">
+        <f>SUM(M29:O29)/(Q$1-P29)</f>
+        <v>0</v>
+      </c>
+      <c r="R29" s="64">
+        <v>0</v>
+      </c>
+      <c r="S29" s="64">
+        <v>0</v>
+      </c>
+      <c r="T29" s="63">
+        <f>SUM(R29:S29)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U29" s="65"/>
+      <c r="V29" s="66"/>
+      <c r="W29" s="67">
+        <f>L29*0.2+Q29*0.25+T29*0.25+U29*0.3+V29*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="48" t="s">
+      <c r="C30" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="50">
-        <v>0</v>
-      </c>
-      <c r="E30" s="50">
-        <v>0</v>
-      </c>
-      <c r="F30" s="50">
-        <v>0</v>
-      </c>
-      <c r="G30" s="50">
-        <v>0</v>
-      </c>
-      <c r="H30" s="62">
-        <v>0</v>
-      </c>
-      <c r="I30" s="51">
-        <v>0</v>
-      </c>
-      <c r="J30" s="51"/>
-      <c r="K30" s="58">
-        <v>0</v>
-      </c>
-      <c r="L30" s="16">
+      <c r="D30" s="59">
+        <v>0</v>
+      </c>
+      <c r="E30" s="59">
+        <v>0</v>
+      </c>
+      <c r="F30" s="59">
+        <v>0</v>
+      </c>
+      <c r="G30" s="59">
+        <v>0</v>
+      </c>
+      <c r="H30" s="60">
+        <v>0</v>
+      </c>
+      <c r="I30" s="61">
+        <v>0</v>
+      </c>
+      <c r="J30" s="61">
+        <v>0</v>
+      </c>
+      <c r="K30" s="62">
+        <v>0</v>
+      </c>
+      <c r="L30" s="63">
         <f>SUM(D30:J30)*50/(L$1-K30)</f>
         <v>0</v>
       </c>
-      <c r="M30" s="53">
-        <v>0</v>
-      </c>
-      <c r="N30" s="54">
-        <v>0</v>
-      </c>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="52">
-        <f>SUM(M30:P30)/Q$1</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="53">
-        <v>0</v>
-      </c>
-      <c r="S30" s="53">
-        <v>0</v>
-      </c>
-      <c r="T30" s="53"/>
-      <c r="U30" s="53"/>
-      <c r="V30" s="52">
-        <f>SUM(R30:U30)/V$1</f>
-        <v>0</v>
-      </c>
-      <c r="W30" s="54"/>
-      <c r="X30" s="55"/>
-      <c r="Y30" s="56">
-        <f>L30*0.2+Q30*0.25+V30*0.25+W30*0.3+X30*0.1</f>
-        <v>0</v>
-      </c>
-      <c r="Z30" s="57"/>
-    </row>
-    <row r="31" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M30" s="64">
+        <v>0</v>
+      </c>
+      <c r="N30" s="65">
+        <v>0</v>
+      </c>
+      <c r="O30" s="65">
+        <v>0</v>
+      </c>
+      <c r="P30" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="63">
+        <f>SUM(M30:O30)/(Q$1-P30)</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="64">
+        <v>0</v>
+      </c>
+      <c r="S30" s="64">
+        <v>0</v>
+      </c>
+      <c r="T30" s="63">
+        <f>SUM(R30:S30)/T$1</f>
+        <v>0</v>
+      </c>
+      <c r="U30" s="65"/>
+      <c r="V30" s="66"/>
+      <c r="W30" s="67">
+        <f>L30*0.2+Q30*0.25+T30*0.25+U30*0.3+V30*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="X30" s="68"/>
+    </row>
+    <row r="31" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -3451,7 +3570,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="63"/>
+      <c r="H31" s="52"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3464,10 +3583,8 @@
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-    </row>
-    <row r="32" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -3475,7 +3592,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="63"/>
+      <c r="H32" s="52"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3488,10 +3605,8 @@
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-    </row>
-    <row r="33" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -3499,7 +3614,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="63"/>
+      <c r="H33" s="52"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3512,10 +3627,8 @@
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-    </row>
-    <row r="34" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3523,7 +3636,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="63"/>
+      <c r="H34" s="52"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3536,10 +3649,8 @@
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
       <c r="T34" s="9"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="9"/>
-    </row>
-    <row r="35" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3547,7 +3658,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="63"/>
+      <c r="H35" s="52"/>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3560,10 +3671,8 @@
       <c r="R35" s="9"/>
       <c r="S35" s="9"/>
       <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-    </row>
-    <row r="36" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -3571,7 +3680,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="63"/>
+      <c r="H36" s="52"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -3584,10 +3693,8 @@
       <c r="R36" s="9"/>
       <c r="S36" s="9"/>
       <c r="T36" s="9"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
-    </row>
-    <row r="37" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3595,7 +3702,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="63"/>
+      <c r="H37" s="52"/>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -3608,10 +3715,8 @@
       <c r="R37" s="9"/>
       <c r="S37" s="9"/>
       <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="9"/>
-    </row>
-    <row r="38" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3619,7 +3724,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="63"/>
+      <c r="H38" s="52"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -3632,10 +3737,8 @@
       <c r="R38" s="9"/>
       <c r="S38" s="9"/>
       <c r="T38" s="9"/>
-      <c r="U38" s="9"/>
-      <c r="V38" s="9"/>
-    </row>
-    <row r="39" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -3643,7 +3746,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="63"/>
+      <c r="H39" s="52"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -3656,10 +3759,8 @@
       <c r="R39" s="9"/>
       <c r="S39" s="9"/>
       <c r="T39" s="9"/>
-      <c r="U39" s="9"/>
-      <c r="V39" s="9"/>
-    </row>
-    <row r="40" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -3667,7 +3768,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="63"/>
+      <c r="H40" s="52"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
@@ -3680,10 +3781,8 @@
       <c r="R40" s="9"/>
       <c r="S40" s="9"/>
       <c r="T40" s="9"/>
-      <c r="U40" s="9"/>
-      <c r="V40" s="9"/>
-    </row>
-    <row r="41" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -3691,7 +3790,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="63"/>
+      <c r="H41" s="52"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
@@ -3704,10 +3803,8 @@
       <c r="R41" s="9"/>
       <c r="S41" s="9"/>
       <c r="T41" s="9"/>
-      <c r="U41" s="9"/>
-      <c r="V41" s="9"/>
-    </row>
-    <row r="42" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -3715,7 +3812,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="63"/>
+      <c r="H42" s="52"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -3728,10 +3825,8 @@
       <c r="R42" s="9"/>
       <c r="S42" s="9"/>
       <c r="T42" s="9"/>
-      <c r="U42" s="9"/>
-      <c r="V42" s="9"/>
-    </row>
-    <row r="43" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -3739,7 +3834,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="63"/>
+      <c r="H43" s="52"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
@@ -3752,10 +3847,8 @@
       <c r="R43" s="9"/>
       <c r="S43" s="9"/>
       <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
-      <c r="V43" s="9"/>
-    </row>
-    <row r="44" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -3763,7 +3856,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="63"/>
+      <c r="H44" s="52"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -3776,10 +3869,8 @@
       <c r="R44" s="9"/>
       <c r="S44" s="9"/>
       <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-      <c r="V44" s="9"/>
-    </row>
-    <row r="45" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3787,7 +3878,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="63"/>
+      <c r="H45" s="52"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -3800,10 +3891,8 @@
       <c r="R45" s="9"/>
       <c r="S45" s="9"/>
       <c r="T45" s="9"/>
-      <c r="U45" s="9"/>
-      <c r="V45" s="9"/>
-    </row>
-    <row r="46" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -3811,7 +3900,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="63"/>
+      <c r="H46" s="52"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -3824,10 +3913,8 @@
       <c r="R46" s="9"/>
       <c r="S46" s="9"/>
       <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
-      <c r="V46" s="9"/>
-    </row>
-    <row r="47" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -3835,7 +3922,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="63"/>
+      <c r="H47" s="52"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -3848,10 +3935,8 @@
       <c r="R47" s="9"/>
       <c r="S47" s="9"/>
       <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
-      <c r="V47" s="9"/>
-    </row>
-    <row r="48" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -3859,7 +3944,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="63"/>
+      <c r="H48" s="52"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -3872,10 +3957,8 @@
       <c r="R48" s="9"/>
       <c r="S48" s="9"/>
       <c r="T48" s="9"/>
-      <c r="U48" s="9"/>
-      <c r="V48" s="9"/>
-    </row>
-    <row r="49" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -3883,7 +3966,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="63"/>
+      <c r="H49" s="52"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -3896,10 +3979,8 @@
       <c r="R49" s="9"/>
       <c r="S49" s="9"/>
       <c r="T49" s="9"/>
-      <c r="U49" s="9"/>
-      <c r="V49" s="9"/>
-    </row>
-    <row r="50" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -3907,7 +3988,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="63"/>
+      <c r="H50" s="52"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
@@ -3920,10 +4001,8 @@
       <c r="R50" s="9"/>
       <c r="S50" s="9"/>
       <c r="T50" s="9"/>
-      <c r="U50" s="9"/>
-      <c r="V50" s="9"/>
-    </row>
-    <row r="51" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -3931,7 +4010,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="63"/>
+      <c r="H51" s="52"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -3944,10 +4023,8 @@
       <c r="R51" s="9"/>
       <c r="S51" s="9"/>
       <c r="T51" s="9"/>
-      <c r="U51" s="9"/>
-      <c r="V51" s="9"/>
-    </row>
-    <row r="52" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -3955,7 +4032,7 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
-      <c r="H52" s="63"/>
+      <c r="H52" s="52"/>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -3968,10 +4045,8 @@
       <c r="R52" s="9"/>
       <c r="S52" s="9"/>
       <c r="T52" s="9"/>
-      <c r="U52" s="9"/>
-      <c r="V52" s="9"/>
-    </row>
-    <row r="53" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -3979,7 +4054,7 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="63"/>
+      <c r="H53" s="52"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -3992,10 +4067,8 @@
       <c r="R53" s="9"/>
       <c r="S53" s="9"/>
       <c r="T53" s="9"/>
-      <c r="U53" s="9"/>
-      <c r="V53" s="9"/>
-    </row>
-    <row r="54" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -4003,7 +4076,7 @@
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
-      <c r="H54" s="63"/>
+      <c r="H54" s="52"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -4016,10 +4089,8 @@
       <c r="R54" s="9"/>
       <c r="S54" s="9"/>
       <c r="T54" s="9"/>
-      <c r="U54" s="9"/>
-      <c r="V54" s="9"/>
-    </row>
-    <row r="55" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -4027,7 +4098,7 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
-      <c r="H55" s="63"/>
+      <c r="H55" s="52"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -4040,10 +4111,8 @@
       <c r="R55" s="9"/>
       <c r="S55" s="9"/>
       <c r="T55" s="9"/>
-      <c r="U55" s="9"/>
-      <c r="V55" s="9"/>
-    </row>
-    <row r="56" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -4051,7 +4120,7 @@
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="63"/>
+      <c r="H56" s="52"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -4064,10 +4133,8 @@
       <c r="R56" s="9"/>
       <c r="S56" s="9"/>
       <c r="T56" s="9"/>
-      <c r="U56" s="9"/>
-      <c r="V56" s="9"/>
-    </row>
-    <row r="57" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -4075,7 +4142,7 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="63"/>
+      <c r="H57" s="52"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -4088,10 +4155,8 @@
       <c r="R57" s="9"/>
       <c r="S57" s="9"/>
       <c r="T57" s="9"/>
-      <c r="U57" s="9"/>
-      <c r="V57" s="9"/>
-    </row>
-    <row r="58" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -4099,7 +4164,7 @@
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
-      <c r="H58" s="63"/>
+      <c r="H58" s="52"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -4112,10 +4177,8 @@
       <c r="R58" s="9"/>
       <c r="S58" s="9"/>
       <c r="T58" s="9"/>
-      <c r="U58" s="9"/>
-      <c r="V58" s="9"/>
-    </row>
-    <row r="59" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -4123,7 +4186,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="63"/>
+      <c r="H59" s="52"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -4136,10 +4199,8 @@
       <c r="R59" s="9"/>
       <c r="S59" s="9"/>
       <c r="T59" s="9"/>
-      <c r="U59" s="9"/>
-      <c r="V59" s="9"/>
-    </row>
-    <row r="60" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -4147,7 +4208,7 @@
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="63"/>
+      <c r="H60" s="52"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -4160,10 +4221,8 @@
       <c r="R60" s="9"/>
       <c r="S60" s="9"/>
       <c r="T60" s="9"/>
-      <c r="U60" s="9"/>
-      <c r="V60" s="9"/>
-    </row>
-    <row r="61" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -4171,7 +4230,7 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
-      <c r="H61" s="63"/>
+      <c r="H61" s="52"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -4184,10 +4243,8 @@
       <c r="R61" s="9"/>
       <c r="S61" s="9"/>
       <c r="T61" s="9"/>
-      <c r="U61" s="9"/>
-      <c r="V61" s="9"/>
-    </row>
-    <row r="62" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -4195,7 +4252,7 @@
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
-      <c r="H62" s="63"/>
+      <c r="H62" s="52"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -4208,10 +4265,8 @@
       <c r="R62" s="9"/>
       <c r="S62" s="9"/>
       <c r="T62" s="9"/>
-      <c r="U62" s="9"/>
-      <c r="V62" s="9"/>
-    </row>
-    <row r="63" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -4219,7 +4274,7 @@
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
-      <c r="H63" s="63"/>
+      <c r="H63" s="52"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -4232,10 +4287,8 @@
       <c r="R63" s="9"/>
       <c r="S63" s="9"/>
       <c r="T63" s="9"/>
-      <c r="U63" s="9"/>
-      <c r="V63" s="9"/>
-    </row>
-    <row r="64" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -4243,7 +4296,7 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
-      <c r="H64" s="63"/>
+      <c r="H64" s="52"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -4256,10 +4309,8 @@
       <c r="R64" s="9"/>
       <c r="S64" s="9"/>
       <c r="T64" s="9"/>
-      <c r="U64" s="9"/>
-      <c r="V64" s="9"/>
-    </row>
-    <row r="65" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -4267,7 +4318,7 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="63"/>
+      <c r="H65" s="52"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -4280,10 +4331,8 @@
       <c r="R65" s="9"/>
       <c r="S65" s="9"/>
       <c r="T65" s="9"/>
-      <c r="U65" s="9"/>
-      <c r="V65" s="9"/>
-    </row>
-    <row r="66" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -4291,7 +4340,7 @@
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
-      <c r="H66" s="63"/>
+      <c r="H66" s="52"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -4304,10 +4353,8 @@
       <c r="R66" s="9"/>
       <c r="S66" s="9"/>
       <c r="T66" s="9"/>
-      <c r="U66" s="9"/>
-      <c r="V66" s="9"/>
-    </row>
-    <row r="67" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -4315,7 +4362,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="63"/>
+      <c r="H67" s="52"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -4328,10 +4375,8 @@
       <c r="R67" s="9"/>
       <c r="S67" s="9"/>
       <c r="T67" s="9"/>
-      <c r="U67" s="9"/>
-      <c r="V67" s="9"/>
-    </row>
-    <row r="68" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -4339,7 +4384,7 @@
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
-      <c r="H68" s="63"/>
+      <c r="H68" s="52"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -4352,10 +4397,8 @@
       <c r="R68" s="9"/>
       <c r="S68" s="9"/>
       <c r="T68" s="9"/>
-      <c r="U68" s="9"/>
-      <c r="V68" s="9"/>
-    </row>
-    <row r="69" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -4363,7 +4406,7 @@
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
-      <c r="H69" s="63"/>
+      <c r="H69" s="52"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -4376,10 +4419,8 @@
       <c r="R69" s="9"/>
       <c r="S69" s="9"/>
       <c r="T69" s="9"/>
-      <c r="U69" s="9"/>
-      <c r="V69" s="9"/>
-    </row>
-    <row r="70" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -4387,7 +4428,7 @@
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
-      <c r="H70" s="63"/>
+      <c r="H70" s="52"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -4400,10 +4441,8 @@
       <c r="R70" s="9"/>
       <c r="S70" s="9"/>
       <c r="T70" s="9"/>
-      <c r="U70" s="9"/>
-      <c r="V70" s="9"/>
-    </row>
-    <row r="71" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -4411,7 +4450,7 @@
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
-      <c r="H71" s="63"/>
+      <c r="H71" s="52"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -4424,10 +4463,8 @@
       <c r="R71" s="9"/>
       <c r="S71" s="9"/>
       <c r="T71" s="9"/>
-      <c r="U71" s="9"/>
-      <c r="V71" s="9"/>
-    </row>
-    <row r="72" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -4435,7 +4472,7 @@
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
-      <c r="H72" s="63"/>
+      <c r="H72" s="52"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -4448,10 +4485,8 @@
       <c r="R72" s="9"/>
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
-      <c r="U72" s="9"/>
-      <c r="V72" s="9"/>
-    </row>
-    <row r="73" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -4459,7 +4494,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
-      <c r="H73" s="63"/>
+      <c r="H73" s="52"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -4472,10 +4507,8 @@
       <c r="R73" s="9"/>
       <c r="S73" s="9"/>
       <c r="T73" s="9"/>
-      <c r="U73" s="9"/>
-      <c r="V73" s="9"/>
-    </row>
-    <row r="74" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -4483,7 +4516,7 @@
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
-      <c r="H74" s="63"/>
+      <c r="H74" s="52"/>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -4496,10 +4529,8 @@
       <c r="R74" s="9"/>
       <c r="S74" s="9"/>
       <c r="T74" s="9"/>
-      <c r="U74" s="9"/>
-      <c r="V74" s="9"/>
-    </row>
-    <row r="75" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -4507,7 +4538,7 @@
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
-      <c r="H75" s="63"/>
+      <c r="H75" s="52"/>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -4520,10 +4551,8 @@
       <c r="R75" s="9"/>
       <c r="S75" s="9"/>
       <c r="T75" s="9"/>
-      <c r="U75" s="9"/>
-      <c r="V75" s="9"/>
-    </row>
-    <row r="76" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -4531,7 +4560,7 @@
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
-      <c r="H76" s="63"/>
+      <c r="H76" s="52"/>
       <c r="I76" s="9"/>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
@@ -4544,17 +4573,15 @@
       <c r="R76" s="9"/>
       <c r="S76" s="9"/>
       <c r="T76" s="9"/>
-      <c r="U76" s="9"/>
-      <c r="V76" s="9"/>
     </row>
   </sheetData>
-  <sortState ref="A3:Z30">
-    <sortCondition descending="1" ref="Y3"/>
+  <sortState ref="A3:X30">
+    <sortCondition descending="1" ref="W3"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="M1:P1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:J30">
     <cfRule type="cellIs" dxfId="21" priority="19" operator="between">
@@ -4568,7 +4595,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W3:X30 M3:P30">
+  <conditionalFormatting sqref="U3:V30 M3:O30">
     <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
@@ -4585,7 +4612,7 @@
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:U30">
+  <conditionalFormatting sqref="R3:S30">
     <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
@@ -4630,7 +4657,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V30">
+  <conditionalFormatting sqref="T3:T30">
     <cfRule type="dataBar" priority="191">
       <dataBar>
         <cfvo type="min"/>
@@ -4644,7 +4671,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y30">
+  <conditionalFormatting sqref="W3:W30">
     <cfRule type="dataBar" priority="192">
       <dataBar>
         <cfvo type="min"/>
@@ -4695,7 +4722,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V3:V30</xm:sqref>
+          <xm:sqref>T3:T30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{43DC70F4-8291-4430-AFF0-577FC5E79CD9}">
@@ -4706,7 +4733,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Y3:Y30</xm:sqref>
+          <xm:sqref>W3:W30</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4751,30 +4778,30 @@
       <c r="B1" s="18"/>
       <c r="C1" s="34"/>
       <c r="D1" s="40"/>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="67" t="s">
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="33" t="s">
-        <v>45</v>
-      </c>
       <c r="R1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="19" t="s">
         <v>40</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ileri java hafta 8, vize sonrasi
</commit_message>
<xml_diff>
--- a/AdvancedJava/_docs/Notlar.xlsx
+++ b/AdvancedJava/_docs/Notlar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vize" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
   <si>
     <t>Adı</t>
   </si>
@@ -822,7 +822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -897,9 +897,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -951,6 +948,15 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1466,9 +1472,9 @@
   </sheetPr>
   <dimension ref="A1:X76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R16" sqref="R16"/>
+      <selection pane="bottomLeft" activeCell="W3" sqref="W3:W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1484,7 @@
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.44140625" style="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.44140625" style="52" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.44140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -1500,39 +1506,39 @@
       <c r="A1" s="30"/>
       <c r="B1" s="18"/>
       <c r="C1" s="29"/>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="46">
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="45">
         <v>6</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="M1" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="45">
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="44">
         <v>3</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="S1" s="73"/>
-      <c r="T1" s="45">
+      <c r="S1" s="77"/>
+      <c r="T1" s="44">
         <v>2</v>
       </c>
       <c r="U1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="41" t="s">
+      <c r="V1" s="40" t="s">
         <v>42</v>
       </c>
       <c r="W1" s="19" t="s">
@@ -1561,7 +1567,7 @@
       <c r="G2" s="27">
         <v>4</v>
       </c>
-      <c r="H2" s="50">
+      <c r="H2" s="49">
         <v>5</v>
       </c>
       <c r="I2" s="27">
@@ -1603,7 +1609,7 @@
       <c r="U2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="V2" s="43" t="s">
+      <c r="V2" s="42" t="s">
         <v>41</v>
       </c>
       <c r="W2" s="19" t="s">
@@ -1632,7 +1638,7 @@
       <c r="G3" s="7">
         <v>2</v>
       </c>
-      <c r="H3" s="51">
+      <c r="H3" s="50">
         <v>2</v>
       </c>
       <c r="I3" s="7">
@@ -1641,11 +1647,11 @@
       <c r="J3" s="7">
         <v>2</v>
       </c>
-      <c r="K3" s="48">
+      <c r="K3" s="47">
         <v>0</v>
       </c>
       <c r="L3" s="16">
-        <f>SUM(D3:J3)*50/(L$1-K3)</f>
+        <f t="shared" ref="L3:L30" si="0">SUM(D3:J3)*50/(L$1-K3)</f>
         <v>116.66666666666667</v>
       </c>
       <c r="M3" s="14">
@@ -1657,11 +1663,11 @@
       <c r="O3" s="6">
         <v>100</v>
       </c>
-      <c r="P3" s="48">
+      <c r="P3" s="47">
         <v>0</v>
       </c>
       <c r="Q3" s="16">
-        <f>SUM(M3:O3)/(Q$1-P3)</f>
+        <f t="shared" ref="Q3:Q30" si="1">SUM(M3:O3)/(Q$1-P3)</f>
         <v>100</v>
       </c>
       <c r="R3" s="14">
@@ -1671,16 +1677,15 @@
         <v>100</v>
       </c>
       <c r="T3" s="16">
-        <f>SUM(R3:S3)/T$1</f>
+        <f t="shared" ref="T3:T30" si="2">SUM(R3:S3)/T$1</f>
         <v>100</v>
       </c>
       <c r="U3" s="6">
-        <v>60</v>
-      </c>
-      <c r="V3" s="44"/>
+        <v>100</v>
+      </c>
+      <c r="V3" s="43"/>
       <c r="W3" s="21">
-        <f>L3*0.2+Q3*0.25+T3*0.25+U3*0.3+V3*0.15</f>
-        <v>91.333333333333343</v>
+        <v>100</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>37</v>
@@ -1708,7 +1713,7 @@
       <c r="G4" s="7">
         <v>2</v>
       </c>
-      <c r="H4" s="51">
+      <c r="H4" s="50">
         <v>2</v>
       </c>
       <c r="I4" s="7">
@@ -1717,11 +1722,11 @@
       <c r="J4" s="7">
         <v>2</v>
       </c>
-      <c r="K4" s="48">
+      <c r="K4" s="47">
         <v>0</v>
       </c>
       <c r="L4" s="16">
-        <f>SUM(D4:J4)*50/(L$1-K4)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="M4" s="14">
@@ -1733,11 +1738,11 @@
       <c r="O4" s="6">
         <v>90</v>
       </c>
-      <c r="P4" s="48">
+      <c r="P4" s="47">
         <v>0</v>
       </c>
       <c r="Q4" s="16">
-        <f>SUM(M4:O4)/(Q$1-P4)</f>
+        <f t="shared" si="1"/>
         <v>93.333333333333329</v>
       </c>
       <c r="R4" s="14">
@@ -1747,27 +1752,27 @@
         <v>80</v>
       </c>
       <c r="T4" s="16">
-        <f>SUM(R4:S4)/T$1</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="U4" s="6">
-        <v>60</v>
-      </c>
-      <c r="V4" s="44"/>
+        <v>80</v>
+      </c>
+      <c r="V4" s="43"/>
       <c r="W4" s="21">
         <f>L4*0.2+Q4*0.25+T4*0.25+U4*0.3+V4*0.1</f>
-        <v>81.333333333333329</v>
+        <v>87.333333333333329</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="D5" s="12">
         <v>0</v>
@@ -1781,8 +1786,8 @@
       <c r="G5" s="7">
         <v>2</v>
       </c>
-      <c r="H5" s="51">
-        <v>2</v>
+      <c r="H5" s="50">
+        <v>1.7</v>
       </c>
       <c r="I5" s="7">
         <v>2</v>
@@ -1790,130 +1795,130 @@
       <c r="J5" s="7">
         <v>2</v>
       </c>
-      <c r="K5" s="48">
+      <c r="K5" s="47">
         <v>0</v>
       </c>
       <c r="L5" s="16">
-        <f>SUM(D5:J5)*50/(L$1-K5)</f>
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>97.5</v>
       </c>
       <c r="M5" s="14">
         <v>90</v>
       </c>
       <c r="N5" s="6">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="O5" s="6">
-        <v>80</v>
-      </c>
-      <c r="P5" s="48">
+        <v>50</v>
+      </c>
+      <c r="P5" s="47">
         <v>0</v>
       </c>
       <c r="Q5" s="16">
-        <f>SUM(M5:O5)/(Q$1-P5)</f>
-        <v>83.333333333333329</v>
+        <f t="shared" si="1"/>
+        <v>75</v>
       </c>
       <c r="R5" s="14">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="S5" s="14">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="T5" s="16">
-        <f>SUM(R5:S5)/T$1</f>
-        <v>52.5</v>
+        <f t="shared" si="2"/>
+        <v>40</v>
       </c>
       <c r="U5" s="6">
-        <v>60</v>
-      </c>
-      <c r="V5" s="44"/>
+        <v>66</v>
+      </c>
+      <c r="V5" s="43"/>
       <c r="W5" s="21">
-        <f>L5*0.2+Q5*0.25+T5*0.25+U5*0.3+V5*0.15</f>
-        <v>71.958333333333329</v>
+        <f t="shared" ref="W5:W14" si="3">L5*0.2+Q5*0.25+T5*0.25+U5*0.3+V5*0.15</f>
+        <v>68.05</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7">
+        <v>2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
+      <c r="H6" s="50">
+        <v>2</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>2</v>
+      </c>
+      <c r="K6" s="47">
+        <v>0</v>
+      </c>
+      <c r="L6" s="16">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="M6" s="14">
+        <v>95</v>
+      </c>
+      <c r="N6" s="6">
+        <v>100</v>
+      </c>
+      <c r="O6" s="6">
+        <v>90</v>
+      </c>
+      <c r="P6" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="16">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="R6" s="14">
+        <v>30</v>
+      </c>
+      <c r="S6" s="14">
+        <v>2</v>
+      </c>
+      <c r="T6" s="16">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="U6" s="6">
         <v>53</v>
       </c>
-      <c r="D6" s="12">
-        <v>2</v>
-      </c>
-      <c r="E6" s="7">
-        <v>2</v>
-      </c>
-      <c r="F6" s="7">
-        <v>2</v>
-      </c>
-      <c r="G6" s="7">
-        <v>2</v>
-      </c>
-      <c r="H6" s="51">
-        <v>2</v>
-      </c>
-      <c r="I6" s="7">
-        <v>2</v>
-      </c>
-      <c r="J6" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="K6" s="48">
-        <v>0</v>
-      </c>
-      <c r="L6" s="16">
-        <f>SUM(D6:J6)*50/(L$1-K6)</f>
-        <v>115</v>
-      </c>
-      <c r="M6" s="14">
-        <v>85</v>
-      </c>
-      <c r="N6" s="6">
-        <v>90</v>
-      </c>
-      <c r="O6" s="6">
-        <v>50</v>
-      </c>
-      <c r="P6" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="16">
-        <f>SUM(M6:O6)/(Q$1-P6)</f>
-        <v>75</v>
-      </c>
-      <c r="R6" s="14">
-        <v>20</v>
-      </c>
-      <c r="S6" s="14">
-        <v>65</v>
-      </c>
-      <c r="T6" s="16">
-        <f>SUM(R6:S6)/T$1</f>
-        <v>42.5</v>
-      </c>
-      <c r="U6" s="6">
-        <v>60</v>
-      </c>
-      <c r="V6" s="44"/>
+      <c r="V6" s="43"/>
       <c r="W6" s="21">
-        <f>L6*0.2+Q6*0.25+T6*0.25+U6*0.3+V6*0.15</f>
-        <v>70.375</v>
+        <f t="shared" si="3"/>
+        <v>63.65</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="D7" s="12">
         <v>2</v>
@@ -1927,97 +1932,97 @@
       <c r="G7" s="7">
         <v>2</v>
       </c>
-      <c r="H7" s="51">
+      <c r="H7" s="50">
         <v>2</v>
       </c>
       <c r="I7" s="7">
         <v>2</v>
       </c>
       <c r="J7" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="K7" s="48">
+        <v>2</v>
+      </c>
+      <c r="K7" s="47">
         <v>0</v>
       </c>
       <c r="L7" s="16">
-        <f>SUM(D7:J7)*50/(L$1-K7)</f>
-        <v>115</v>
+        <f t="shared" si="0"/>
+        <v>116.66666666666667</v>
       </c>
       <c r="M7" s="14">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="N7" s="6">
+        <v>100</v>
+      </c>
+      <c r="O7" s="6">
         <v>90</v>
       </c>
-      <c r="O7" s="6">
-        <v>60</v>
-      </c>
-      <c r="P7" s="48">
+      <c r="P7" s="47">
         <v>0</v>
       </c>
       <c r="Q7" s="16">
-        <f>SUM(M7:O7)/(Q$1-P7)</f>
-        <v>76.666666666666671</v>
+        <f t="shared" si="1"/>
+        <v>95</v>
       </c>
       <c r="R7" s="14">
         <v>40</v>
       </c>
       <c r="S7" s="14">
-        <v>30</v>
+        <v>-25</v>
       </c>
       <c r="T7" s="16">
-        <f>SUM(R7:S7)/T$1</f>
-        <v>35</v>
+        <f t="shared" si="2"/>
+        <v>7.5</v>
       </c>
       <c r="U7" s="6">
-        <v>60</v>
-      </c>
-      <c r="V7" s="44"/>
+        <v>42</v>
+      </c>
+      <c r="V7" s="43"/>
       <c r="W7" s="21">
-        <f>L7*0.2+Q7*0.25+T7*0.25+U7*0.3+V7*0.15</f>
-        <v>68.916666666666671</v>
+        <f t="shared" si="3"/>
+        <v>61.558333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D8" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" s="7">
         <v>2</v>
       </c>
       <c r="F8" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="7">
         <v>2</v>
       </c>
-      <c r="H8" s="51">
+      <c r="H8" s="50">
         <v>2</v>
       </c>
       <c r="I8" s="7">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="J8" s="7">
         <v>2</v>
       </c>
-      <c r="K8" s="48">
+      <c r="K8" s="47">
         <v>0</v>
       </c>
       <c r="L8" s="16">
-        <f>SUM(D8:J8)*50/(L$1-K8)</f>
-        <v>116.66666666666667</v>
+        <f t="shared" si="0"/>
+        <v>81.666666666666671</v>
       </c>
       <c r="M8" s="14">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N8" s="6">
         <v>100</v>
@@ -2025,41 +2030,41 @@
       <c r="O8" s="6">
         <v>90</v>
       </c>
-      <c r="P8" s="48">
+      <c r="P8" s="47">
         <v>0</v>
       </c>
       <c r="Q8" s="16">
-        <f>SUM(M8:O8)/(Q$1-P8)</f>
-        <v>95</v>
+        <f t="shared" si="1"/>
+        <v>93.333333333333329</v>
       </c>
       <c r="R8" s="14">
+        <v>10</v>
+      </c>
+      <c r="S8" s="14">
+        <v>61</v>
+      </c>
+      <c r="T8" s="16">
+        <f t="shared" si="2"/>
+        <v>35.5</v>
+      </c>
+      <c r="U8" s="6">
         <v>40</v>
       </c>
-      <c r="S8" s="14">
-        <v>-25</v>
-      </c>
-      <c r="T8" s="16">
-        <f>SUM(R8:S8)/T$1</f>
-        <v>7.5</v>
-      </c>
-      <c r="U8" s="6">
-        <v>60</v>
-      </c>
-      <c r="V8" s="44"/>
+      <c r="V8" s="43"/>
       <c r="W8" s="21">
-        <f>L8*0.2+Q8*0.25+T8*0.25+U8*0.3+V8*0.15</f>
-        <v>66.958333333333343</v>
+        <f t="shared" si="3"/>
+        <v>60.541666666666671</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D9" s="12">
         <v>0</v>
@@ -2068,71 +2073,71 @@
         <v>2</v>
       </c>
       <c r="F9" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="7">
         <v>2</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H9" s="50">
         <v>2</v>
       </c>
       <c r="I9" s="7">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="J9" s="7">
         <v>2</v>
       </c>
-      <c r="K9" s="48">
+      <c r="K9" s="47">
         <v>0</v>
       </c>
       <c r="L9" s="16">
-        <f>SUM(D9:J9)*50/(L$1-K9)</f>
-        <v>81.666666666666671</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="M9" s="14">
         <v>90</v>
       </c>
       <c r="N9" s="6">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="O9" s="6">
-        <v>90</v>
-      </c>
-      <c r="P9" s="48">
+        <v>80</v>
+      </c>
+      <c r="P9" s="47">
         <v>0</v>
       </c>
       <c r="Q9" s="16">
-        <f>SUM(M9:O9)/(Q$1-P9)</f>
-        <v>93.333333333333329</v>
+        <f t="shared" si="1"/>
+        <v>83.333333333333329</v>
       </c>
       <c r="R9" s="14">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="S9" s="14">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="T9" s="16">
-        <f>SUM(R9:S9)/T$1</f>
-        <v>35.5</v>
+        <f t="shared" si="2"/>
+        <v>52.5</v>
       </c>
       <c r="U9" s="6">
-        <v>60</v>
-      </c>
-      <c r="V9" s="44"/>
+        <v>16</v>
+      </c>
+      <c r="V9" s="43"/>
       <c r="W9" s="21">
-        <f>L9*0.2+Q9*0.25+T9*0.25+U9*0.3+V9*0.15</f>
-        <v>66.541666666666671</v>
+        <f t="shared" si="3"/>
+        <v>58.758333333333326</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D10" s="12">
         <v>0</v>
@@ -2146,8 +2151,8 @@
       <c r="G10" s="7">
         <v>2</v>
       </c>
-      <c r="H10" s="51">
-        <v>1.7</v>
+      <c r="H10" s="50">
+        <v>2</v>
       </c>
       <c r="I10" s="7">
         <v>2</v>
@@ -2155,60 +2160,60 @@
       <c r="J10" s="7">
         <v>2</v>
       </c>
-      <c r="K10" s="48">
+      <c r="K10" s="47">
         <v>0</v>
       </c>
       <c r="L10" s="16">
-        <f>SUM(D10:J10)*50/(L$1-K10)</f>
-        <v>97.5</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="M10" s="14">
         <v>90</v>
       </c>
       <c r="N10" s="6">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="O10" s="6">
-        <v>50</v>
-      </c>
-      <c r="P10" s="48">
+        <v>90</v>
+      </c>
+      <c r="P10" s="47">
         <v>0</v>
       </c>
       <c r="Q10" s="16">
-        <f>SUM(M10:O10)/(Q$1-P10)</f>
-        <v>75</v>
+        <f t="shared" si="1"/>
+        <v>93.333333333333329</v>
       </c>
       <c r="R10" s="14">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="S10" s="14">
-        <v>50</v>
+        <v>-25</v>
       </c>
       <c r="T10" s="16">
-        <f>SUM(R10:S10)/T$1</f>
-        <v>40</v>
+        <f t="shared" si="2"/>
+        <v>7.5</v>
       </c>
       <c r="U10" s="6">
-        <v>60</v>
-      </c>
-      <c r="V10" s="44"/>
+        <v>42</v>
+      </c>
+      <c r="V10" s="43"/>
       <c r="W10" s="21">
-        <f>L10*0.2+Q10*0.25+T10*0.25+U10*0.3+V10*0.15</f>
-        <v>66.25</v>
+        <f t="shared" si="3"/>
+        <v>57.80833333333333</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D11" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" s="7">
         <v>2</v>
@@ -2219,69 +2224,69 @@
       <c r="G11" s="7">
         <v>2</v>
       </c>
-      <c r="H11" s="51">
+      <c r="H11" s="50">
         <v>2</v>
       </c>
       <c r="I11" s="7">
         <v>2</v>
       </c>
       <c r="J11" s="7">
-        <v>2</v>
-      </c>
-      <c r="K11" s="48">
+        <v>1.8</v>
+      </c>
+      <c r="K11" s="47">
         <v>0</v>
       </c>
       <c r="L11" s="16">
-        <f>SUM(D11:J11)*50/(L$1-K11)</f>
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>115</v>
       </c>
       <c r="M11" s="14">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="N11" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="O11" s="6">
-        <v>90</v>
-      </c>
-      <c r="P11" s="48">
+        <v>60</v>
+      </c>
+      <c r="P11" s="47">
         <v>0</v>
       </c>
       <c r="Q11" s="16">
-        <f>SUM(M11:O11)/(Q$1-P11)</f>
-        <v>95</v>
+        <f t="shared" si="1"/>
+        <v>76.666666666666671</v>
       </c>
       <c r="R11" s="14">
+        <v>40</v>
+      </c>
+      <c r="S11" s="14">
         <v>30</v>
       </c>
-      <c r="S11" s="14">
-        <v>2</v>
-      </c>
       <c r="T11" s="16">
-        <f>SUM(R11:S11)/T$1</f>
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>35</v>
       </c>
       <c r="U11" s="6">
-        <v>60</v>
-      </c>
-      <c r="V11" s="44"/>
+        <v>15</v>
+      </c>
+      <c r="V11" s="43"/>
       <c r="W11" s="21">
-        <f>L11*0.2+Q11*0.25+T11*0.25+U11*0.3+V11*0.15</f>
-        <v>65.75</v>
+        <f t="shared" si="3"/>
+        <v>55.416666666666671</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D12" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="7">
         <v>2</v>
@@ -2292,55 +2297,55 @@
       <c r="G12" s="7">
         <v>2</v>
       </c>
-      <c r="H12" s="51">
+      <c r="H12" s="50">
         <v>2</v>
       </c>
       <c r="I12" s="7">
         <v>2</v>
       </c>
       <c r="J12" s="7">
-        <v>2</v>
-      </c>
-      <c r="K12" s="48">
+        <v>1.8</v>
+      </c>
+      <c r="K12" s="47">
         <v>0</v>
       </c>
       <c r="L12" s="16">
-        <f>SUM(D12:J12)*50/(L$1-K12)</f>
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>115</v>
       </c>
       <c r="M12" s="14">
+        <v>85</v>
+      </c>
+      <c r="N12" s="6">
         <v>90</v>
       </c>
-      <c r="N12" s="6">
-        <v>100</v>
-      </c>
       <c r="O12" s="6">
-        <v>90</v>
-      </c>
-      <c r="P12" s="48">
+        <v>50</v>
+      </c>
+      <c r="P12" s="47">
         <v>0</v>
       </c>
       <c r="Q12" s="16">
-        <f>SUM(M12:O12)/(Q$1-P12)</f>
-        <v>93.333333333333329</v>
+        <f t="shared" si="1"/>
+        <v>75</v>
       </c>
       <c r="R12" s="14">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="S12" s="14">
-        <v>-25</v>
+        <v>65</v>
       </c>
       <c r="T12" s="16">
-        <f>SUM(R12:S12)/T$1</f>
-        <v>7.5</v>
+        <f t="shared" si="2"/>
+        <v>42.5</v>
       </c>
       <c r="U12" s="6">
-        <v>60</v>
-      </c>
-      <c r="V12" s="44"/>
+        <v>5</v>
+      </c>
+      <c r="V12" s="43"/>
       <c r="W12" s="21">
-        <f>L12*0.2+Q12*0.25+T12*0.25+U12*0.3+V12*0.15</f>
-        <v>63.208333333333329</v>
+        <f t="shared" si="3"/>
+        <v>53.875</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2365,7 +2370,7 @@
       <c r="G13" s="7">
         <v>1.8</v>
       </c>
-      <c r="H13" s="51">
+      <c r="H13" s="50">
         <v>2</v>
       </c>
       <c r="I13" s="7">
@@ -2374,11 +2379,11 @@
       <c r="J13" s="7">
         <v>2</v>
       </c>
-      <c r="K13" s="48">
+      <c r="K13" s="47">
         <v>0</v>
       </c>
       <c r="L13" s="16">
-        <f>SUM(D13:J13)*50/(L$1-K13)</f>
+        <f t="shared" si="0"/>
         <v>98.333333333333329</v>
       </c>
       <c r="M13" s="14">
@@ -2390,11 +2395,11 @@
       <c r="O13" s="6">
         <v>70</v>
       </c>
-      <c r="P13" s="48">
+      <c r="P13" s="47">
         <v>0</v>
       </c>
       <c r="Q13" s="16">
-        <f>SUM(M13:O13)/(Q$1-P13)</f>
+        <f t="shared" si="1"/>
         <v>86.666666666666671</v>
       </c>
       <c r="R13" s="14">
@@ -2404,173 +2409,173 @@
         <v>-25</v>
       </c>
       <c r="T13" s="16">
-        <f>SUM(R13:S13)/T$1</f>
+        <f t="shared" si="2"/>
         <v>-2.5</v>
       </c>
       <c r="U13" s="6">
-        <v>60</v>
-      </c>
-      <c r="V13" s="44"/>
+        <v>42</v>
+      </c>
+      <c r="V13" s="43"/>
       <c r="W13" s="21">
-        <f>L13*0.2+Q13*0.25+T13*0.25+U13*0.3+V13*0.15</f>
-        <v>58.708333333333336</v>
+        <f t="shared" si="3"/>
+        <v>53.308333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D14" s="12">
         <v>0</v>
       </c>
-      <c r="E14" s="51" t="s">
+      <c r="E14" s="7">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
+      <c r="G14" s="7">
+        <v>2</v>
+      </c>
+      <c r="H14" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="51" t="s">
+      <c r="I14" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="J14" s="7">
+        <v>2</v>
+      </c>
+      <c r="K14" s="48">
+        <v>1</v>
+      </c>
+      <c r="L14" s="16">
+        <f t="shared" si="0"/>
+        <v>98.000000000000014</v>
+      </c>
+      <c r="M14" s="14">
         <v>95</v>
       </c>
-      <c r="G14" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" s="51">
-        <v>0</v>
-      </c>
-      <c r="I14" s="7">
-        <v>2</v>
-      </c>
-      <c r="J14" s="7">
-        <v>2</v>
-      </c>
-      <c r="K14" s="48">
-        <v>3</v>
-      </c>
-      <c r="L14" s="16">
-        <f>SUM(D14:J14)*50/(L$1-K14)</f>
-        <v>66.666666666666671</v>
-      </c>
-      <c r="M14" s="55" t="s">
-        <v>95</v>
-      </c>
       <c r="N14" s="6">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="O14" s="6">
-        <v>50</v>
-      </c>
-      <c r="P14" s="48">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="P14" s="47">
+        <v>0</v>
       </c>
       <c r="Q14" s="16">
-        <f>SUM(M14:O14)/(Q$1-P14)</f>
-        <v>62.5</v>
+        <f t="shared" si="1"/>
+        <v>91.666666666666671</v>
       </c>
       <c r="R14" s="14">
-        <v>61</v>
+        <v>-25</v>
       </c>
       <c r="S14" s="14">
-        <v>20</v>
+        <v>-25</v>
       </c>
       <c r="T14" s="16">
-        <f>SUM(R14:S14)/T$1</f>
-        <v>40.5</v>
+        <f t="shared" si="2"/>
+        <v>-25</v>
       </c>
       <c r="U14" s="6">
-        <v>60</v>
-      </c>
-      <c r="V14" s="44"/>
+        <v>52</v>
+      </c>
+      <c r="V14" s="43"/>
       <c r="W14" s="21">
-        <f>L14*0.2+Q14*0.25+T14*0.25+U14*0.3+V14*0.1</f>
-        <v>57.083333333333336</v>
+        <f t="shared" si="3"/>
+        <v>51.866666666666674</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
       </c>
-      <c r="E15" s="7">
-        <v>2</v>
-      </c>
-      <c r="F15" s="7">
-        <v>2</v>
-      </c>
-      <c r="G15" s="7">
-        <v>2</v>
-      </c>
-      <c r="H15" s="51" t="s">
+      <c r="E15" s="50" t="s">
         <v>95</v>
       </c>
+      <c r="F15" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="50">
+        <v>0</v>
+      </c>
       <c r="I15" s="7">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="J15" s="7">
         <v>2</v>
       </c>
-      <c r="K15" s="49">
+      <c r="K15" s="47">
+        <v>3</v>
+      </c>
+      <c r="L15" s="16">
+        <f t="shared" si="0"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="M15" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="N15" s="6">
+        <v>75</v>
+      </c>
+      <c r="O15" s="6">
+        <v>50</v>
+      </c>
+      <c r="P15" s="47">
         <v>1</v>
       </c>
-      <c r="L15" s="16">
-        <f>SUM(D15:J15)*50/(L$1-K15)</f>
-        <v>98.000000000000014</v>
-      </c>
-      <c r="M15" s="14">
-        <v>95</v>
-      </c>
-      <c r="N15" s="6">
-        <v>100</v>
-      </c>
-      <c r="O15" s="6">
-        <v>80</v>
-      </c>
-      <c r="P15" s="48">
-        <v>0</v>
-      </c>
       <c r="Q15" s="16">
-        <f>SUM(M15:O15)/(Q$1-P15)</f>
-        <v>91.666666666666671</v>
+        <f t="shared" si="1"/>
+        <v>62.5</v>
       </c>
       <c r="R15" s="14">
-        <v>-25</v>
+        <v>61</v>
       </c>
       <c r="S15" s="14">
-        <v>-25</v>
+        <v>20</v>
       </c>
       <c r="T15" s="16">
-        <f>SUM(R15:S15)/T$1</f>
-        <v>-25</v>
+        <f t="shared" si="2"/>
+        <v>40.5</v>
       </c>
       <c r="U15" s="6">
-        <v>60</v>
-      </c>
-      <c r="V15" s="44"/>
+        <v>0</v>
+      </c>
+      <c r="V15" s="43"/>
       <c r="W15" s="21">
-        <f>L15*0.2+Q15*0.25+T15*0.25+U15*0.3+V15*0.15</f>
-        <v>54.266666666666673</v>
+        <f>L15*0.2+Q15*0.25+T15*0.25+U15*0.3+V15*0.1</f>
+        <v>39.083333333333336</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="D16" s="12">
         <v>0</v>
@@ -2584,66 +2589,66 @@
       <c r="G16" s="7">
         <v>2</v>
       </c>
-      <c r="H16" s="51">
-        <v>2</v>
+      <c r="H16" s="50">
+        <v>0</v>
       </c>
       <c r="I16" s="7">
         <v>2</v>
       </c>
       <c r="J16" s="7">
-        <v>2</v>
-      </c>
-      <c r="K16" s="48">
+        <v>0</v>
+      </c>
+      <c r="K16" s="47">
         <v>0</v>
       </c>
       <c r="L16" s="16">
-        <f>SUM(D16:J16)*50/(L$1-K16)</f>
-        <v>100</v>
+        <f t="shared" si="0"/>
+        <v>66.666666666666671</v>
       </c>
       <c r="M16" s="14">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="N16" s="6">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O16" s="6">
-        <v>80</v>
-      </c>
-      <c r="P16" s="48">
+        <v>0</v>
+      </c>
+      <c r="P16" s="47">
         <v>0</v>
       </c>
       <c r="Q16" s="16">
-        <f>SUM(M16:O16)/(Q$1-P16)</f>
-        <v>90</v>
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
       <c r="R16" s="14">
-        <v>-25</v>
+        <v>1</v>
       </c>
       <c r="S16" s="14">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="T16" s="16">
-        <f>SUM(R16:S16)/T$1</f>
-        <v>-25</v>
+        <f t="shared" si="2"/>
+        <v>0.5</v>
       </c>
       <c r="U16" s="6">
-        <v>60</v>
-      </c>
-      <c r="V16" s="44"/>
+        <v>31</v>
+      </c>
+      <c r="V16" s="43"/>
       <c r="W16" s="21">
         <f>L16*0.2+Q16*0.25+T16*0.25+U16*0.3+V16*0.15</f>
-        <v>54.25</v>
+        <v>37.758333333333333</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="D17" s="12">
         <v>0</v>
@@ -2657,205 +2662,206 @@
       <c r="G17" s="7">
         <v>2</v>
       </c>
-      <c r="H17" s="51">
-        <v>0</v>
+      <c r="H17" s="50">
+        <v>2</v>
       </c>
       <c r="I17" s="7">
         <v>2</v>
       </c>
       <c r="J17" s="7">
-        <v>0</v>
-      </c>
-      <c r="K17" s="48">
+        <v>2</v>
+      </c>
+      <c r="K17" s="47">
         <v>0</v>
       </c>
       <c r="L17" s="16">
-        <f>SUM(D17:J17)*50/(L$1-K17)</f>
-        <v>66.666666666666671</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="M17" s="14">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N17" s="6">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="O17" s="6">
-        <v>0</v>
-      </c>
-      <c r="P17" s="48">
+        <v>80</v>
+      </c>
+      <c r="P17" s="47">
         <v>0</v>
       </c>
       <c r="Q17" s="16">
-        <f>SUM(M17:O17)/(Q$1-P17)</f>
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>90</v>
       </c>
       <c r="R17" s="14">
-        <v>1</v>
+        <v>-25</v>
       </c>
       <c r="S17" s="14">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="T17" s="16">
-        <f>SUM(R17:S17)/T$1</f>
-        <v>0.5</v>
+        <f t="shared" si="2"/>
+        <v>-25</v>
       </c>
       <c r="U17" s="6">
-        <v>60</v>
-      </c>
-      <c r="V17" s="44"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="43"/>
       <c r="W17" s="21">
         <f>L17*0.2+Q17*0.25+T17*0.25+U17*0.3+V17*0.15</f>
-        <v>46.458333333333336</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" s="47" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" s="46" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="D18" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="12">
         <v>0</v>
       </c>
-      <c r="H18" s="51">
-        <v>0</v>
+      <c r="H18" s="50">
+        <v>2</v>
       </c>
       <c r="I18" s="7">
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="J18" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="K18" s="48">
+        <v>0</v>
+      </c>
+      <c r="K18" s="47">
         <v>0</v>
       </c>
       <c r="L18" s="16">
-        <f>SUM(D18:J18)*50/(L$1-K18)</f>
-        <v>11.666666666666666</v>
+        <f t="shared" si="0"/>
+        <v>83.333333333333329</v>
       </c>
       <c r="M18" s="14">
         <v>0</v>
       </c>
       <c r="N18" s="6">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="O18" s="6">
-        <v>80</v>
-      </c>
-      <c r="P18" s="48">
+        <v>0</v>
+      </c>
+      <c r="P18" s="47">
         <v>0</v>
       </c>
       <c r="Q18" s="16">
-        <f>SUM(M18:O18)/(Q$1-P18)</f>
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>33.333333333333336</v>
       </c>
       <c r="R18" s="14">
-        <v>40</v>
+        <v>-25</v>
       </c>
       <c r="S18" s="14">
-        <v>61</v>
+        <v>-25</v>
       </c>
       <c r="T18" s="16">
-        <f>SUM(R18:S18)/T$1</f>
-        <v>50.5</v>
+        <f t="shared" si="2"/>
+        <v>-25</v>
       </c>
       <c r="U18" s="6">
-        <v>60</v>
-      </c>
-      <c r="V18" s="44"/>
+        <v>45</v>
+      </c>
+      <c r="V18" s="43"/>
       <c r="W18" s="21">
-        <f>L18*0.2+Q18*0.25+T18*0.25+U18*0.3+V18*0.1</f>
-        <v>42.958333333333336</v>
-      </c>
-      <c r="X18" s="9"/>
+        <f>L18*0.2+Q18*0.25+T18*0.25+U18*0.3+V18*0.15</f>
+        <v>32.25</v>
+      </c>
+      <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="D19" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E19" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G19" s="12">
         <v>0</v>
       </c>
-      <c r="H19" s="51">
-        <v>2</v>
+      <c r="H19" s="50">
+        <v>0</v>
       </c>
       <c r="I19" s="7">
-        <v>2</v>
+        <v>0.9</v>
       </c>
       <c r="J19" s="7">
-        <v>0</v>
-      </c>
-      <c r="K19" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="K19" s="47">
         <v>0</v>
       </c>
       <c r="L19" s="16">
-        <f>SUM(D19:J19)*50/(L$1-K19)</f>
-        <v>83.333333333333329</v>
+        <f t="shared" si="0"/>
+        <v>11.666666666666666</v>
       </c>
       <c r="M19" s="14">
         <v>0</v>
       </c>
       <c r="N19" s="6">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="O19" s="6">
-        <v>0</v>
-      </c>
-      <c r="P19" s="48">
+        <v>80</v>
+      </c>
+      <c r="P19" s="47">
         <v>0</v>
       </c>
       <c r="Q19" s="16">
-        <f>SUM(M19:O19)/(Q$1-P19)</f>
-        <v>33.333333333333336</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="R19" s="14">
-        <v>-25</v>
+        <v>40</v>
       </c>
       <c r="S19" s="14">
-        <v>-25</v>
+        <v>61</v>
       </c>
       <c r="T19" s="16">
-        <f>SUM(R19:S19)/T$1</f>
-        <v>-25</v>
+        <f t="shared" si="2"/>
+        <v>50.5</v>
       </c>
       <c r="U19" s="6">
-        <v>60</v>
-      </c>
-      <c r="V19" s="44"/>
+        <v>2</v>
+      </c>
+      <c r="V19" s="43"/>
       <c r="W19" s="21">
-        <f>L19*0.2+Q19*0.25+T19*0.25+U19*0.3+V19*0.15</f>
-        <v>36.75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" s="47" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+        <f>L19*0.2+Q19*0.25+T19*0.25+U19*0.3+V19*0.1</f>
+        <v>25.558333333333337</v>
+      </c>
+      <c r="X19" s="9"/>
+    </row>
+    <row r="20" spans="1:24" s="46" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>85</v>
       </c>
@@ -2868,7 +2874,7 @@
       <c r="D20" s="12">
         <v>0</v>
       </c>
-      <c r="E20" s="54" t="s">
+      <c r="E20" s="53" t="s">
         <v>95</v>
       </c>
       <c r="F20" s="12">
@@ -2877,7 +2883,7 @@
       <c r="G20" s="12">
         <v>0</v>
       </c>
-      <c r="H20" s="51">
+      <c r="H20" s="50">
         <v>0</v>
       </c>
       <c r="I20" s="7">
@@ -2886,11 +2892,11 @@
       <c r="J20" s="7">
         <v>2</v>
       </c>
-      <c r="K20" s="48">
+      <c r="K20" s="47">
         <v>1</v>
       </c>
       <c r="L20" s="16">
-        <f>SUM(D20:J20)*50/(L$1-K20)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="M20" s="14">
@@ -2902,11 +2908,11 @@
       <c r="O20" s="6">
         <v>20</v>
       </c>
-      <c r="P20" s="48">
+      <c r="P20" s="47">
         <v>0</v>
       </c>
       <c r="Q20" s="16">
-        <f>SUM(M20:O20)/(Q$1-P20)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="R20" s="14">
@@ -2916,16 +2922,16 @@
         <v>0</v>
       </c>
       <c r="T20" s="16">
-        <f>SUM(R20:S20)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U20" s="6">
-        <v>60</v>
-      </c>
-      <c r="V20" s="44"/>
+        <v>1</v>
+      </c>
+      <c r="V20" s="43"/>
       <c r="W20" s="21">
         <f>L20*0.2+Q20*0.25+T20*0.25+U20*0.3+V20*0.1</f>
-        <v>30.2</v>
+        <v>12.5</v>
       </c>
       <c r="X20" s="1"/>
     </row>
@@ -2951,7 +2957,7 @@
       <c r="G21" s="12">
         <v>0</v>
       </c>
-      <c r="H21" s="51">
+      <c r="H21" s="50">
         <v>2</v>
       </c>
       <c r="I21" s="7">
@@ -2960,11 +2966,11 @@
       <c r="J21" s="7">
         <v>0</v>
       </c>
-      <c r="K21" s="48">
+      <c r="K21" s="47">
         <v>0</v>
       </c>
       <c r="L21" s="16">
-        <f>SUM(D21:J21)*50/(L$1-K21)</f>
+        <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
       <c r="M21" s="14">
@@ -2976,11 +2982,11 @@
       <c r="O21" s="6">
         <v>0</v>
       </c>
-      <c r="P21" s="48">
+      <c r="P21" s="47">
         <v>0</v>
       </c>
       <c r="Q21" s="16">
-        <f>SUM(M21:O21)/(Q$1-P21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R21" s="14">
@@ -2990,657 +2996,675 @@
         <v>25</v>
       </c>
       <c r="T21" s="16">
-        <f>SUM(R21:S21)/T$1</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="U21" s="6">
-        <v>60</v>
-      </c>
-      <c r="V21" s="44"/>
+        <v>0</v>
+      </c>
+      <c r="V21" s="43"/>
       <c r="W21" s="21">
-        <f>L21*0.2+Q21*0.25+T21*0.25+U21*0.3+V21*0.15</f>
-        <v>27.583333333333336</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="56" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="57" t="s">
+        <f t="shared" ref="W21:W29" si="4">L21*0.2+Q21*0.25+T21*0.25+U21*0.3+V21*0.15</f>
+        <v>9.5833333333333339</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" s="67" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="59">
-        <v>0</v>
-      </c>
-      <c r="E22" s="59">
-        <v>0</v>
-      </c>
-      <c r="F22" s="59">
-        <v>0</v>
-      </c>
-      <c r="G22" s="59">
-        <v>0</v>
-      </c>
-      <c r="H22" s="60">
-        <v>0</v>
-      </c>
-      <c r="I22" s="61">
-        <v>0</v>
-      </c>
-      <c r="J22" s="61">
-        <v>0</v>
-      </c>
-      <c r="K22" s="62">
-        <v>0</v>
-      </c>
-      <c r="L22" s="63">
-        <f>SUM(D22:J22)*50/(L$1-K22)</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="64">
-        <v>0</v>
-      </c>
-      <c r="N22" s="65">
-        <v>0</v>
-      </c>
-      <c r="O22" s="65">
-        <v>0</v>
-      </c>
-      <c r="P22" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="63">
-        <f>SUM(M22:O22)/(Q$1-P22)</f>
-        <v>0</v>
-      </c>
-      <c r="R22" s="64">
-        <v>0</v>
-      </c>
-      <c r="S22" s="64">
-        <v>0</v>
-      </c>
-      <c r="T22" s="63">
-        <f>SUM(R22:S22)/T$1</f>
-        <v>0</v>
-      </c>
-      <c r="U22" s="65"/>
-      <c r="V22" s="66"/>
-      <c r="W22" s="67">
-        <f>L22*0.2+Q22*0.25+T22*0.25+U22*0.3+V22*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+      <c r="D22" s="58">
+        <v>0</v>
+      </c>
+      <c r="E22" s="58">
+        <v>0</v>
+      </c>
+      <c r="F22" s="58">
+        <v>0</v>
+      </c>
+      <c r="G22" s="58">
+        <v>0</v>
+      </c>
+      <c r="H22" s="59">
+        <v>0</v>
+      </c>
+      <c r="I22" s="60">
+        <v>0</v>
+      </c>
+      <c r="J22" s="60">
+        <v>0</v>
+      </c>
+      <c r="K22" s="61">
+        <v>0</v>
+      </c>
+      <c r="L22" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="63">
+        <v>0</v>
+      </c>
+      <c r="N22" s="64">
+        <v>0</v>
+      </c>
+      <c r="O22" s="64">
+        <v>0</v>
+      </c>
+      <c r="P22" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="63">
+        <v>0</v>
+      </c>
+      <c r="S22" s="63">
+        <v>0</v>
+      </c>
+      <c r="T22" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="64">
+        <v>0</v>
+      </c>
+      <c r="V22" s="65"/>
+      <c r="W22" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" s="67" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="57" t="s">
+      <c r="B23" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="58" t="s">
+      <c r="C23" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="59">
-        <v>0</v>
-      </c>
-      <c r="E23" s="59">
-        <v>0</v>
-      </c>
-      <c r="F23" s="59">
-        <v>0</v>
-      </c>
-      <c r="G23" s="59">
-        <v>0</v>
-      </c>
-      <c r="H23" s="60">
-        <v>0</v>
-      </c>
-      <c r="I23" s="61">
-        <v>0</v>
-      </c>
-      <c r="J23" s="61">
-        <v>0</v>
-      </c>
-      <c r="K23" s="62">
-        <v>0</v>
-      </c>
-      <c r="L23" s="63">
-        <f>SUM(D23:J23)*50/(L$1-K23)</f>
-        <v>0</v>
-      </c>
-      <c r="M23" s="64">
-        <v>0</v>
-      </c>
-      <c r="N23" s="65">
-        <v>0</v>
-      </c>
-      <c r="O23" s="65">
-        <v>0</v>
-      </c>
-      <c r="P23" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="63">
-        <f>SUM(M23:O23)/(Q$1-P23)</f>
-        <v>0</v>
-      </c>
-      <c r="R23" s="64">
-        <v>0</v>
-      </c>
-      <c r="S23" s="64">
-        <v>0</v>
-      </c>
-      <c r="T23" s="63">
-        <f>SUM(R23:S23)/T$1</f>
-        <v>0</v>
-      </c>
-      <c r="U23" s="65"/>
-      <c r="V23" s="66"/>
-      <c r="W23" s="67">
-        <f>L23*0.2+Q23*0.25+T23*0.25+U23*0.3+V23*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
+      <c r="D23" s="58">
+        <v>0</v>
+      </c>
+      <c r="E23" s="58">
+        <v>0</v>
+      </c>
+      <c r="F23" s="58">
+        <v>0</v>
+      </c>
+      <c r="G23" s="58">
+        <v>0</v>
+      </c>
+      <c r="H23" s="59">
+        <v>0</v>
+      </c>
+      <c r="I23" s="60">
+        <v>0</v>
+      </c>
+      <c r="J23" s="60">
+        <v>0</v>
+      </c>
+      <c r="K23" s="61">
+        <v>0</v>
+      </c>
+      <c r="L23" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="63">
+        <v>0</v>
+      </c>
+      <c r="N23" s="64">
+        <v>0</v>
+      </c>
+      <c r="O23" s="64">
+        <v>0</v>
+      </c>
+      <c r="P23" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="63">
+        <v>0</v>
+      </c>
+      <c r="S23" s="63">
+        <v>0</v>
+      </c>
+      <c r="T23" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="64">
+        <v>0</v>
+      </c>
+      <c r="V23" s="65"/>
+      <c r="W23" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" s="67" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="59">
-        <v>0</v>
-      </c>
-      <c r="E24" s="59">
-        <v>0</v>
-      </c>
-      <c r="F24" s="59">
-        <v>0</v>
-      </c>
-      <c r="G24" s="59">
-        <v>0</v>
-      </c>
-      <c r="H24" s="60">
-        <v>0</v>
-      </c>
-      <c r="I24" s="61">
-        <v>0</v>
-      </c>
-      <c r="J24" s="61">
-        <v>0</v>
-      </c>
-      <c r="K24" s="62">
-        <v>0</v>
-      </c>
-      <c r="L24" s="63">
-        <f>SUM(D24:J24)*50/(L$1-K24)</f>
-        <v>0</v>
-      </c>
-      <c r="M24" s="64">
-        <v>0</v>
-      </c>
-      <c r="N24" s="65">
-        <v>0</v>
-      </c>
-      <c r="O24" s="65">
-        <v>0</v>
-      </c>
-      <c r="P24" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="63">
-        <f>SUM(M24:O24)/(Q$1-P24)</f>
-        <v>0</v>
-      </c>
-      <c r="R24" s="64">
-        <v>0</v>
-      </c>
-      <c r="S24" s="64">
-        <v>0</v>
-      </c>
-      <c r="T24" s="63">
-        <f>SUM(R24:S24)/T$1</f>
-        <v>0</v>
-      </c>
-      <c r="U24" s="65"/>
-      <c r="V24" s="66"/>
-      <c r="W24" s="67">
-        <f>L24*0.2+Q24*0.25+T24*0.25+U24*0.3+V24*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="D24" s="58">
+        <v>0</v>
+      </c>
+      <c r="E24" s="58">
+        <v>0</v>
+      </c>
+      <c r="F24" s="58">
+        <v>0</v>
+      </c>
+      <c r="G24" s="58">
+        <v>0</v>
+      </c>
+      <c r="H24" s="59">
+        <v>0</v>
+      </c>
+      <c r="I24" s="60">
+        <v>0</v>
+      </c>
+      <c r="J24" s="60">
+        <v>0</v>
+      </c>
+      <c r="K24" s="61">
+        <v>0</v>
+      </c>
+      <c r="L24" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="63">
+        <v>0</v>
+      </c>
+      <c r="N24" s="64">
+        <v>0</v>
+      </c>
+      <c r="O24" s="64">
+        <v>0</v>
+      </c>
+      <c r="P24" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="63">
+        <v>0</v>
+      </c>
+      <c r="S24" s="63">
+        <v>0</v>
+      </c>
+      <c r="T24" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="64">
+        <v>0</v>
+      </c>
+      <c r="V24" s="65"/>
+      <c r="W24" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" s="67" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="58" t="s">
+      <c r="C25" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="59">
-        <v>0</v>
-      </c>
-      <c r="E25" s="59">
-        <v>0</v>
-      </c>
-      <c r="F25" s="59">
-        <v>0</v>
-      </c>
-      <c r="G25" s="59">
-        <v>0</v>
-      </c>
-      <c r="H25" s="60">
-        <v>0</v>
-      </c>
-      <c r="I25" s="61">
-        <v>0</v>
-      </c>
-      <c r="J25" s="61">
-        <v>0</v>
-      </c>
-      <c r="K25" s="62">
-        <v>0</v>
-      </c>
-      <c r="L25" s="63">
-        <f>SUM(D25:J25)*50/(L$1-K25)</f>
-        <v>0</v>
-      </c>
-      <c r="M25" s="64">
-        <v>0</v>
-      </c>
-      <c r="N25" s="65">
-        <v>0</v>
-      </c>
-      <c r="O25" s="65">
-        <v>0</v>
-      </c>
-      <c r="P25" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="63">
-        <f>SUM(M25:O25)/(Q$1-P25)</f>
-        <v>0</v>
-      </c>
-      <c r="R25" s="64">
-        <v>0</v>
-      </c>
-      <c r="S25" s="64">
-        <v>0</v>
-      </c>
-      <c r="T25" s="63">
-        <f>SUM(R25:S25)/T$1</f>
-        <v>0</v>
-      </c>
-      <c r="U25" s="65"/>
-      <c r="V25" s="66"/>
-      <c r="W25" s="67">
-        <f>L25*0.2+Q25*0.25+T25*0.25+U25*0.3+V25*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="s">
+      <c r="D25" s="58">
+        <v>0</v>
+      </c>
+      <c r="E25" s="58">
+        <v>0</v>
+      </c>
+      <c r="F25" s="58">
+        <v>0</v>
+      </c>
+      <c r="G25" s="58">
+        <v>0</v>
+      </c>
+      <c r="H25" s="59">
+        <v>0</v>
+      </c>
+      <c r="I25" s="60">
+        <v>0</v>
+      </c>
+      <c r="J25" s="60">
+        <v>0</v>
+      </c>
+      <c r="K25" s="61">
+        <v>0</v>
+      </c>
+      <c r="L25" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="63">
+        <v>0</v>
+      </c>
+      <c r="N25" s="64">
+        <v>0</v>
+      </c>
+      <c r="O25" s="64">
+        <v>0</v>
+      </c>
+      <c r="P25" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="63">
+        <v>0</v>
+      </c>
+      <c r="S25" s="63">
+        <v>0</v>
+      </c>
+      <c r="T25" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="64">
+        <v>0</v>
+      </c>
+      <c r="V25" s="65"/>
+      <c r="W25" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" s="67" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="58" t="s">
+      <c r="C26" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="59">
-        <v>0</v>
-      </c>
-      <c r="E26" s="59">
-        <v>0</v>
-      </c>
-      <c r="F26" s="59">
-        <v>0</v>
-      </c>
-      <c r="G26" s="59">
-        <v>0</v>
-      </c>
-      <c r="H26" s="60">
-        <v>0</v>
-      </c>
-      <c r="I26" s="61">
-        <v>0</v>
-      </c>
-      <c r="J26" s="61">
-        <v>0</v>
-      </c>
-      <c r="K26" s="62">
-        <v>0</v>
-      </c>
-      <c r="L26" s="63">
-        <f>SUM(D26:J26)*50/(L$1-K26)</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="64">
-        <v>0</v>
-      </c>
-      <c r="N26" s="65">
-        <v>0</v>
-      </c>
-      <c r="O26" s="65">
-        <v>0</v>
-      </c>
-      <c r="P26" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="63">
-        <f>SUM(M26:O26)/(Q$1-P26)</f>
-        <v>0</v>
-      </c>
-      <c r="R26" s="64">
-        <v>0</v>
-      </c>
-      <c r="S26" s="64">
-        <v>0</v>
-      </c>
-      <c r="T26" s="63">
-        <f>SUM(R26:S26)/T$1</f>
-        <v>0</v>
-      </c>
-      <c r="U26" s="65"/>
-      <c r="V26" s="66"/>
-      <c r="W26" s="67">
-        <f>L26*0.2+Q26*0.25+T26*0.25+U26*0.3+V26*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="s">
+      <c r="D26" s="58">
+        <v>0</v>
+      </c>
+      <c r="E26" s="58">
+        <v>0</v>
+      </c>
+      <c r="F26" s="58">
+        <v>0</v>
+      </c>
+      <c r="G26" s="58">
+        <v>0</v>
+      </c>
+      <c r="H26" s="59">
+        <v>0</v>
+      </c>
+      <c r="I26" s="60">
+        <v>0</v>
+      </c>
+      <c r="J26" s="60">
+        <v>0</v>
+      </c>
+      <c r="K26" s="61">
+        <v>0</v>
+      </c>
+      <c r="L26" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="63">
+        <v>0</v>
+      </c>
+      <c r="N26" s="64">
+        <v>0</v>
+      </c>
+      <c r="O26" s="64">
+        <v>0</v>
+      </c>
+      <c r="P26" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="63">
+        <v>0</v>
+      </c>
+      <c r="S26" s="63">
+        <v>0</v>
+      </c>
+      <c r="T26" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U26" s="64">
+        <v>0</v>
+      </c>
+      <c r="V26" s="65"/>
+      <c r="W26" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" s="67" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="58" t="s">
+      <c r="C27" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="59">
-        <v>0</v>
-      </c>
-      <c r="E27" s="59">
-        <v>0</v>
-      </c>
-      <c r="F27" s="59">
-        <v>0</v>
-      </c>
-      <c r="G27" s="59">
-        <v>0</v>
-      </c>
-      <c r="H27" s="60">
-        <v>0</v>
-      </c>
-      <c r="I27" s="61">
-        <v>0</v>
-      </c>
-      <c r="J27" s="61">
-        <v>0</v>
-      </c>
-      <c r="K27" s="62">
-        <v>0</v>
-      </c>
-      <c r="L27" s="63">
-        <f>SUM(D27:J27)*50/(L$1-K27)</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="64">
-        <v>0</v>
-      </c>
-      <c r="N27" s="65">
-        <v>0</v>
-      </c>
-      <c r="O27" s="65">
-        <v>0</v>
-      </c>
-      <c r="P27" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="63">
-        <f>SUM(M27:O27)/(Q$1-P27)</f>
-        <v>0</v>
-      </c>
-      <c r="R27" s="64">
-        <v>0</v>
-      </c>
-      <c r="S27" s="64">
-        <v>0</v>
-      </c>
-      <c r="T27" s="63">
-        <f>SUM(R27:S27)/T$1</f>
-        <v>0</v>
-      </c>
-      <c r="U27" s="65"/>
-      <c r="V27" s="66"/>
-      <c r="W27" s="67">
-        <f>L27*0.2+Q27*0.25+T27*0.25+U27*0.3+V27*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="56" t="s">
+      <c r="D27" s="58">
+        <v>0</v>
+      </c>
+      <c r="E27" s="58">
+        <v>0</v>
+      </c>
+      <c r="F27" s="58">
+        <v>0</v>
+      </c>
+      <c r="G27" s="58">
+        <v>0</v>
+      </c>
+      <c r="H27" s="59">
+        <v>0</v>
+      </c>
+      <c r="I27" s="60">
+        <v>0</v>
+      </c>
+      <c r="J27" s="60">
+        <v>0</v>
+      </c>
+      <c r="K27" s="61">
+        <v>0</v>
+      </c>
+      <c r="L27" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="63">
+        <v>0</v>
+      </c>
+      <c r="N27" s="64">
+        <v>0</v>
+      </c>
+      <c r="O27" s="64">
+        <v>0</v>
+      </c>
+      <c r="P27" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="63">
+        <v>0</v>
+      </c>
+      <c r="S27" s="63">
+        <v>0</v>
+      </c>
+      <c r="T27" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U27" s="64">
+        <v>0</v>
+      </c>
+      <c r="V27" s="65"/>
+      <c r="W27" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" s="67" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="59">
-        <v>0</v>
-      </c>
-      <c r="E28" s="59">
-        <v>0</v>
-      </c>
-      <c r="F28" s="59">
-        <v>0</v>
-      </c>
-      <c r="G28" s="59">
-        <v>0</v>
-      </c>
-      <c r="H28" s="60">
-        <v>0</v>
-      </c>
-      <c r="I28" s="61">
-        <v>0</v>
-      </c>
-      <c r="J28" s="61">
-        <v>0</v>
-      </c>
-      <c r="K28" s="62">
-        <v>0</v>
-      </c>
-      <c r="L28" s="63">
-        <f>SUM(D28:J28)*50/(L$1-K28)</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="64">
-        <v>0</v>
-      </c>
-      <c r="N28" s="65">
-        <v>0</v>
-      </c>
-      <c r="O28" s="65">
-        <v>0</v>
-      </c>
-      <c r="P28" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="63">
-        <f>SUM(M28:O28)/(Q$1-P28)</f>
-        <v>0</v>
-      </c>
-      <c r="R28" s="64">
-        <v>0</v>
-      </c>
-      <c r="S28" s="64">
-        <v>0</v>
-      </c>
-      <c r="T28" s="63">
-        <f>SUM(R28:S28)/T$1</f>
-        <v>0</v>
-      </c>
-      <c r="U28" s="65"/>
-      <c r="V28" s="66"/>
-      <c r="W28" s="67">
-        <f>L28*0.2+Q28*0.25+T28*0.25+U28*0.3+V28*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
+      <c r="D28" s="58">
+        <v>0</v>
+      </c>
+      <c r="E28" s="58">
+        <v>0</v>
+      </c>
+      <c r="F28" s="58">
+        <v>0</v>
+      </c>
+      <c r="G28" s="58">
+        <v>0</v>
+      </c>
+      <c r="H28" s="59">
+        <v>0</v>
+      </c>
+      <c r="I28" s="60">
+        <v>0</v>
+      </c>
+      <c r="J28" s="60">
+        <v>0</v>
+      </c>
+      <c r="K28" s="61">
+        <v>0</v>
+      </c>
+      <c r="L28" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="63">
+        <v>0</v>
+      </c>
+      <c r="N28" s="64">
+        <v>0</v>
+      </c>
+      <c r="O28" s="64">
+        <v>0</v>
+      </c>
+      <c r="P28" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="63">
+        <v>0</v>
+      </c>
+      <c r="S28" s="63">
+        <v>0</v>
+      </c>
+      <c r="T28" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U28" s="64">
+        <v>0</v>
+      </c>
+      <c r="V28" s="65"/>
+      <c r="W28" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" s="67" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="57" t="s">
+      <c r="B29" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C29" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="59">
-        <v>0</v>
-      </c>
-      <c r="E29" s="59">
-        <v>0</v>
-      </c>
-      <c r="F29" s="59">
-        <v>0</v>
-      </c>
-      <c r="G29" s="59">
-        <v>0</v>
-      </c>
-      <c r="H29" s="60">
-        <v>0</v>
-      </c>
-      <c r="I29" s="61">
-        <v>0</v>
-      </c>
-      <c r="J29" s="61">
-        <v>0</v>
-      </c>
-      <c r="K29" s="62">
-        <v>0</v>
-      </c>
-      <c r="L29" s="63">
-        <f>SUM(D29:J29)*50/(L$1-K29)</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="64">
-        <v>0</v>
-      </c>
-      <c r="N29" s="65">
-        <v>0</v>
-      </c>
-      <c r="O29" s="65">
-        <v>0</v>
-      </c>
-      <c r="P29" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="63">
-        <f>SUM(M29:O29)/(Q$1-P29)</f>
-        <v>0</v>
-      </c>
-      <c r="R29" s="64">
-        <v>0</v>
-      </c>
-      <c r="S29" s="64">
-        <v>0</v>
-      </c>
-      <c r="T29" s="63">
-        <f>SUM(R29:S29)/T$1</f>
-        <v>0</v>
-      </c>
-      <c r="U29" s="65"/>
-      <c r="V29" s="66"/>
-      <c r="W29" s="67">
-        <f>L29*0.2+Q29*0.25+T29*0.25+U29*0.3+V29*0.15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" s="69" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="56" t="s">
+      <c r="D29" s="58">
+        <v>0</v>
+      </c>
+      <c r="E29" s="58">
+        <v>0</v>
+      </c>
+      <c r="F29" s="58">
+        <v>0</v>
+      </c>
+      <c r="G29" s="58">
+        <v>0</v>
+      </c>
+      <c r="H29" s="59">
+        <v>0</v>
+      </c>
+      <c r="I29" s="60">
+        <v>0</v>
+      </c>
+      <c r="J29" s="60">
+        <v>0</v>
+      </c>
+      <c r="K29" s="61">
+        <v>0</v>
+      </c>
+      <c r="L29" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="63">
+        <v>0</v>
+      </c>
+      <c r="N29" s="64">
+        <v>0</v>
+      </c>
+      <c r="O29" s="64">
+        <v>0</v>
+      </c>
+      <c r="P29" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="63">
+        <v>0</v>
+      </c>
+      <c r="S29" s="63">
+        <v>0</v>
+      </c>
+      <c r="T29" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U29" s="64">
+        <v>0</v>
+      </c>
+      <c r="V29" s="65"/>
+      <c r="W29" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" s="68" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="58" t="s">
+      <c r="C30" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="59">
-        <v>0</v>
-      </c>
-      <c r="E30" s="59">
-        <v>0</v>
-      </c>
-      <c r="F30" s="59">
-        <v>0</v>
-      </c>
-      <c r="G30" s="59">
-        <v>0</v>
-      </c>
-      <c r="H30" s="60">
-        <v>0</v>
-      </c>
-      <c r="I30" s="61">
-        <v>0</v>
-      </c>
-      <c r="J30" s="61">
-        <v>0</v>
-      </c>
-      <c r="K30" s="62">
-        <v>0</v>
-      </c>
-      <c r="L30" s="63">
-        <f>SUM(D30:J30)*50/(L$1-K30)</f>
-        <v>0</v>
-      </c>
-      <c r="M30" s="64">
-        <v>0</v>
-      </c>
-      <c r="N30" s="65">
-        <v>0</v>
-      </c>
-      <c r="O30" s="65">
-        <v>0</v>
-      </c>
-      <c r="P30" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="63">
-        <f>SUM(M30:O30)/(Q$1-P30)</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="64">
-        <v>0</v>
-      </c>
-      <c r="S30" s="64">
-        <v>0</v>
-      </c>
-      <c r="T30" s="63">
-        <f>SUM(R30:S30)/T$1</f>
-        <v>0</v>
-      </c>
-      <c r="U30" s="65"/>
-      <c r="V30" s="66"/>
-      <c r="W30" s="67">
+      <c r="D30" s="58">
+        <v>0</v>
+      </c>
+      <c r="E30" s="58">
+        <v>0</v>
+      </c>
+      <c r="F30" s="58">
+        <v>0</v>
+      </c>
+      <c r="G30" s="58">
+        <v>0</v>
+      </c>
+      <c r="H30" s="59">
+        <v>0</v>
+      </c>
+      <c r="I30" s="60">
+        <v>0</v>
+      </c>
+      <c r="J30" s="60">
+        <v>0</v>
+      </c>
+      <c r="K30" s="61">
+        <v>0</v>
+      </c>
+      <c r="L30" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="63">
+        <v>0</v>
+      </c>
+      <c r="N30" s="64">
+        <v>0</v>
+      </c>
+      <c r="O30" s="64">
+        <v>0</v>
+      </c>
+      <c r="P30" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R30" s="63">
+        <v>0</v>
+      </c>
+      <c r="S30" s="63">
+        <v>0</v>
+      </c>
+      <c r="T30" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U30" s="64">
+        <v>0</v>
+      </c>
+      <c r="V30" s="65"/>
+      <c r="W30" s="66">
         <f>L30*0.2+Q30*0.25+T30*0.25+U30*0.3+V30*0.1</f>
         <v>0</v>
       </c>
-      <c r="X30" s="68"/>
+      <c r="X30" s="67"/>
     </row>
     <row r="31" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
@@ -3650,7 +3674,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="52"/>
+      <c r="H31" s="51"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3672,7 +3696,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="52"/>
+      <c r="H32" s="51"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3694,7 +3718,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="52"/>
+      <c r="H33" s="51"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3716,7 +3740,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="52"/>
+      <c r="H34" s="51"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3738,7 +3762,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="52"/>
+      <c r="H35" s="51"/>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3760,7 +3784,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="52"/>
+      <c r="H36" s="51"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -3782,7 +3806,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="52"/>
+      <c r="H37" s="51"/>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -3804,7 +3828,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="52"/>
+      <c r="H38" s="51"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -3826,7 +3850,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="52"/>
+      <c r="H39" s="51"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -3848,7 +3872,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="52"/>
+      <c r="H40" s="51"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
@@ -3870,7 +3894,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="52"/>
+      <c r="H41" s="51"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
@@ -3892,7 +3916,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="52"/>
+      <c r="H42" s="51"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -3914,7 +3938,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="52"/>
+      <c r="H43" s="51"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
@@ -3936,7 +3960,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="52"/>
+      <c r="H44" s="51"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -3958,7 +3982,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="52"/>
+      <c r="H45" s="51"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -3980,7 +4004,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="52"/>
+      <c r="H46" s="51"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -4002,7 +4026,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="52"/>
+      <c r="H47" s="51"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -4024,7 +4048,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="52"/>
+      <c r="H48" s="51"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -4046,7 +4070,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="52"/>
+      <c r="H49" s="51"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -4068,7 +4092,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="52"/>
+      <c r="H50" s="51"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
@@ -4090,7 +4114,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="52"/>
+      <c r="H51" s="51"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -4112,7 +4136,7 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
-      <c r="H52" s="52"/>
+      <c r="H52" s="51"/>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -4134,7 +4158,7 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="52"/>
+      <c r="H53" s="51"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -4156,7 +4180,7 @@
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
-      <c r="H54" s="52"/>
+      <c r="H54" s="51"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -4178,7 +4202,7 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
-      <c r="H55" s="52"/>
+      <c r="H55" s="51"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -4200,7 +4224,7 @@
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="52"/>
+      <c r="H56" s="51"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -4222,7 +4246,7 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="52"/>
+      <c r="H57" s="51"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -4244,7 +4268,7 @@
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
-      <c r="H58" s="52"/>
+      <c r="H58" s="51"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -4266,7 +4290,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="52"/>
+      <c r="H59" s="51"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -4288,7 +4312,7 @@
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="52"/>
+      <c r="H60" s="51"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -4310,7 +4334,7 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
-      <c r="H61" s="52"/>
+      <c r="H61" s="51"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -4332,7 +4356,7 @@
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
-      <c r="H62" s="52"/>
+      <c r="H62" s="51"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -4354,7 +4378,7 @@
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
-      <c r="H63" s="52"/>
+      <c r="H63" s="51"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -4376,7 +4400,7 @@
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
-      <c r="H64" s="52"/>
+      <c r="H64" s="51"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -4398,7 +4422,7 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="52"/>
+      <c r="H65" s="51"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -4420,7 +4444,7 @@
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
-      <c r="H66" s="52"/>
+      <c r="H66" s="51"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -4442,7 +4466,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="52"/>
+      <c r="H67" s="51"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -4464,7 +4488,7 @@
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
-      <c r="H68" s="52"/>
+      <c r="H68" s="51"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -4486,7 +4510,7 @@
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
-      <c r="H69" s="52"/>
+      <c r="H69" s="51"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -4508,7 +4532,7 @@
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
-      <c r="H70" s="52"/>
+      <c r="H70" s="51"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -4530,7 +4554,7 @@
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
-      <c r="H71" s="52"/>
+      <c r="H71" s="51"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -4552,7 +4576,7 @@
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
-      <c r="H72" s="52"/>
+      <c r="H72" s="51"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -4574,7 +4598,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
-      <c r="H73" s="52"/>
+      <c r="H73" s="51"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -4596,7 +4620,7 @@
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
-      <c r="H74" s="52"/>
+      <c r="H74" s="51"/>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -4618,7 +4642,7 @@
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
-      <c r="H75" s="52"/>
+      <c r="H75" s="51"/>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -4640,7 +4664,7 @@
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
-      <c r="H76" s="52"/>
+      <c r="H76" s="51"/>
       <c r="I76" s="9"/>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
@@ -4828,9 +4852,9 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y34" sqref="Y34"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4838,7 +4862,7 @@
     <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="73" customWidth="1"/>
     <col min="5" max="6" width="3.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -4857,23 +4881,23 @@
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="34"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="72" t="s">
+      <c r="D1" s="69"/>
+      <c r="E1" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="72" t="s">
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="74"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="78"/>
       <c r="Q1" s="33" t="s">
         <v>44</v>
       </c>
@@ -4894,23 +4918,23 @@
       <c r="C2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="70" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="37">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F2" s="27">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G2" s="27">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H2" s="27">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I2" s="27">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>30</v>
@@ -4945,10 +4969,18 @@
     </row>
     <row r="3" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="71">
+        <v>100</v>
+      </c>
+      <c r="E3" s="38">
+        <v>2</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -4966,10 +4998,18 @@
     </row>
     <row r="4" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="38"/>
+      <c r="B4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="71">
+        <v>87.333333333333329</v>
+      </c>
+      <c r="E4" s="38">
+        <v>2</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -4987,10 +5027,18 @@
     </row>
     <row r="5" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="71">
+        <v>68.05</v>
+      </c>
+      <c r="E5" s="38">
+        <v>2</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -5008,10 +5056,18 @@
     </row>
     <row r="6" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="38"/>
+      <c r="B6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="71">
+        <v>63.65</v>
+      </c>
+      <c r="E6" s="38">
+        <v>2</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -5029,10 +5085,18 @@
     </row>
     <row r="7" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="38"/>
+      <c r="B7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="71">
+        <v>61.558333333333337</v>
+      </c>
+      <c r="E7" s="38">
+        <v>2</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -5050,10 +5114,18 @@
     </row>
     <row r="8" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="38"/>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="71">
+        <v>60.541666666666671</v>
+      </c>
+      <c r="E8" s="38">
+        <v>2</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -5071,10 +5143,18 @@
     </row>
     <row r="9" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="38"/>
+      <c r="B9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="71">
+        <v>58.758333333333326</v>
+      </c>
+      <c r="E9" s="38">
+        <v>2</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -5092,10 +5172,18 @@
     </row>
     <row r="10" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="38"/>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="71">
+        <v>57.80833333333333</v>
+      </c>
+      <c r="E10" s="38">
+        <v>2</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -5113,10 +5201,18 @@
     </row>
     <row r="11" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="38"/>
+      <c r="B11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="71">
+        <v>55.416666666666671</v>
+      </c>
+      <c r="E11" s="38">
+        <v>2</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -5134,10 +5230,18 @@
     </row>
     <row r="12" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="38"/>
+      <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="71">
+        <v>53.875</v>
+      </c>
+      <c r="E12" s="38">
+        <v>2</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -5155,10 +5259,18 @@
     </row>
     <row r="13" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="71">
+        <v>53.308333333333337</v>
+      </c>
+      <c r="E13" s="38">
+        <v>2</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -5176,10 +5288,18 @@
     </row>
     <row r="14" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="38"/>
+      <c r="B14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="71">
+        <v>51.866666666666674</v>
+      </c>
+      <c r="E14" s="38">
+        <v>2</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -5197,10 +5317,18 @@
     </row>
     <row r="15" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="38"/>
+      <c r="B15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="71">
+        <v>39.083333333333336</v>
+      </c>
+      <c r="E15" s="38">
+        <v>0</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -5218,10 +5346,18 @@
     </row>
     <row r="16" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="38"/>
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="71">
+        <v>37.758333333333333</v>
+      </c>
+      <c r="E16" s="38">
+        <v>1</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -5239,10 +5375,18 @@
     </row>
     <row r="17" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="71">
+        <v>36.25</v>
+      </c>
+      <c r="E17" s="38">
+        <v>2</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -5260,10 +5404,18 @@
     </row>
     <row r="18" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="38"/>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="71">
+        <v>32.25</v>
+      </c>
+      <c r="E18" s="38">
+        <v>2</v>
+      </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -5281,11 +5433,19 @@
     </row>
     <row r="19" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="42"/>
+      <c r="B19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="71">
+        <v>25.558333333333337</v>
+      </c>
+      <c r="E19" s="38">
+        <v>0</v>
+      </c>
+      <c r="F19" s="41"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -5302,10 +5462,18 @@
     </row>
     <row r="20" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="38"/>
+      <c r="B20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="71">
+        <v>12.5</v>
+      </c>
+      <c r="E20" s="38">
+        <v>0</v>
+      </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -5323,10 +5491,18 @@
     </row>
     <row r="21" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="38"/>
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="71">
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="E21" s="38">
+        <v>0</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -5344,10 +5520,18 @@
     </row>
     <row r="22" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="38"/>
+      <c r="B22" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="71">
+        <v>0</v>
+      </c>
+      <c r="E22" s="38">
+        <v>0</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -5365,10 +5549,18 @@
     </row>
     <row r="23" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="38"/>
+      <c r="B23" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="71">
+        <v>0</v>
+      </c>
+      <c r="E23" s="38">
+        <v>0</v>
+      </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -5386,10 +5578,18 @@
     </row>
     <row r="24" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="38"/>
+      <c r="B24" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="71">
+        <v>0</v>
+      </c>
+      <c r="E24" s="38">
+        <v>0</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -5407,10 +5607,18 @@
     </row>
     <row r="25" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="38"/>
+      <c r="B25" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="71">
+        <v>0</v>
+      </c>
+      <c r="E25" s="38">
+        <v>0</v>
+      </c>
       <c r="F25" s="12"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -5428,10 +5636,18 @@
     </row>
     <row r="26" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="38"/>
+      <c r="B26" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="71">
+        <v>0</v>
+      </c>
+      <c r="E26" s="38">
+        <v>0</v>
+      </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
@@ -5449,10 +5665,18 @@
     </row>
     <row r="27" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="38"/>
+      <c r="B27" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="71">
+        <v>0</v>
+      </c>
+      <c r="E27" s="38">
+        <v>0</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
@@ -5470,10 +5694,18 @@
     </row>
     <row r="28" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="38"/>
+      <c r="B28" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="71">
+        <v>0</v>
+      </c>
+      <c r="E28" s="38">
+        <v>0</v>
+      </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -5491,10 +5723,18 @@
     </row>
     <row r="29" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="38"/>
+      <c r="B29" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="71">
+        <v>0</v>
+      </c>
+      <c r="E29" s="38">
+        <v>0</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -5512,10 +5752,18 @@
     </row>
     <row r="30" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="38"/>
+      <c r="B30" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="71">
+        <v>0</v>
+      </c>
+      <c r="E30" s="38">
+        <v>0</v>
+      </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -5535,7 +5783,7 @@
       <c r="A31" s="20"/>
       <c r="B31" s="11"/>
       <c r="C31" s="36"/>
-      <c r="D31" s="21"/>
+      <c r="D31" s="71"/>
       <c r="E31" s="38"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -5556,7 +5804,7 @@
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="36"/>
-      <c r="D32" s="21"/>
+      <c r="D32" s="71"/>
       <c r="E32" s="38"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
@@ -5577,7 +5825,7 @@
       <c r="A33" s="22"/>
       <c r="B33" s="23"/>
       <c r="C33" s="36"/>
-      <c r="D33" s="21"/>
+      <c r="D33" s="71"/>
       <c r="E33" s="39"/>
       <c r="F33" s="13"/>
       <c r="G33" s="7"/>
@@ -5598,7 +5846,7 @@
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
@@ -5608,7 +5856,7 @@
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="D35" s="72"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
@@ -5626,7 +5874,7 @@
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="D36" s="72"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
@@ -5644,7 +5892,7 @@
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+      <c r="D37" s="72"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -5662,7 +5910,7 @@
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
+      <c r="D38" s="72"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
@@ -5680,7 +5928,7 @@
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="D39" s="72"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -5698,7 +5946,7 @@
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
+      <c r="D40" s="72"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -5716,7 +5964,7 @@
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
+      <c r="D41" s="72"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
@@ -5734,7 +5982,7 @@
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
@@ -5752,7 +6000,7 @@
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
+      <c r="D43" s="72"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
@@ -5770,7 +6018,7 @@
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
+      <c r="D44" s="72"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
@@ -5788,7 +6036,7 @@
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
+      <c r="D45" s="72"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -5806,7 +6054,7 @@
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
+      <c r="D46" s="72"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -5824,7 +6072,7 @@
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
+      <c r="D47" s="72"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
@@ -5842,7 +6090,7 @@
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
+      <c r="D48" s="72"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
@@ -5860,7 +6108,7 @@
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
+      <c r="D49" s="72"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
@@ -5878,7 +6126,7 @@
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
+      <c r="D50" s="72"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
@@ -5896,7 +6144,7 @@
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
+      <c r="D51" s="72"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
@@ -5914,7 +6162,7 @@
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
+      <c r="D52" s="72"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
@@ -5932,7 +6180,7 @@
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
+      <c r="D53" s="72"/>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
@@ -5950,7 +6198,7 @@
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
+      <c r="D54" s="72"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
@@ -5968,7 +6216,7 @@
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
+      <c r="D55" s="72"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
@@ -5986,7 +6234,7 @@
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
+      <c r="D56" s="72"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
@@ -6004,7 +6252,7 @@
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
+      <c r="D57" s="72"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
@@ -6022,7 +6270,7 @@
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
+      <c r="D58" s="72"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
@@ -6040,7 +6288,7 @@
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
+      <c r="D59" s="72"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
@@ -6058,7 +6306,7 @@
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
+      <c r="D60" s="72"/>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
@@ -6076,7 +6324,7 @@
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
+      <c r="D61" s="72"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
@@ -6094,7 +6342,7 @@
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
+      <c r="D62" s="72"/>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
@@ -6112,7 +6360,7 @@
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
+      <c r="D63" s="72"/>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
@@ -6130,7 +6378,7 @@
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
+      <c r="D64" s="72"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
@@ -6148,7 +6396,7 @@
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
+      <c r="D65" s="72"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
@@ -6166,7 +6414,7 @@
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
+      <c r="D66" s="72"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
@@ -6184,7 +6432,7 @@
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
+      <c r="D67" s="72"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
@@ -6202,7 +6450,7 @@
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
+      <c r="D68" s="72"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
@@ -6220,7 +6468,7 @@
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
+      <c r="D69" s="72"/>
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
@@ -6238,7 +6486,7 @@
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
+      <c r="D70" s="72"/>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
@@ -6256,7 +6504,7 @@
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
+      <c r="D71" s="72"/>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
@@ -6274,7 +6522,7 @@
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
+      <c r="D72" s="72"/>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
@@ -6292,7 +6540,7 @@
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
+      <c r="D73" s="72"/>
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
@@ -6310,7 +6558,7 @@
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
+      <c r="D74" s="72"/>
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
@@ -6328,7 +6576,7 @@
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
+      <c r="D75" s="72"/>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
@@ -6346,7 +6594,7 @@
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
+      <c r="D76" s="72"/>
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
@@ -6364,7 +6612,7 @@
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
+      <c r="D77" s="72"/>
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
       <c r="G77" s="8"/>
@@ -6382,7 +6630,7 @@
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
+      <c r="D78" s="72"/>
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
@@ -6400,7 +6648,7 @@
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
+      <c r="D79" s="72"/>
       <c r="E79" s="8"/>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
@@ -6418,7 +6666,7 @@
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
+      <c r="D80" s="72"/>
       <c r="E80" s="8"/>
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
@@ -6436,7 +6684,7 @@
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
+      <c r="D81" s="72"/>
       <c r="E81" s="8"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
@@ -6459,19 +6707,19 @@
     <mergeCell ref="K1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:I33">
-    <cfRule type="cellIs" dxfId="10" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="26" operator="between">
       <formula>0.1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="28" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J33">
-    <cfRule type="dataBar" priority="24">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6485,7 +6733,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P33">
-    <cfRule type="dataBar" priority="23">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6499,7 +6747,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R33">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6513,24 +6761,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:O33">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="19" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="20" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S33">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6544,7 +6792,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D6 D8:D33">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6558,7 +6806,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6572,19 +6820,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q33">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
       <formula>60</formula>
       <formula>79</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThanOrEqual">
       <formula>80</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{71125D8B-F38D-441C-A719-0BEE1515DAA1}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6659,6 +6921,19 @@
           </x14:cfRule>
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{71125D8B-F38D-441C-A719-0BEE1515DAA1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
ileri java hafta 9
</commit_message>
<xml_diff>
--- a/AdvancedJava/_docs/Notlar.xlsx
+++ b/AdvancedJava/_docs/Notlar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vize" sheetId="1" r:id="rId1"/>
@@ -1469,9 +1469,9 @@
   </sheetPr>
   <dimension ref="A1:X76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W20" sqref="W20"/>
+      <selection pane="bottomLeft" activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="16">
-        <f>SUM(D3:J3)*50/(L$1-K3)</f>
+        <f t="shared" ref="L3:L30" si="0">SUM(D3:J3)*50/(L$1-K3)</f>
         <v>116.66666666666667</v>
       </c>
       <c r="M3" s="14">
@@ -1664,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="16">
-        <f>SUM(M3:O3)/(Q$1-P3)</f>
+        <f t="shared" ref="Q3:Q30" si="1">SUM(M3:O3)/(Q$1-P3)</f>
         <v>100</v>
       </c>
       <c r="R3" s="14">
@@ -1674,7 +1674,7 @@
         <v>100</v>
       </c>
       <c r="T3" s="16">
-        <f>SUM(R3:S3)/T$1</f>
+        <f t="shared" ref="T3:T30" si="2">SUM(R3:S3)/T$1</f>
         <v>100</v>
       </c>
       <c r="U3" s="6">
@@ -1723,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="16">
-        <f>SUM(D4:J4)*50/(L$1-K4)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="M4" s="14">
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="16">
-        <f>SUM(M4:O4)/(Q$1-P4)</f>
+        <f t="shared" si="1"/>
         <v>93.333333333333329</v>
       </c>
       <c r="R4" s="14">
@@ -1749,7 +1749,7 @@
         <v>80</v>
       </c>
       <c r="T4" s="16">
-        <f>SUM(R4:S4)/T$1</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="U4" s="6">
@@ -1796,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="16">
-        <f>SUM(D5:J5)*50/(L$1-K5)</f>
+        <f t="shared" si="0"/>
         <v>97.5</v>
       </c>
       <c r="M5" s="14">
@@ -1812,7 +1812,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="16">
-        <f>SUM(M5:O5)/(Q$1-P5)</f>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="R5" s="14">
@@ -1822,7 +1822,7 @@
         <v>50</v>
       </c>
       <c r="T5" s="16">
-        <f>SUM(R5:S5)/T$1</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="U5" s="6">
@@ -1832,7 +1832,7 @@
         <v>70</v>
       </c>
       <c r="W5" s="21">
-        <f>L5*0.2+Q5*0.25+T5*0.25+U5*0.3+V5*0.15</f>
+        <f t="shared" ref="W5:W12" si="3">L5*0.2+Q5*0.25+T5*0.25+U5*0.3+V5*0.15</f>
         <v>78.55</v>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="16">
-        <f>SUM(D6:J6)*50/(L$1-K6)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="M6" s="14">
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="16">
-        <f>SUM(M6:O6)/(Q$1-P6)</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="R6" s="14">
@@ -1897,7 +1897,7 @@
         <v>20</v>
       </c>
       <c r="T6" s="16">
-        <f>SUM(R6:S6)/T$1</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="U6" s="6">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="V6" s="43"/>
       <c r="W6" s="21">
-        <f>L6*0.2+Q6*0.25+T6*0.25+U6*0.3+V6*0.15</f>
+        <f t="shared" si="3"/>
         <v>65.900000000000006</v>
       </c>
     </row>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="16">
-        <f>SUM(D7:J7)*50/(L$1-K7)</f>
+        <f t="shared" si="0"/>
         <v>116.66666666666667</v>
       </c>
       <c r="M7" s="14">
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="16">
-        <f>SUM(M7:O7)/(Q$1-P7)</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="R7" s="14">
@@ -1970,7 +1970,7 @@
         <v>-25</v>
       </c>
       <c r="T7" s="16">
-        <f>SUM(R7:S7)/T$1</f>
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="U7" s="6">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="V7" s="43"/>
       <c r="W7" s="21">
-        <f>L7*0.2+Q7*0.25+T7*0.25+U7*0.3+V7*0.15</f>
+        <f t="shared" si="3"/>
         <v>61.558333333333337</v>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="16">
-        <f>SUM(D8:J8)*50/(L$1-K8)</f>
+        <f t="shared" si="0"/>
         <v>81.666666666666671</v>
       </c>
       <c r="M8" s="14">
@@ -2033,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="16">
-        <f>SUM(M8:O8)/(Q$1-P8)</f>
+        <f t="shared" si="1"/>
         <v>93.333333333333329</v>
       </c>
       <c r="R8" s="14">
@@ -2043,7 +2043,7 @@
         <v>61</v>
       </c>
       <c r="T8" s="16">
-        <f>SUM(R8:S8)/T$1</f>
+        <f t="shared" si="2"/>
         <v>35.5</v>
       </c>
       <c r="U8" s="6">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="V8" s="43"/>
       <c r="W8" s="21">
-        <f>L8*0.2+Q8*0.25+T8*0.25+U8*0.3+V8*0.15</f>
+        <f t="shared" si="3"/>
         <v>60.541666666666671</v>
       </c>
     </row>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="16">
-        <f>SUM(D9:J9)*50/(L$1-K9)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="M9" s="14">
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="16">
-        <f>SUM(M9:O9)/(Q$1-P9)</f>
+        <f t="shared" si="1"/>
         <v>83.333333333333329</v>
       </c>
       <c r="R9" s="14">
@@ -2116,7 +2116,7 @@
         <v>30</v>
       </c>
       <c r="T9" s="16">
-        <f>SUM(R9:S9)/T$1</f>
+        <f t="shared" si="2"/>
         <v>52.5</v>
       </c>
       <c r="U9" s="6">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="V9" s="43"/>
       <c r="W9" s="21">
-        <f>L9*0.2+Q9*0.25+T9*0.25+U9*0.3+V9*0.15</f>
+        <f t="shared" si="3"/>
         <v>58.758333333333326</v>
       </c>
     </row>
@@ -2163,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="16">
-        <f>SUM(D10:J10)*50/(L$1-K10)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="M10" s="14">
@@ -2179,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="16">
-        <f>SUM(M10:O10)/(Q$1-P10)</f>
+        <f t="shared" si="1"/>
         <v>93.333333333333329</v>
       </c>
       <c r="R10" s="14">
@@ -2189,7 +2189,7 @@
         <v>-25</v>
       </c>
       <c r="T10" s="16">
-        <f>SUM(R10:S10)/T$1</f>
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="U10" s="6">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="V10" s="43"/>
       <c r="W10" s="21">
-        <f>L10*0.2+Q10*0.25+T10*0.25+U10*0.3+V10*0.15</f>
+        <f t="shared" si="3"/>
         <v>57.80833333333333</v>
       </c>
     </row>
@@ -2236,7 +2236,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="16">
-        <f>SUM(D11:J11)*50/(L$1-K11)</f>
+        <f t="shared" si="0"/>
         <v>98.333333333333329</v>
       </c>
       <c r="M11" s="14">
@@ -2252,7 +2252,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="16">
-        <f>SUM(M11:O11)/(Q$1-P11)</f>
+        <f t="shared" si="1"/>
         <v>86.666666666666671</v>
       </c>
       <c r="R11" s="14">
@@ -2262,7 +2262,7 @@
         <v>-25</v>
       </c>
       <c r="T11" s="16">
-        <f>SUM(R11:S11)/T$1</f>
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="U11" s="6">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="V11" s="43"/>
       <c r="W11" s="21">
-        <f>L11*0.2+Q11*0.25+T11*0.25+U11*0.3+V11*0.15</f>
+        <f t="shared" si="3"/>
         <v>55.808333333333337</v>
       </c>
     </row>
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="16">
-        <f>SUM(D12:J12)*50/(L$1-K12)</f>
+        <f t="shared" si="0"/>
         <v>115</v>
       </c>
       <c r="M12" s="14">
@@ -2325,7 +2325,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="16">
-        <f>SUM(M12:O12)/(Q$1-P12)</f>
+        <f t="shared" si="1"/>
         <v>76.666666666666671</v>
       </c>
       <c r="R12" s="14">
@@ -2335,7 +2335,7 @@
         <v>30</v>
       </c>
       <c r="T12" s="16">
-        <f>SUM(R12:S12)/T$1</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="U12" s="6">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="V12" s="43"/>
       <c r="W12" s="21">
-        <f>L12*0.2+Q12*0.25+T12*0.25+U12*0.3+V12*0.15</f>
+        <f t="shared" si="3"/>
         <v>55.416666666666671</v>
       </c>
     </row>
@@ -2382,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="16">
-        <f>SUM(D13:J13)*50/(L$1-K13)</f>
+        <f t="shared" si="0"/>
         <v>11.666666666666666</v>
       </c>
       <c r="M13" s="14">
@@ -2398,7 +2398,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="16">
-        <f>SUM(M13:O13)/(Q$1-P13)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="R13" s="14">
@@ -2408,7 +2408,7 @@
         <v>61</v>
       </c>
       <c r="T13" s="16">
-        <f>SUM(R13:S13)/T$1</f>
+        <f t="shared" si="2"/>
         <v>50.5</v>
       </c>
       <c r="U13" s="6">
@@ -2458,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="16">
-        <f>SUM(D14:J14)*50/(L$1-K14)</f>
+        <f t="shared" si="0"/>
         <v>115</v>
       </c>
       <c r="M14" s="14">
@@ -2474,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="16">
-        <f>SUM(M14:O14)/(Q$1-P14)</f>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="R14" s="14">
@@ -2484,7 +2484,7 @@
         <v>65</v>
       </c>
       <c r="T14" s="16">
-        <f>SUM(R14:S14)/T$1</f>
+        <f t="shared" si="2"/>
         <v>42.5</v>
       </c>
       <c r="U14" s="6">
@@ -2531,7 +2531,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="16">
-        <f>SUM(D15:J15)*50/(L$1-K15)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="M15" s="14">
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="16">
-        <f>SUM(M15:O15)/(Q$1-P15)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="R15" s="14">
@@ -2557,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="16">
-        <f>SUM(R15:S15)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U15" s="6">
@@ -2606,7 +2606,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="16">
-        <f>SUM(D16:J16)*50/(L$1-K16)</f>
+        <f t="shared" si="0"/>
         <v>98.000000000000014</v>
       </c>
       <c r="M16" s="14">
@@ -2622,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="Q16" s="16">
-        <f>SUM(M16:O16)/(Q$1-P16)</f>
+        <f t="shared" si="1"/>
         <v>91.666666666666671</v>
       </c>
       <c r="R16" s="14">
@@ -2632,7 +2632,7 @@
         <v>-25</v>
       </c>
       <c r="T16" s="16">
-        <f>SUM(R16:S16)/T$1</f>
+        <f t="shared" si="2"/>
         <v>-25</v>
       </c>
       <c r="U16" s="6">
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="16">
-        <f>SUM(D17:J17)*50/(L$1-K17)</f>
+        <f t="shared" si="0"/>
         <v>66.666666666666671</v>
       </c>
       <c r="M17" s="14">
@@ -2695,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="16">
-        <f>SUM(M17:O17)/(Q$1-P17)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="R17" s="14">
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="16">
-        <f>SUM(R17:S17)/T$1</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="U17" s="6">
@@ -2752,7 +2752,7 @@
         <v>3</v>
       </c>
       <c r="L18" s="16">
-        <f>SUM(D18:J18)*50/(L$1-K18)</f>
+        <f t="shared" si="0"/>
         <v>66.666666666666671</v>
       </c>
       <c r="M18" s="54" t="s">
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="Q18" s="16">
-        <f>SUM(M18:O18)/(Q$1-P18)</f>
+        <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
       <c r="R18" s="14">
@@ -2778,7 +2778,7 @@
         <v>20</v>
       </c>
       <c r="T18" s="16">
-        <f>SUM(R18:S18)/T$1</f>
+        <f t="shared" si="2"/>
         <v>40.5</v>
       </c>
       <c r="U18" s="6">
@@ -2826,7 +2826,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="16">
-        <f>SUM(D19:J19)*50/(L$1-K19)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="M19" s="14">
@@ -2842,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="16">
-        <f>SUM(M19:O19)/(Q$1-P19)</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="R19" s="14">
@@ -2852,7 +2852,7 @@
         <v>-25</v>
       </c>
       <c r="T19" s="16">
-        <f>SUM(R19:S19)/T$1</f>
+        <f t="shared" si="2"/>
         <v>-25</v>
       </c>
       <c r="U19" s="6">
@@ -2860,7 +2860,7 @@
       </c>
       <c r="V19" s="43"/>
       <c r="W19" s="21">
-        <f>L19*0.2+Q19*0.25+T19*0.25+U19*0.3+V19*0.15</f>
+        <f t="shared" ref="W19:W29" si="4">L19*0.2+Q19*0.25+T19*0.25+U19*0.3+V19*0.15</f>
         <v>36.25</v>
       </c>
     </row>
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="16">
-        <f>SUM(D20:J20)*50/(L$1-K20)</f>
+        <f t="shared" si="0"/>
         <v>83.333333333333329</v>
       </c>
       <c r="M20" s="14">
@@ -2915,7 +2915,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="16">
-        <f>SUM(M20:O20)/(Q$1-P20)</f>
+        <f t="shared" si="1"/>
         <v>33.333333333333336</v>
       </c>
       <c r="R20" s="14">
@@ -2925,7 +2925,7 @@
         <v>-25</v>
       </c>
       <c r="T20" s="16">
-        <f>SUM(R20:S20)/T$1</f>
+        <f t="shared" si="2"/>
         <v>-25</v>
       </c>
       <c r="U20" s="6">
@@ -2933,7 +2933,7 @@
       </c>
       <c r="V20" s="43"/>
       <c r="W20" s="21">
-        <f>L20*0.2+Q20*0.25+T20*0.25+U20*0.3+V20*0.15</f>
+        <f t="shared" si="4"/>
         <v>32.25</v>
       </c>
       <c r="X20" s="1"/>
@@ -2973,7 +2973,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="16">
-        <f>SUM(D21:J21)*50/(L$1-K21)</f>
+        <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
       <c r="M21" s="14">
@@ -2989,7 +2989,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="16">
-        <f>SUM(M21:O21)/(Q$1-P21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R21" s="14">
@@ -2999,7 +2999,7 @@
         <v>25</v>
       </c>
       <c r="T21" s="16">
-        <f>SUM(R21:S21)/T$1</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="U21" s="6">
@@ -3007,7 +3007,7 @@
       </c>
       <c r="V21" s="43"/>
       <c r="W21" s="21">
-        <f>L21*0.2+Q21*0.25+T21*0.25+U21*0.3+V21*0.15</f>
+        <f t="shared" si="4"/>
         <v>9.5833333333333339</v>
       </c>
     </row>
@@ -3046,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="62">
-        <f>SUM(D22:J22)*50/(L$1-K22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M22" s="63">
@@ -3062,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="62">
-        <f>SUM(M22:O22)/(Q$1-P22)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R22" s="63">
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="T22" s="62">
-        <f>SUM(R22:S22)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U22" s="64">
@@ -3080,7 +3080,7 @@
       </c>
       <c r="V22" s="65"/>
       <c r="W22" s="66">
-        <f>L22*0.2+Q22*0.25+T22*0.25+U22*0.3+V22*0.15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3119,7 +3119,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="62">
-        <f>SUM(D23:J23)*50/(L$1-K23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M23" s="63">
@@ -3135,7 +3135,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="62">
-        <f>SUM(M23:O23)/(Q$1-P23)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R23" s="63">
@@ -3145,7 +3145,7 @@
         <v>0</v>
       </c>
       <c r="T23" s="62">
-        <f>SUM(R23:S23)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U23" s="64">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="V23" s="65"/>
       <c r="W23" s="66">
-        <f>L23*0.2+Q23*0.25+T23*0.25+U23*0.3+V23*0.15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3192,7 +3192,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="62">
-        <f>SUM(D24:J24)*50/(L$1-K24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M24" s="63">
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="62">
-        <f>SUM(M24:O24)/(Q$1-P24)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R24" s="63">
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="T24" s="62">
-        <f>SUM(R24:S24)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U24" s="64">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="V24" s="65"/>
       <c r="W24" s="66">
-        <f>L24*0.2+Q24*0.25+T24*0.25+U24*0.3+V24*0.15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3265,7 +3265,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="62">
-        <f>SUM(D25:J25)*50/(L$1-K25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M25" s="63">
@@ -3281,7 +3281,7 @@
         <v>0</v>
       </c>
       <c r="Q25" s="62">
-        <f>SUM(M25:O25)/(Q$1-P25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R25" s="63">
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="T25" s="62">
-        <f>SUM(R25:S25)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U25" s="64">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="V25" s="65"/>
       <c r="W25" s="66">
-        <f>L25*0.2+Q25*0.25+T25*0.25+U25*0.3+V25*0.15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="62">
-        <f>SUM(D26:J26)*50/(L$1-K26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M26" s="63">
@@ -3354,7 +3354,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="62">
-        <f>SUM(M26:O26)/(Q$1-P26)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R26" s="63">
@@ -3364,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="T26" s="62">
-        <f>SUM(R26:S26)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U26" s="64">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="V26" s="65"/>
       <c r="W26" s="66">
-        <f>L26*0.2+Q26*0.25+T26*0.25+U26*0.3+V26*0.15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3411,7 +3411,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="62">
-        <f>SUM(D27:J27)*50/(L$1-K27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M27" s="63">
@@ -3427,7 +3427,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="62">
-        <f>SUM(M27:O27)/(Q$1-P27)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R27" s="63">
@@ -3437,7 +3437,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="62">
-        <f>SUM(R27:S27)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U27" s="64">
@@ -3445,7 +3445,7 @@
       </c>
       <c r="V27" s="65"/>
       <c r="W27" s="66">
-        <f>L27*0.2+Q27*0.25+T27*0.25+U27*0.3+V27*0.15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3484,7 +3484,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="62">
-        <f>SUM(D28:J28)*50/(L$1-K28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M28" s="63">
@@ -3500,7 +3500,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="62">
-        <f>SUM(M28:O28)/(Q$1-P28)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R28" s="63">
@@ -3510,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="T28" s="62">
-        <f>SUM(R28:S28)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U28" s="64">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="V28" s="65"/>
       <c r="W28" s="66">
-        <f>L28*0.2+Q28*0.25+T28*0.25+U28*0.3+V28*0.15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="62">
-        <f>SUM(D29:J29)*50/(L$1-K29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M29" s="63">
@@ -3573,7 +3573,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="62">
-        <f>SUM(M29:O29)/(Q$1-P29)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R29" s="63">
@@ -3583,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="T29" s="62">
-        <f>SUM(R29:S29)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U29" s="64">
@@ -3591,7 +3591,7 @@
       </c>
       <c r="V29" s="65"/>
       <c r="W29" s="66">
-        <f>L29*0.2+Q29*0.25+T29*0.25+U29*0.3+V29*0.15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3630,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="62">
-        <f>SUM(D30:J30)*50/(L$1-K30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M30" s="63">
@@ -3646,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="Q30" s="62">
-        <f>SUM(M30:O30)/(Q$1-P30)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R30" s="63">
@@ -3656,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="T30" s="62">
-        <f>SUM(R30:S30)/T$1</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U30" s="64">
@@ -4853,11 +4853,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U13" sqref="U13"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4870,14 +4870,14 @@
     <col min="7" max="8" width="2.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.44140625" style="1" customWidth="1"/>
-    <col min="11" max="14" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.77734375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="5.77734375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="11" max="13" width="2.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.77734375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="5.77734375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30">
         <v>5</v>
       </c>
@@ -4895,19 +4895,18 @@
       <c r="K1" s="77"/>
       <c r="L1" s="77"/>
       <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="33" t="s">
+      <c r="N1" s="78"/>
+      <c r="O1" s="33" t="s">
         <v>43</v>
       </c>
+      <c r="P1" s="19" t="s">
+        <v>39</v>
+      </c>
       <c r="Q1" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>29</v>
       </c>
@@ -4939,31 +4938,28 @@
         <v>30</v>
       </c>
       <c r="K2" s="27">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L2" s="27">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M2" s="27">
-        <v>11</v>
-      </c>
-      <c r="N2" s="27">
         <v>12</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="N2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="O2" s="26" t="s">
         <v>33</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="Q2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="3" t="s">
         <v>45</v>
@@ -4977,7 +4973,9 @@
       <c r="E3" s="38">
         <v>2</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7">
+        <v>2</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -4985,13 +4983,12 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="6"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="21"/>
       <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-    </row>
-    <row r="4" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
       <c r="B4" s="3" t="s">
         <v>82</v>
@@ -5005,7 +5002,9 @@
       <c r="E4" s="38">
         <v>2</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7">
+        <v>2</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -5013,13 +5012,12 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="6"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-    </row>
-    <row r="5" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="3" t="s">
         <v>72</v>
@@ -5033,7 +5031,9 @@
       <c r="E5" s="38">
         <v>2</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7">
+        <v>1.5</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -5041,13 +5041,12 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="6"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="21"/>
       <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-    </row>
-    <row r="6" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="3" t="s">
         <v>61</v>
@@ -5061,7 +5060,9 @@
       <c r="E6" s="38">
         <v>2</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <v>2</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -5069,13 +5070,12 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="6"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="21"/>
       <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-    </row>
-    <row r="7" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="3" t="s">
         <v>47</v>
@@ -5089,7 +5089,9 @@
       <c r="E7" s="38">
         <v>2</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <v>2</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -5097,13 +5099,12 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="6"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="21"/>
       <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-    </row>
-    <row r="8" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="3" t="s">
         <v>64</v>
@@ -5117,7 +5118,9 @@
       <c r="E8" s="38">
         <v>2</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -5125,13 +5128,12 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="6"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="21"/>
       <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-    </row>
-    <row r="9" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="3" t="s">
         <v>79</v>
@@ -5145,7 +5147,9 @@
       <c r="E9" s="38">
         <v>2</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -5153,13 +5157,12 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="6"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="21"/>
       <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-    </row>
-    <row r="10" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="3" t="s">
         <v>10</v>
@@ -5173,7 +5176,9 @@
       <c r="E10" s="38">
         <v>2</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -5181,13 +5186,12 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="6"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-    </row>
-    <row r="11" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="3" t="s">
         <v>10</v>
@@ -5201,7 +5205,9 @@
       <c r="E11" s="38">
         <v>2</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7">
+        <v>1.9</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -5209,13 +5215,12 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="6"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="21"/>
       <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-    </row>
-    <row r="12" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="3" t="s">
         <v>55</v>
@@ -5229,7 +5234,9 @@
       <c r="E12" s="38">
         <v>2</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -5237,13 +5244,12 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="6"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="21"/>
       <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-    </row>
-    <row r="13" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="3" t="s">
         <v>91</v>
@@ -5257,7 +5263,9 @@
       <c r="E13" s="38">
         <v>0</v>
       </c>
-      <c r="F13" s="41"/>
+      <c r="F13" s="41">
+        <v>0</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -5265,13 +5273,12 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="6"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-    </row>
-    <row r="14" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="3" t="s">
         <v>51</v>
@@ -5285,7 +5292,9 @@
       <c r="E14" s="38">
         <v>2</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -5293,13 +5302,12 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="6"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="21"/>
       <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-    </row>
-    <row r="15" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="3" t="s">
         <v>85</v>
@@ -5313,7 +5321,9 @@
       <c r="E15" s="38">
         <v>0</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -5321,13 +5331,12 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="6"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="21"/>
       <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-    </row>
-    <row r="16" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="3" t="s">
         <v>69</v>
@@ -5341,7 +5350,9 @@
       <c r="E16" s="38">
         <v>2</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7">
+        <v>2</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -5349,13 +5360,12 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="6"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="21"/>
       <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-    </row>
-    <row r="17" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="3" t="s">
         <v>18</v>
@@ -5369,7 +5379,9 @@
       <c r="E17" s="38">
         <v>1</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>1.8</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -5377,13 +5389,12 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="6"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="21"/>
       <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-    </row>
-    <row r="18" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="3" t="s">
         <v>95</v>
@@ -5397,7 +5408,9 @@
       <c r="E18" s="38">
         <v>0</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -5405,13 +5418,12 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="6"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="21"/>
       <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-    </row>
-    <row r="19" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="3" t="s">
         <v>74</v>
@@ -5425,7 +5437,9 @@
       <c r="E19" s="38">
         <v>2</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7">
+        <v>2</v>
+      </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -5433,13 +5447,12 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="6"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-    </row>
-    <row r="20" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="3" t="s">
         <v>49</v>
@@ -5453,7 +5466,9 @@
       <c r="E20" s="38">
         <v>2</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -5461,13 +5476,12 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="6"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="21"/>
       <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-    </row>
-    <row r="21" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="3" t="s">
         <v>35</v>
@@ -5481,7 +5495,9 @@
       <c r="E21" s="38">
         <v>0</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -5489,13 +5505,12 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="6"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-    </row>
-    <row r="22" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="56" t="s">
         <v>3</v>
@@ -5509,7 +5524,9 @@
       <c r="E22" s="38">
         <v>0</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7">
+        <v>0</v>
+      </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -5517,13 +5534,12 @@
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="6"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="21"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-    </row>
-    <row r="23" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="56" t="s">
         <v>58</v>
@@ -5537,7 +5553,9 @@
       <c r="E23" s="38">
         <v>0</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7">
+        <v>0</v>
+      </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -5545,13 +5563,12 @@
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="6"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
-      <c r="R23" s="21"/>
-    </row>
-    <row r="24" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="56" t="s">
         <v>8</v>
@@ -5565,7 +5582,9 @@
       <c r="E24" s="38">
         <v>0</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7">
+        <v>0</v>
+      </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -5573,13 +5592,12 @@
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="6"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="21"/>
       <c r="Q24" s="21"/>
-      <c r="R24" s="21"/>
-    </row>
-    <row r="25" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="56" t="s">
         <v>12</v>
@@ -5593,7 +5611,9 @@
       <c r="E25" s="38">
         <v>0</v>
       </c>
-      <c r="F25" s="12"/>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -5601,13 +5621,12 @@
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="6"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="21"/>
       <c r="Q25" s="21"/>
-      <c r="R25" s="21"/>
-    </row>
-    <row r="26" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="56" t="s">
         <v>15</v>
@@ -5621,7 +5640,9 @@
       <c r="E26" s="38">
         <v>0</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <v>0</v>
+      </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -5629,13 +5650,12 @@
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="6"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="21"/>
       <c r="Q26" s="21"/>
-      <c r="R26" s="21"/>
-    </row>
-    <row r="27" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="56" t="s">
         <v>21</v>
@@ -5649,7 +5669,9 @@
       <c r="E27" s="38">
         <v>0</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="7">
+        <v>0</v>
+      </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -5657,13 +5679,12 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="6"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="21"/>
       <c r="Q27" s="21"/>
-      <c r="R27" s="21"/>
-    </row>
-    <row r="28" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="56" t="s">
         <v>24</v>
@@ -5677,7 +5698,9 @@
       <c r="E28" s="38">
         <v>0</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -5685,13 +5708,12 @@
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="6"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="21"/>
       <c r="Q28" s="21"/>
-      <c r="R28" s="21"/>
-    </row>
-    <row r="29" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="56" t="s">
         <v>27</v>
@@ -5705,7 +5727,9 @@
       <c r="E29" s="38">
         <v>0</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -5713,13 +5737,12 @@
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="6"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="21"/>
       <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-    </row>
-    <row r="30" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
       <c r="B30" s="56" t="s">
         <v>88</v>
@@ -5733,7 +5756,9 @@
       <c r="E30" s="38">
         <v>0</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7">
+        <v>0</v>
+      </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -5741,13 +5766,12 @@
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="6"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="21"/>
       <c r="Q30" s="21"/>
-      <c r="R30" s="21"/>
-    </row>
-    <row r="31" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
       <c r="B31" s="11"/>
       <c r="C31" s="36"/>
@@ -5761,13 +5785,12 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="6"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="21"/>
       <c r="Q31" s="21"/>
-      <c r="R31" s="21"/>
-    </row>
-    <row r="32" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="36"/>
@@ -5781,13 +5804,12 @@
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="6"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="21"/>
       <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-    </row>
-    <row r="33" spans="1:18" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:17" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
       <c r="B33" s="23"/>
       <c r="C33" s="36"/>
@@ -5799,15 +5821,14 @@
       <c r="I33" s="13"/>
       <c r="J33" s="16"/>
       <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="6"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="21"/>
       <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-    </row>
-    <row r="34" spans="1:18" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:17" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -5817,7 +5838,7 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
     </row>
-    <row r="35" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -5832,9 +5853,8 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-    </row>
-    <row r="36" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -5849,9 +5869,8 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-    </row>
-    <row r="37" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -5866,9 +5885,8 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-    </row>
-    <row r="38" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -5883,9 +5901,8 @@
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-    </row>
-    <row r="39" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -5900,9 +5917,8 @@
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-    </row>
-    <row r="40" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -5917,9 +5933,8 @@
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-    </row>
-    <row r="41" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -5934,9 +5949,8 @@
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-    </row>
-    <row r="42" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -5951,9 +5965,8 @@
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-    </row>
-    <row r="43" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -5968,9 +5981,8 @@
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-    </row>
-    <row r="44" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -5985,9 +5997,8 @@
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-    </row>
-    <row r="45" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -6002,9 +6013,8 @@
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-    </row>
-    <row r="46" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -6019,9 +6029,8 @@
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-    </row>
-    <row r="47" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -6036,9 +6045,8 @@
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-    </row>
-    <row r="48" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -6053,9 +6061,8 @@
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="9"/>
-      <c r="O48" s="9"/>
-    </row>
-    <row r="49" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -6070,9 +6077,8 @@
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
       <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-    </row>
-    <row r="50" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -6087,9 +6093,8 @@
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
       <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-    </row>
-    <row r="51" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -6104,9 +6109,8 @@
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
-      <c r="O51" s="9"/>
-    </row>
-    <row r="52" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -6121,9 +6125,8 @@
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
-      <c r="O52" s="9"/>
-    </row>
-    <row r="53" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -6138,9 +6141,8 @@
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
-      <c r="O53" s="9"/>
-    </row>
-    <row r="54" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -6155,9 +6157,8 @@
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
-      <c r="O54" s="9"/>
-    </row>
-    <row r="55" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -6172,9 +6173,8 @@
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
-      <c r="O55" s="9"/>
-    </row>
-    <row r="56" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -6189,9 +6189,8 @@
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
-      <c r="O56" s="9"/>
-    </row>
-    <row r="57" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -6206,9 +6205,8 @@
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
-      <c r="O57" s="9"/>
-    </row>
-    <row r="58" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -6223,9 +6221,8 @@
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
-      <c r="O58" s="9"/>
-    </row>
-    <row r="59" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -6240,9 +6237,8 @@
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
-      <c r="O59" s="9"/>
-    </row>
-    <row r="60" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -6257,9 +6253,8 @@
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
       <c r="N60" s="9"/>
-      <c r="O60" s="9"/>
-    </row>
-    <row r="61" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -6274,9 +6269,8 @@
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
-      <c r="O61" s="9"/>
-    </row>
-    <row r="62" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -6291,9 +6285,8 @@
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
       <c r="N62" s="9"/>
-      <c r="O62" s="9"/>
-    </row>
-    <row r="63" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -6308,9 +6301,8 @@
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
-      <c r="O63" s="9"/>
-    </row>
-    <row r="64" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -6325,9 +6317,8 @@
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
       <c r="N64" s="9"/>
-      <c r="O64" s="9"/>
-    </row>
-    <row r="65" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -6342,9 +6333,8 @@
       <c r="L65" s="9"/>
       <c r="M65" s="9"/>
       <c r="N65" s="9"/>
-      <c r="O65" s="9"/>
-    </row>
-    <row r="66" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -6359,9 +6349,8 @@
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
       <c r="N66" s="9"/>
-      <c r="O66" s="9"/>
-    </row>
-    <row r="67" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -6376,9 +6365,8 @@
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
-      <c r="O67" s="9"/>
-    </row>
-    <row r="68" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -6393,9 +6381,8 @@
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
       <c r="N68" s="9"/>
-      <c r="O68" s="9"/>
-    </row>
-    <row r="69" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -6410,9 +6397,8 @@
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
       <c r="N69" s="9"/>
-      <c r="O69" s="9"/>
-    </row>
-    <row r="70" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -6427,9 +6413,8 @@
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
       <c r="N70" s="9"/>
-      <c r="O70" s="9"/>
-    </row>
-    <row r="71" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -6444,9 +6429,8 @@
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
       <c r="N71" s="9"/>
-      <c r="O71" s="9"/>
-    </row>
-    <row r="72" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -6461,9 +6445,8 @@
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
       <c r="N72" s="9"/>
-      <c r="O72" s="9"/>
-    </row>
-    <row r="73" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -6478,9 +6461,8 @@
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
       <c r="N73" s="9"/>
-      <c r="O73" s="9"/>
-    </row>
-    <row r="74" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -6495,9 +6477,8 @@
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="9"/>
-      <c r="O74" s="9"/>
-    </row>
-    <row r="75" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -6512,9 +6493,8 @@
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
       <c r="N75" s="9"/>
-      <c r="O75" s="9"/>
-    </row>
-    <row r="76" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -6529,9 +6509,8 @@
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
       <c r="N76" s="9"/>
-      <c r="O76" s="9"/>
-    </row>
-    <row r="77" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -6546,9 +6525,8 @@
       <c r="L77" s="9"/>
       <c r="M77" s="9"/>
       <c r="N77" s="9"/>
-      <c r="O77" s="9"/>
-    </row>
-    <row r="78" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
@@ -6563,9 +6541,8 @@
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
       <c r="N78" s="9"/>
-      <c r="O78" s="9"/>
-    </row>
-    <row r="79" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
@@ -6580,9 +6557,8 @@
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
       <c r="N79" s="9"/>
-      <c r="O79" s="9"/>
-    </row>
-    <row r="80" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
@@ -6597,9 +6573,8 @@
       <c r="L80" s="9"/>
       <c r="M80" s="9"/>
       <c r="N80" s="9"/>
-      <c r="O80" s="9"/>
-    </row>
-    <row r="81" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
@@ -6614,7 +6589,6 @@
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
       <c r="N81" s="9"/>
-      <c r="O81" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A3:R30">
@@ -6622,7 +6596,7 @@
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="E1:J1"/>
-    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:I33">
     <cfRule type="cellIs" dxfId="10" priority="26" operator="between">
@@ -6650,7 +6624,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O33">
+  <conditionalFormatting sqref="N3:N33">
     <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
@@ -6664,7 +6638,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q33">
+  <conditionalFormatting sqref="P3:P33">
     <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
@@ -6678,7 +6652,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:N33">
+  <conditionalFormatting sqref="K3:M33">
     <cfRule type="cellIs" dxfId="7" priority="17" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
@@ -6695,7 +6669,7 @@
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3:R33">
+  <conditionalFormatting sqref="Q3:Q33">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
@@ -6737,7 +6711,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P33">
+  <conditionalFormatting sqref="O3:O33">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>0.1</formula>
       <formula>59.9</formula>
@@ -6793,7 +6767,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>O3:O33</xm:sqref>
+          <xm:sqref>N3:N33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F9C7B28C-32E1-4B0D-97BC-F416D05D2AA7}">
@@ -6804,7 +6778,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Q3:Q33</xm:sqref>
+          <xm:sqref>P3:P33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2008DEFA-B118-4E92-B0F8-C5059B874A32}">
@@ -6815,7 +6789,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>R3:R33</xm:sqref>
+          <xm:sqref>Q3:Q33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FF44BC67-0C1D-46A1-8F9C-F95AA3B0ECDF}">

</xml_diff>

<commit_message>
ileri java not bonus
</commit_message>
<xml_diff>
--- a/AdvancedJava/_docs/Notlar.xlsx
+++ b/AdvancedJava/_docs/Notlar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Vize" sheetId="1" r:id="rId1"/>
@@ -1469,9 +1469,9 @@
   </sheetPr>
   <dimension ref="A1:X76"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S17" sqref="S17"/>
+      <selection pane="bottomLeft" activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1829,11 +1829,11 @@
         <v>66</v>
       </c>
       <c r="V5" s="43">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="W5" s="21">
         <f t="shared" ref="W5:W12" si="3">L5*0.2+Q5*0.25+T5*0.25+U5*0.3+V5*0.15</f>
-        <v>78.55</v>
+        <v>81.55</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1976,10 +1976,12 @@
       <c r="U7" s="6">
         <v>42</v>
       </c>
-      <c r="V7" s="43"/>
+      <c r="V7" s="43">
+        <v>75</v>
+      </c>
       <c r="W7" s="21">
         <f t="shared" si="3"/>
-        <v>61.558333333333337</v>
+        <v>72.808333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2049,10 +2051,12 @@
       <c r="U8" s="6">
         <v>40</v>
       </c>
-      <c r="V8" s="43"/>
+      <c r="V8" s="43">
+        <v>85</v>
+      </c>
       <c r="W8" s="21">
         <f t="shared" si="3"/>
-        <v>60.541666666666671</v>
+        <v>73.291666666666671</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2122,10 +2126,12 @@
       <c r="U9" s="6">
         <v>16</v>
       </c>
-      <c r="V9" s="43"/>
+      <c r="V9" s="43">
+        <v>90</v>
+      </c>
       <c r="W9" s="21">
         <f t="shared" si="3"/>
-        <v>58.758333333333326</v>
+        <v>72.258333333333326</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2490,10 +2496,12 @@
       <c r="U14" s="6">
         <v>5</v>
       </c>
-      <c r="V14" s="43"/>
+      <c r="V14" s="43">
+        <v>65</v>
+      </c>
       <c r="W14" s="21">
         <f>L14*0.2+Q14*0.25+T14*0.25+U14*0.3+V14*0.15</f>
-        <v>53.875</v>
+        <v>63.625</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2638,10 +2646,12 @@
       <c r="U16" s="6">
         <v>52</v>
       </c>
-      <c r="V16" s="43"/>
+      <c r="V16" s="43">
+        <v>60</v>
+      </c>
       <c r="W16" s="21">
         <f>L16*0.2+Q16*0.25+T16*0.25+U16*0.3+V16*0.15</f>
-        <v>51.866666666666674</v>
+        <v>60.866666666666674</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4855,7 +4865,7 @@
   </sheetPr>
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>

</xml_diff>